<commit_message>
finished LCA on all cmat files, new results file with all results
</commit_message>
<xml_diff>
--- a/data/ref.xlsx
+++ b/data/ref.xlsx
@@ -1,16 +1,16 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
-  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="11011"/>
+  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="11113"/>
   <workbookPr defaultThemeVersion="166925"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="/Users/jorjaelliott/Desktop/Repositories/LCAdata/data/"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{E4A08CFE-D463-9A41-8512-C5DE012578B4}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{FC23EC0F-C65D-F240-BA09-B878B1B2DAB2}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="0" yWindow="500" windowWidth="17860" windowHeight="15880" xr2:uid="{4F28B243-04AE-1E4D-B411-E86C9FDA2FDF}"/>
+    <workbookView xWindow="220" yWindow="500" windowWidth="27140" windowHeight="15880" xr2:uid="{4F28B243-04AE-1E4D-B411-E86C9FDA2FDF}"/>
   </bookViews>
   <sheets>
     <sheet name="data" sheetId="1" r:id="rId1"/>
@@ -37,7 +37,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="1259" uniqueCount="456">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="1262" uniqueCount="459">
   <si>
     <t>old file name</t>
   </si>
@@ -2059,9 +2059,6 @@
     <t>cmat = cmat.fox.csv</t>
   </si>
   <si>
-    <t>cmat=cmat.etterson.csv</t>
-  </si>
-  <si>
     <t>cmat=cmat.mcclelland.csv</t>
   </si>
   <si>
@@ -2072,6 +2069,18 @@
   </si>
   <si>
     <t>high density</t>
+  </si>
+  <si>
+    <t>cmat=cmatrix.sperm.csv</t>
+  </si>
+  <si>
+    <t>cmat=cmatrix.sr.csv</t>
+  </si>
+  <si>
+    <t>cmat=cmat.etterson.BDF.csv</t>
+  </si>
+  <si>
+    <t>cmat=cmat.etterson.ACE.csv</t>
   </si>
 </sst>
 </file>
@@ -2124,12 +2133,18 @@
       <scheme val="minor"/>
     </font>
   </fonts>
-  <fills count="2">
+  <fills count="3">
     <fill>
       <patternFill patternType="none"/>
     </fill>
     <fill>
       <patternFill patternType="gray125"/>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor rgb="FFFF0000"/>
+        <bgColor indexed="64"/>
+      </patternFill>
     </fill>
   </fills>
   <borders count="1">
@@ -2144,18 +2159,27 @@
   <cellStyleXfs count="1">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
   </cellStyleXfs>
-  <cellXfs count="6">
+  <cellXfs count="8">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="1" fillId="0" borderId="0" xfId="0" applyFont="1"/>
     <xf numFmtId="0" fontId="2" fillId="0" borderId="0" xfId="0" applyFont="1"/>
     <xf numFmtId="0" fontId="4" fillId="0" borderId="0" xfId="0" applyFont="1"/>
     <xf numFmtId="0" fontId="5" fillId="0" borderId="0" xfId="0" applyFont="1"/>
     <xf numFmtId="16" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1"/>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyFill="1"/>
+    <xf numFmtId="0" fontId="0" fillId="2" borderId="0" xfId="0" applyFill="1"/>
   </cellXfs>
   <cellStyles count="1">
     <cellStyle name="Normal" xfId="0" builtinId="0"/>
   </cellStyles>
-  <dxfs count="1">
+  <dxfs count="2">
+    <dxf>
+      <fill>
+        <patternFill>
+          <bgColor rgb="FFFFC7CE"/>
+        </patternFill>
+      </fill>
+    </dxf>
     <dxf>
       <fill>
         <patternFill>
@@ -2473,11 +2497,11 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{1137BAE9-F081-9948-9F37-D6A451EE45DA}">
-  <dimension ref="A1:S229"/>
+  <dimension ref="A1:S227"/>
   <sheetViews>
     <sheetView tabSelected="1" zoomScale="106" workbookViewId="0">
-      <pane ySplit="1" topLeftCell="A114" activePane="bottomLeft" state="frozen"/>
-      <selection pane="bottomLeft" activeCell="F129" sqref="F129"/>
+      <pane ySplit="1" topLeftCell="A148" activePane="bottomLeft" state="frozen"/>
+      <selection pane="bottomLeft" activeCell="A166" sqref="A166"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="16" x14ac:dyDescent="0.2"/>
@@ -3004,97 +3028,91 @@
       </c>
     </row>
     <row r="27" spans="1:7" x14ac:dyDescent="0.2">
-      <c r="A27" t="s">
-        <v>55</v>
-      </c>
-      <c r="B27" s="3" t="s">
-        <v>156</v>
-      </c>
-      <c r="C27" s="4" t="s">
-        <v>195</v>
+      <c r="B27" t="s">
+        <v>416</v>
+      </c>
+      <c r="C27" t="s">
+        <v>400</v>
       </c>
       <c r="D27" t="s">
-        <v>102</v>
+        <v>447</v>
       </c>
       <c r="E27" t="s">
-        <v>168</v>
+        <v>169</v>
       </c>
       <c r="F27" t="s">
-        <v>166</v>
+        <v>420</v>
       </c>
       <c r="G27" t="s">
-        <v>99</v>
+        <v>389</v>
       </c>
     </row>
     <row r="28" spans="1:7" x14ac:dyDescent="0.2">
-      <c r="A28" t="s">
-        <v>56</v>
-      </c>
-      <c r="B28" s="3" t="s">
-        <v>157</v>
-      </c>
-      <c r="C28" s="4" t="s">
-        <v>195</v>
+      <c r="B28" t="s">
+        <v>250</v>
+      </c>
+      <c r="C28" t="s">
+        <v>400</v>
       </c>
       <c r="D28" t="s">
-        <v>102</v>
+        <v>447</v>
       </c>
       <c r="E28" t="s">
-        <v>168</v>
+        <v>169</v>
       </c>
       <c r="F28" t="s">
-        <v>166</v>
+        <v>236</v>
       </c>
       <c r="G28" t="s">
-        <v>99</v>
+        <v>393</v>
       </c>
     </row>
     <row r="29" spans="1:7" x14ac:dyDescent="0.2">
       <c r="B29" t="s">
-        <v>416</v>
+        <v>397</v>
       </c>
       <c r="C29" t="s">
-        <v>400</v>
+        <v>403</v>
       </c>
       <c r="D29" t="s">
-        <v>447</v>
+        <v>102</v>
       </c>
       <c r="E29" t="s">
-        <v>169</v>
+        <v>168</v>
       </c>
       <c r="F29" t="s">
-        <v>420</v>
+        <v>212</v>
       </c>
       <c r="G29" t="s">
-        <v>389</v>
+        <v>386</v>
       </c>
     </row>
     <row r="30" spans="1:7" x14ac:dyDescent="0.2">
       <c r="B30" t="s">
-        <v>250</v>
+        <v>270</v>
       </c>
       <c r="C30" t="s">
-        <v>400</v>
+        <v>449</v>
       </c>
       <c r="D30" t="s">
         <v>447</v>
       </c>
       <c r="E30" t="s">
-        <v>169</v>
+        <v>168</v>
       </c>
       <c r="F30" t="s">
-        <v>236</v>
+        <v>269</v>
       </c>
       <c r="G30" t="s">
-        <v>393</v>
+        <v>395</v>
       </c>
     </row>
     <row r="31" spans="1:7" x14ac:dyDescent="0.2">
       <c r="B31" t="s">
-        <v>397</v>
-      </c>
-      <c r="C31" t="s">
-        <v>403</v>
+        <v>88</v>
+      </c>
+      <c r="C31" s="2" t="s">
+        <v>198</v>
       </c>
       <c r="D31" t="s">
         <v>102</v>
@@ -3102,39 +3120,39 @@
       <c r="E31" t="s">
         <v>168</v>
       </c>
-      <c r="F31" t="s">
-        <v>212</v>
-      </c>
       <c r="G31" t="s">
-        <v>386</v>
+        <v>205</v>
       </c>
     </row>
     <row r="32" spans="1:7" x14ac:dyDescent="0.2">
       <c r="B32" t="s">
-        <v>270</v>
+        <v>345</v>
       </c>
       <c r="C32" t="s">
-        <v>449</v>
+        <v>403</v>
       </c>
       <c r="D32" t="s">
-        <v>447</v>
+        <v>102</v>
       </c>
       <c r="E32" t="s">
-        <v>168</v>
+        <v>169</v>
       </c>
       <c r="F32" t="s">
-        <v>269</v>
+        <v>411</v>
       </c>
       <c r="G32" t="s">
-        <v>395</v>
+        <v>394</v>
       </c>
     </row>
     <row r="33" spans="1:7" x14ac:dyDescent="0.2">
-      <c r="B33" t="s">
-        <v>88</v>
-      </c>
-      <c r="C33" s="2" t="s">
-        <v>198</v>
+      <c r="A33" t="s">
+        <v>57</v>
+      </c>
+      <c r="B33" s="3" t="s">
+        <v>158</v>
+      </c>
+      <c r="C33" s="3" t="s">
+        <v>196</v>
       </c>
       <c r="D33" t="s">
         <v>102</v>
@@ -3143,15 +3161,15 @@
         <v>168</v>
       </c>
       <c r="G33" t="s">
-        <v>205</v>
+        <v>100</v>
       </c>
     </row>
     <row r="34" spans="1:7" x14ac:dyDescent="0.2">
       <c r="B34" t="s">
-        <v>345</v>
-      </c>
-      <c r="C34" t="s">
-        <v>403</v>
+        <v>89</v>
+      </c>
+      <c r="C34" s="2" t="s">
+        <v>199</v>
       </c>
       <c r="D34" t="s">
         <v>102</v>
@@ -3159,56 +3177,56 @@
       <c r="E34" t="s">
         <v>169</v>
       </c>
-      <c r="F34" t="s">
-        <v>411</v>
-      </c>
       <c r="G34" t="s">
-        <v>394</v>
+        <v>206</v>
       </c>
     </row>
     <row r="35" spans="1:7" x14ac:dyDescent="0.2">
-      <c r="A35" t="s">
-        <v>57</v>
-      </c>
-      <c r="B35" s="3" t="s">
-        <v>158</v>
-      </c>
-      <c r="C35" s="3" t="s">
-        <v>196</v>
+      <c r="B35" t="s">
+        <v>379</v>
+      </c>
+      <c r="C35" t="s">
+        <v>434</v>
       </c>
       <c r="D35" t="s">
-        <v>102</v>
+        <v>447</v>
       </c>
       <c r="E35" t="s">
         <v>168</v>
       </c>
+      <c r="F35" t="s">
+        <v>221</v>
+      </c>
       <c r="G35" t="s">
-        <v>100</v>
+        <v>390</v>
       </c>
     </row>
     <row r="36" spans="1:7" x14ac:dyDescent="0.2">
       <c r="B36" t="s">
-        <v>89</v>
-      </c>
-      <c r="C36" s="2" t="s">
-        <v>199</v>
+        <v>376</v>
+      </c>
+      <c r="C36" t="s">
+        <v>434</v>
       </c>
       <c r="D36" t="s">
-        <v>102</v>
+        <v>447</v>
       </c>
       <c r="E36" t="s">
-        <v>169</v>
+        <v>168</v>
+      </c>
+      <c r="F36" t="s">
+        <v>218</v>
       </c>
       <c r="G36" t="s">
-        <v>206</v>
+        <v>390</v>
       </c>
     </row>
     <row r="37" spans="1:7" x14ac:dyDescent="0.2">
       <c r="B37" t="s">
-        <v>379</v>
+        <v>90</v>
       </c>
       <c r="C37" t="s">
-        <v>434</v>
+        <v>194</v>
       </c>
       <c r="D37" t="s">
         <v>447</v>
@@ -3216,16 +3234,13 @@
       <c r="E37" t="s">
         <v>168</v>
       </c>
-      <c r="F37" t="s">
-        <v>221</v>
-      </c>
       <c r="G37" t="s">
-        <v>390</v>
+        <v>85</v>
       </c>
     </row>
     <row r="38" spans="1:7" x14ac:dyDescent="0.2">
       <c r="B38" t="s">
-        <v>376</v>
+        <v>381</v>
       </c>
       <c r="C38" t="s">
         <v>434</v>
@@ -3237,17 +3252,20 @@
         <v>168</v>
       </c>
       <c r="F38" t="s">
-        <v>218</v>
+        <v>223</v>
       </c>
       <c r="G38" t="s">
         <v>390</v>
       </c>
     </row>
     <row r="39" spans="1:7" x14ac:dyDescent="0.2">
-      <c r="B39" t="s">
-        <v>90</v>
-      </c>
-      <c r="C39" t="s">
+      <c r="A39" t="s">
+        <v>40</v>
+      </c>
+      <c r="B39" s="3" t="s">
+        <v>141</v>
+      </c>
+      <c r="C39" s="3" t="s">
         <v>194</v>
       </c>
       <c r="D39" t="s">
@@ -3257,15 +3275,18 @@
         <v>168</v>
       </c>
       <c r="G39" t="s">
-        <v>85</v>
+        <v>98</v>
       </c>
     </row>
     <row r="40" spans="1:7" x14ac:dyDescent="0.2">
-      <c r="B40" t="s">
-        <v>381</v>
-      </c>
-      <c r="C40" t="s">
-        <v>434</v>
+      <c r="A40" t="s">
+        <v>42</v>
+      </c>
+      <c r="B40" s="3" t="s">
+        <v>143</v>
+      </c>
+      <c r="C40" s="3" t="s">
+        <v>194</v>
       </c>
       <c r="D40" t="s">
         <v>447</v>
@@ -3273,19 +3294,16 @@
       <c r="E40" t="s">
         <v>168</v>
       </c>
-      <c r="F40" t="s">
-        <v>223</v>
-      </c>
       <c r="G40" t="s">
-        <v>390</v>
+        <v>98</v>
       </c>
     </row>
     <row r="41" spans="1:7" x14ac:dyDescent="0.2">
       <c r="A41" t="s">
-        <v>40</v>
+        <v>41</v>
       </c>
       <c r="B41" s="3" t="s">
-        <v>141</v>
+        <v>142</v>
       </c>
       <c r="C41" s="3" t="s">
         <v>194</v>
@@ -3302,10 +3320,10 @@
     </row>
     <row r="42" spans="1:7" x14ac:dyDescent="0.2">
       <c r="A42" t="s">
-        <v>42</v>
+        <v>43</v>
       </c>
       <c r="B42" s="3" t="s">
-        <v>143</v>
+        <v>144</v>
       </c>
       <c r="C42" s="3" t="s">
         <v>194</v>
@@ -3322,10 +3340,10 @@
     </row>
     <row r="43" spans="1:7" x14ac:dyDescent="0.2">
       <c r="A43" t="s">
-        <v>41</v>
+        <v>44</v>
       </c>
       <c r="B43" s="3" t="s">
-        <v>142</v>
+        <v>145</v>
       </c>
       <c r="C43" s="3" t="s">
         <v>194</v>
@@ -3341,14 +3359,11 @@
       </c>
     </row>
     <row r="44" spans="1:7" x14ac:dyDescent="0.2">
-      <c r="A44" t="s">
-        <v>43</v>
-      </c>
-      <c r="B44" s="3" t="s">
-        <v>144</v>
-      </c>
-      <c r="C44" s="3" t="s">
-        <v>194</v>
+      <c r="B44" t="s">
+        <v>380</v>
+      </c>
+      <c r="C44" t="s">
+        <v>434</v>
       </c>
       <c r="D44" t="s">
         <v>447</v>
@@ -3356,16 +3371,19 @@
       <c r="E44" t="s">
         <v>168</v>
       </c>
+      <c r="F44" t="s">
+        <v>222</v>
+      </c>
       <c r="G44" t="s">
-        <v>98</v>
+        <v>390</v>
       </c>
     </row>
     <row r="45" spans="1:7" x14ac:dyDescent="0.2">
       <c r="A45" t="s">
-        <v>44</v>
+        <v>30</v>
       </c>
       <c r="B45" s="3" t="s">
-        <v>145</v>
+        <v>131</v>
       </c>
       <c r="C45" s="3" t="s">
         <v>194</v>
@@ -3381,11 +3399,14 @@
       </c>
     </row>
     <row r="46" spans="1:7" x14ac:dyDescent="0.2">
-      <c r="B46" t="s">
-        <v>380</v>
-      </c>
-      <c r="C46" t="s">
-        <v>434</v>
+      <c r="A46" t="s">
+        <v>31</v>
+      </c>
+      <c r="B46" s="3" t="s">
+        <v>132</v>
+      </c>
+      <c r="C46" s="3" t="s">
+        <v>194</v>
       </c>
       <c r="D46" t="s">
         <v>447</v>
@@ -3393,19 +3414,16 @@
       <c r="E46" t="s">
         <v>168</v>
       </c>
-      <c r="F46" t="s">
-        <v>222</v>
-      </c>
       <c r="G46" t="s">
-        <v>390</v>
+        <v>98</v>
       </c>
     </row>
     <row r="47" spans="1:7" x14ac:dyDescent="0.2">
       <c r="A47" t="s">
-        <v>30</v>
+        <v>32</v>
       </c>
       <c r="B47" s="3" t="s">
-        <v>131</v>
+        <v>133</v>
       </c>
       <c r="C47" s="3" t="s">
         <v>194</v>
@@ -3422,10 +3440,10 @@
     </row>
     <row r="48" spans="1:7" x14ac:dyDescent="0.2">
       <c r="A48" t="s">
-        <v>31</v>
+        <v>33</v>
       </c>
       <c r="B48" s="3" t="s">
-        <v>132</v>
+        <v>134</v>
       </c>
       <c r="C48" s="3" t="s">
         <v>194</v>
@@ -3442,10 +3460,10 @@
     </row>
     <row r="49" spans="1:7" x14ac:dyDescent="0.2">
       <c r="A49" t="s">
-        <v>32</v>
+        <v>34</v>
       </c>
       <c r="B49" s="3" t="s">
-        <v>133</v>
+        <v>135</v>
       </c>
       <c r="C49" s="3" t="s">
         <v>194</v>
@@ -3461,14 +3479,11 @@
       </c>
     </row>
     <row r="50" spans="1:7" x14ac:dyDescent="0.2">
-      <c r="A50" t="s">
-        <v>33</v>
-      </c>
-      <c r="B50" s="3" t="s">
-        <v>134</v>
-      </c>
-      <c r="C50" s="3" t="s">
-        <v>194</v>
+      <c r="B50" t="s">
+        <v>335</v>
+      </c>
+      <c r="C50" t="s">
+        <v>449</v>
       </c>
       <c r="D50" t="s">
         <v>447</v>
@@ -3476,19 +3491,19 @@
       <c r="E50" t="s">
         <v>168</v>
       </c>
+      <c r="F50" t="s">
+        <v>271</v>
+      </c>
       <c r="G50" t="s">
-        <v>98</v>
+        <v>395</v>
       </c>
     </row>
     <row r="51" spans="1:7" x14ac:dyDescent="0.2">
-      <c r="A51" t="s">
-        <v>34</v>
-      </c>
-      <c r="B51" s="3" t="s">
-        <v>135</v>
-      </c>
-      <c r="C51" s="3" t="s">
-        <v>194</v>
+      <c r="B51" t="s">
+        <v>415</v>
+      </c>
+      <c r="C51" t="s">
+        <v>400</v>
       </c>
       <c r="D51" t="s">
         <v>447</v>
@@ -3496,16 +3511,19 @@
       <c r="E51" t="s">
         <v>168</v>
       </c>
+      <c r="F51" t="s">
+        <v>417</v>
+      </c>
       <c r="G51" t="s">
-        <v>98</v>
+        <v>389</v>
       </c>
     </row>
     <row r="52" spans="1:7" x14ac:dyDescent="0.2">
       <c r="B52" t="s">
-        <v>335</v>
+        <v>91</v>
       </c>
       <c r="C52" t="s">
-        <v>449</v>
+        <v>194</v>
       </c>
       <c r="D52" t="s">
         <v>447</v>
@@ -3513,53 +3531,53 @@
       <c r="E52" t="s">
         <v>168</v>
       </c>
-      <c r="F52" t="s">
-        <v>271</v>
-      </c>
       <c r="G52" t="s">
-        <v>395</v>
+        <v>85</v>
       </c>
     </row>
     <row r="53" spans="1:7" x14ac:dyDescent="0.2">
       <c r="B53" t="s">
-        <v>415</v>
+        <v>233</v>
       </c>
       <c r="C53" t="s">
-        <v>400</v>
+        <v>203</v>
       </c>
       <c r="D53" t="s">
-        <v>447</v>
+        <v>102</v>
       </c>
       <c r="E53" t="s">
-        <v>168</v>
+        <v>169</v>
       </c>
       <c r="F53" t="s">
-        <v>417</v>
+        <v>228</v>
       </c>
       <c r="G53" t="s">
-        <v>389</v>
+        <v>391</v>
       </c>
     </row>
     <row r="54" spans="1:7" x14ac:dyDescent="0.2">
       <c r="B54" t="s">
-        <v>91</v>
+        <v>232</v>
       </c>
       <c r="C54" t="s">
-        <v>194</v>
+        <v>203</v>
       </c>
       <c r="D54" t="s">
-        <v>447</v>
+        <v>102</v>
       </c>
       <c r="E54" t="s">
-        <v>168</v>
+        <v>169</v>
+      </c>
+      <c r="F54" t="s">
+        <v>227</v>
       </c>
       <c r="G54" t="s">
-        <v>85</v>
+        <v>391</v>
       </c>
     </row>
     <row r="55" spans="1:7" x14ac:dyDescent="0.2">
       <c r="B55" t="s">
-        <v>233</v>
+        <v>268</v>
       </c>
       <c r="C55" t="s">
         <v>203</v>
@@ -3568,10 +3586,10 @@
         <v>102</v>
       </c>
       <c r="E55" t="s">
-        <v>169</v>
+        <v>168</v>
       </c>
       <c r="F55" t="s">
-        <v>228</v>
+        <v>231</v>
       </c>
       <c r="G55" t="s">
         <v>391</v>
@@ -3579,30 +3597,33 @@
     </row>
     <row r="56" spans="1:7" x14ac:dyDescent="0.2">
       <c r="B56" t="s">
-        <v>232</v>
+        <v>375</v>
       </c>
       <c r="C56" t="s">
-        <v>203</v>
+        <v>434</v>
       </c>
       <c r="D56" t="s">
-        <v>102</v>
+        <v>447</v>
       </c>
       <c r="E56" t="s">
-        <v>169</v>
+        <v>168</v>
       </c>
       <c r="F56" t="s">
-        <v>227</v>
+        <v>217</v>
       </c>
       <c r="G56" t="s">
-        <v>391</v>
+        <v>390</v>
       </c>
     </row>
     <row r="57" spans="1:7" x14ac:dyDescent="0.2">
-      <c r="B57" t="s">
-        <v>268</v>
-      </c>
-      <c r="C57" t="s">
-        <v>203</v>
+      <c r="A57" t="s">
+        <v>18</v>
+      </c>
+      <c r="B57" s="3" t="s">
+        <v>119</v>
+      </c>
+      <c r="C57" s="4" t="s">
+        <v>193</v>
       </c>
       <c r="D57" t="s">
         <v>102</v>
@@ -3610,39 +3631,36 @@
       <c r="E57" t="s">
         <v>168</v>
       </c>
-      <c r="F57" t="s">
-        <v>231</v>
-      </c>
       <c r="G57" t="s">
-        <v>391</v>
+        <v>97</v>
       </c>
     </row>
     <row r="58" spans="1:7" x14ac:dyDescent="0.2">
-      <c r="B58" t="s">
-        <v>375</v>
-      </c>
-      <c r="C58" t="s">
-        <v>434</v>
+      <c r="A58" t="s">
+        <v>19</v>
+      </c>
+      <c r="B58" s="3" t="s">
+        <v>120</v>
+      </c>
+      <c r="C58" s="4" t="s">
+        <v>193</v>
       </c>
       <c r="D58" t="s">
-        <v>447</v>
+        <v>102</v>
       </c>
       <c r="E58" t="s">
         <v>168</v>
       </c>
-      <c r="F58" t="s">
-        <v>217</v>
-      </c>
       <c r="G58" t="s">
-        <v>390</v>
+        <v>97</v>
       </c>
     </row>
     <row r="59" spans="1:7" x14ac:dyDescent="0.2">
       <c r="A59" t="s">
-        <v>18</v>
+        <v>20</v>
       </c>
       <c r="B59" s="3" t="s">
-        <v>119</v>
+        <v>121</v>
       </c>
       <c r="C59" s="4" t="s">
         <v>193</v>
@@ -3659,10 +3677,10 @@
     </row>
     <row r="60" spans="1:7" x14ac:dyDescent="0.2">
       <c r="A60" t="s">
-        <v>19</v>
+        <v>21</v>
       </c>
       <c r="B60" s="3" t="s">
-        <v>120</v>
+        <v>122</v>
       </c>
       <c r="C60" s="4" t="s">
         <v>193</v>
@@ -3679,10 +3697,10 @@
     </row>
     <row r="61" spans="1:7" x14ac:dyDescent="0.2">
       <c r="A61" t="s">
-        <v>20</v>
+        <v>22</v>
       </c>
       <c r="B61" s="3" t="s">
-        <v>121</v>
+        <v>123</v>
       </c>
       <c r="C61" s="4" t="s">
         <v>193</v>
@@ -3699,10 +3717,10 @@
     </row>
     <row r="62" spans="1:7" x14ac:dyDescent="0.2">
       <c r="A62" t="s">
-        <v>21</v>
+        <v>23</v>
       </c>
       <c r="B62" s="3" t="s">
-        <v>122</v>
+        <v>124</v>
       </c>
       <c r="C62" s="4" t="s">
         <v>193</v>
@@ -3719,10 +3737,10 @@
     </row>
     <row r="63" spans="1:7" x14ac:dyDescent="0.2">
       <c r="A63" t="s">
-        <v>22</v>
+        <v>24</v>
       </c>
       <c r="B63" s="3" t="s">
-        <v>123</v>
+        <v>125</v>
       </c>
       <c r="C63" s="4" t="s">
         <v>193</v>
@@ -3739,10 +3757,10 @@
     </row>
     <row r="64" spans="1:7" x14ac:dyDescent="0.2">
       <c r="A64" t="s">
-        <v>23</v>
+        <v>25</v>
       </c>
       <c r="B64" s="3" t="s">
-        <v>124</v>
+        <v>126</v>
       </c>
       <c r="C64" s="4" t="s">
         <v>193</v>
@@ -3759,10 +3777,10 @@
     </row>
     <row r="65" spans="1:7" x14ac:dyDescent="0.2">
       <c r="A65" t="s">
-        <v>24</v>
+        <v>26</v>
       </c>
       <c r="B65" s="3" t="s">
-        <v>125</v>
+        <v>127</v>
       </c>
       <c r="C65" s="4" t="s">
         <v>193</v>
@@ -3778,91 +3796,91 @@
       </c>
     </row>
     <row r="66" spans="1:7" x14ac:dyDescent="0.2">
-      <c r="A66" t="s">
-        <v>25</v>
-      </c>
-      <c r="B66" s="3" t="s">
-        <v>126</v>
-      </c>
-      <c r="C66" s="4" t="s">
-        <v>193</v>
+      <c r="B66" t="s">
+        <v>262</v>
+      </c>
+      <c r="C66" t="s">
+        <v>400</v>
       </c>
       <c r="D66" t="s">
-        <v>102</v>
+        <v>447</v>
       </c>
       <c r="E66" t="s">
-        <v>168</v>
+        <v>169</v>
+      </c>
+      <c r="F66" t="s">
+        <v>245</v>
       </c>
       <c r="G66" t="s">
-        <v>97</v>
+        <v>393</v>
       </c>
     </row>
     <row r="67" spans="1:7" x14ac:dyDescent="0.2">
-      <c r="A67" t="s">
-        <v>26</v>
-      </c>
-      <c r="B67" s="3" t="s">
-        <v>127</v>
-      </c>
-      <c r="C67" s="4" t="s">
-        <v>193</v>
+      <c r="B67" t="s">
+        <v>258</v>
+      </c>
+      <c r="C67" t="s">
+        <v>400</v>
       </c>
       <c r="D67" t="s">
-        <v>102</v>
+        <v>447</v>
       </c>
       <c r="E67" t="s">
-        <v>168</v>
+        <v>169</v>
+      </c>
+      <c r="F67" t="s">
+        <v>244</v>
       </c>
       <c r="G67" t="s">
-        <v>97</v>
+        <v>393</v>
       </c>
     </row>
     <row r="68" spans="1:7" x14ac:dyDescent="0.2">
-      <c r="B68" t="s">
-        <v>262</v>
-      </c>
-      <c r="C68" t="s">
-        <v>400</v>
+      <c r="A68" t="s">
+        <v>35</v>
+      </c>
+      <c r="B68" s="3" t="s">
+        <v>136</v>
+      </c>
+      <c r="C68" s="3" t="s">
+        <v>194</v>
       </c>
       <c r="D68" t="s">
         <v>447</v>
       </c>
       <c r="E68" t="s">
-        <v>169</v>
-      </c>
-      <c r="F68" t="s">
-        <v>245</v>
+        <v>168</v>
       </c>
       <c r="G68" t="s">
-        <v>393</v>
+        <v>98</v>
       </c>
     </row>
     <row r="69" spans="1:7" x14ac:dyDescent="0.2">
-      <c r="B69" t="s">
-        <v>258</v>
-      </c>
-      <c r="C69" t="s">
-        <v>400</v>
+      <c r="A69" t="s">
+        <v>37</v>
+      </c>
+      <c r="B69" s="3" t="s">
+        <v>138</v>
+      </c>
+      <c r="C69" s="3" t="s">
+        <v>194</v>
       </c>
       <c r="D69" t="s">
         <v>447</v>
       </c>
       <c r="E69" t="s">
-        <v>169</v>
-      </c>
-      <c r="F69" t="s">
-        <v>244</v>
+        <v>168</v>
       </c>
       <c r="G69" t="s">
-        <v>393</v>
+        <v>98</v>
       </c>
     </row>
     <row r="70" spans="1:7" x14ac:dyDescent="0.2">
       <c r="A70" t="s">
-        <v>35</v>
+        <v>36</v>
       </c>
       <c r="B70" s="3" t="s">
-        <v>136</v>
+        <v>137</v>
       </c>
       <c r="C70" s="3" t="s">
         <v>194</v>
@@ -3879,10 +3897,10 @@
     </row>
     <row r="71" spans="1:7" x14ac:dyDescent="0.2">
       <c r="A71" t="s">
-        <v>37</v>
+        <v>38</v>
       </c>
       <c r="B71" s="3" t="s">
-        <v>138</v>
+        <v>139</v>
       </c>
       <c r="C71" s="3" t="s">
         <v>194</v>
@@ -3899,10 +3917,10 @@
     </row>
     <row r="72" spans="1:7" x14ac:dyDescent="0.2">
       <c r="A72" t="s">
-        <v>36</v>
+        <v>39</v>
       </c>
       <c r="B72" s="3" t="s">
-        <v>137</v>
+        <v>140</v>
       </c>
       <c r="C72" s="3" t="s">
         <v>194</v>
@@ -3919,50 +3937,50 @@
     </row>
     <row r="73" spans="1:7" x14ac:dyDescent="0.2">
       <c r="A73" t="s">
-        <v>38</v>
+        <v>27</v>
       </c>
       <c r="B73" s="3" t="s">
-        <v>139</v>
-      </c>
-      <c r="C73" s="3" t="s">
-        <v>194</v>
+        <v>128</v>
+      </c>
+      <c r="C73" s="4" t="s">
+        <v>193</v>
       </c>
       <c r="D73" t="s">
-        <v>447</v>
+        <v>102</v>
       </c>
       <c r="E73" t="s">
         <v>168</v>
       </c>
       <c r="G73" t="s">
-        <v>98</v>
+        <v>97</v>
       </c>
     </row>
     <row r="74" spans="1:7" x14ac:dyDescent="0.2">
       <c r="A74" t="s">
-        <v>39</v>
+        <v>28</v>
       </c>
       <c r="B74" s="3" t="s">
-        <v>140</v>
-      </c>
-      <c r="C74" s="3" t="s">
-        <v>194</v>
+        <v>129</v>
+      </c>
+      <c r="C74" s="4" t="s">
+        <v>193</v>
       </c>
       <c r="D74" t="s">
-        <v>447</v>
+        <v>102</v>
       </c>
       <c r="E74" t="s">
         <v>168</v>
       </c>
       <c r="G74" t="s">
-        <v>98</v>
+        <v>97</v>
       </c>
     </row>
     <row r="75" spans="1:7" x14ac:dyDescent="0.2">
       <c r="A75" t="s">
-        <v>27</v>
+        <v>29</v>
       </c>
       <c r="B75" s="3" t="s">
-        <v>128</v>
+        <v>130</v>
       </c>
       <c r="C75" s="4" t="s">
         <v>193</v>
@@ -3979,13 +3997,13 @@
     </row>
     <row r="76" spans="1:7" x14ac:dyDescent="0.2">
       <c r="A76" t="s">
-        <v>28</v>
+        <v>58</v>
       </c>
       <c r="B76" s="3" t="s">
-        <v>129</v>
-      </c>
-      <c r="C76" s="4" t="s">
-        <v>193</v>
+        <v>159</v>
+      </c>
+      <c r="C76" s="3" t="s">
+        <v>196</v>
       </c>
       <c r="D76" t="s">
         <v>102</v>
@@ -3994,135 +4012,135 @@
         <v>168</v>
       </c>
       <c r="G76" t="s">
-        <v>97</v>
+        <v>100</v>
       </c>
     </row>
     <row r="77" spans="1:7" x14ac:dyDescent="0.2">
       <c r="A77" t="s">
-        <v>29</v>
+        <v>59</v>
       </c>
       <c r="B77" s="3" t="s">
-        <v>130</v>
-      </c>
-      <c r="C77" s="4" t="s">
+        <v>160</v>
+      </c>
+      <c r="C77" s="3" t="s">
+        <v>196</v>
+      </c>
+      <c r="D77" t="s">
+        <v>102</v>
+      </c>
+      <c r="E77" t="s">
+        <v>168</v>
+      </c>
+      <c r="G77" t="s">
+        <v>100</v>
+      </c>
+    </row>
+    <row r="78" spans="1:7" x14ac:dyDescent="0.2">
+      <c r="B78" t="s">
+        <v>383</v>
+      </c>
+      <c r="C78" t="s">
+        <v>434</v>
+      </c>
+      <c r="D78" t="s">
+        <v>447</v>
+      </c>
+      <c r="E78" t="s">
+        <v>168</v>
+      </c>
+      <c r="F78" t="s">
+        <v>374</v>
+      </c>
+      <c r="G78" t="s">
+        <v>390</v>
+      </c>
+    </row>
+    <row r="79" spans="1:7" x14ac:dyDescent="0.2">
+      <c r="B79" t="s">
+        <v>225</v>
+      </c>
+      <c r="C79" t="s">
+        <v>400</v>
+      </c>
+      <c r="D79" t="s">
+        <v>447</v>
+      </c>
+      <c r="E79" t="s">
+        <v>169</v>
+      </c>
+      <c r="F79" t="s">
+        <v>210</v>
+      </c>
+      <c r="G79" t="s">
+        <v>384</v>
+      </c>
+    </row>
+    <row r="80" spans="1:7" x14ac:dyDescent="0.2">
+      <c r="A80" t="s">
+        <v>11</v>
+      </c>
+      <c r="B80" s="3" t="s">
+        <v>112</v>
+      </c>
+      <c r="C80" s="4" t="s">
         <v>193</v>
       </c>
-      <c r="D77" t="s">
-        <v>102</v>
-      </c>
-      <c r="E77" t="s">
-        <v>168</v>
-      </c>
-      <c r="G77" t="s">
+      <c r="D80" t="s">
+        <v>102</v>
+      </c>
+      <c r="E80" t="s">
+        <v>168</v>
+      </c>
+      <c r="G80" t="s">
         <v>97</v>
       </c>
     </row>
-    <row r="78" spans="1:7" x14ac:dyDescent="0.2">
-      <c r="A78" t="s">
-        <v>58</v>
-      </c>
-      <c r="B78" s="3" t="s">
-        <v>159</v>
-      </c>
-      <c r="C78" s="3" t="s">
-        <v>196</v>
-      </c>
-      <c r="D78" t="s">
-        <v>102</v>
-      </c>
-      <c r="E78" t="s">
-        <v>168</v>
-      </c>
-      <c r="G78" t="s">
-        <v>100</v>
-      </c>
-    </row>
-    <row r="79" spans="1:7" x14ac:dyDescent="0.2">
-      <c r="A79" t="s">
-        <v>59</v>
-      </c>
-      <c r="B79" s="3" t="s">
-        <v>160</v>
-      </c>
-      <c r="C79" s="3" t="s">
-        <v>196</v>
-      </c>
-      <c r="D79" t="s">
-        <v>102</v>
-      </c>
-      <c r="E79" t="s">
-        <v>168</v>
-      </c>
-      <c r="G79" t="s">
-        <v>100</v>
-      </c>
-    </row>
-    <row r="80" spans="1:7" x14ac:dyDescent="0.2">
-      <c r="B80" t="s">
-        <v>383</v>
-      </c>
-      <c r="C80" t="s">
+    <row r="81" spans="1:7" x14ac:dyDescent="0.2">
+      <c r="A81" t="s">
+        <v>12</v>
+      </c>
+      <c r="B81" s="3" t="s">
+        <v>113</v>
+      </c>
+      <c r="C81" s="4" t="s">
+        <v>193</v>
+      </c>
+      <c r="D81" t="s">
+        <v>102</v>
+      </c>
+      <c r="E81" t="s">
+        <v>168</v>
+      </c>
+      <c r="G81" t="s">
+        <v>97</v>
+      </c>
+    </row>
+    <row r="82" spans="1:7" x14ac:dyDescent="0.2">
+      <c r="B82" t="s">
+        <v>378</v>
+      </c>
+      <c r="C82" t="s">
         <v>434</v>
       </c>
-      <c r="D80" t="s">
-        <v>447</v>
-      </c>
-      <c r="E80" t="s">
-        <v>168</v>
-      </c>
-      <c r="F80" t="s">
-        <v>374</v>
-      </c>
-      <c r="G80" t="s">
+      <c r="D82" t="s">
+        <v>447</v>
+      </c>
+      <c r="E82" t="s">
+        <v>169</v>
+      </c>
+      <c r="F82" t="s">
+        <v>220</v>
+      </c>
+      <c r="G82" t="s">
         <v>390</v>
-      </c>
-    </row>
-    <row r="81" spans="1:7" x14ac:dyDescent="0.2">
-      <c r="B81" t="s">
-        <v>225</v>
-      </c>
-      <c r="C81" t="s">
-        <v>400</v>
-      </c>
-      <c r="D81" t="s">
-        <v>447</v>
-      </c>
-      <c r="E81" t="s">
-        <v>169</v>
-      </c>
-      <c r="F81" t="s">
-        <v>210</v>
-      </c>
-      <c r="G81" t="s">
-        <v>384</v>
-      </c>
-    </row>
-    <row r="82" spans="1:7" x14ac:dyDescent="0.2">
-      <c r="A82" t="s">
-        <v>11</v>
-      </c>
-      <c r="B82" s="3" t="s">
-        <v>112</v>
-      </c>
-      <c r="C82" s="4" t="s">
-        <v>193</v>
-      </c>
-      <c r="D82" t="s">
-        <v>102</v>
-      </c>
-      <c r="E82" t="s">
-        <v>168</v>
-      </c>
-      <c r="G82" t="s">
-        <v>97</v>
       </c>
     </row>
     <row r="83" spans="1:7" x14ac:dyDescent="0.2">
       <c r="A83" t="s">
-        <v>12</v>
+        <v>13</v>
       </c>
       <c r="B83" s="3" t="s">
-        <v>113</v>
+        <v>114</v>
       </c>
       <c r="C83" s="4" t="s">
         <v>193</v>
@@ -4138,71 +4156,71 @@
       </c>
     </row>
     <row r="84" spans="1:7" x14ac:dyDescent="0.2">
-      <c r="B84" t="s">
-        <v>378</v>
-      </c>
-      <c r="C84" t="s">
-        <v>434</v>
+      <c r="A84" t="s">
+        <v>60</v>
+      </c>
+      <c r="B84" s="3" t="s">
+        <v>161</v>
+      </c>
+      <c r="C84" s="3" t="s">
+        <v>196</v>
       </c>
       <c r="D84" t="s">
-        <v>447</v>
+        <v>102</v>
       </c>
       <c r="E84" t="s">
-        <v>169</v>
+        <v>168</v>
       </c>
       <c r="F84" t="s">
-        <v>220</v>
+        <v>164</v>
       </c>
       <c r="G84" t="s">
-        <v>390</v>
+        <v>100</v>
       </c>
     </row>
     <row r="85" spans="1:7" x14ac:dyDescent="0.2">
-      <c r="A85" t="s">
-        <v>13</v>
-      </c>
-      <c r="B85" s="3" t="s">
-        <v>114</v>
-      </c>
-      <c r="C85" s="4" t="s">
-        <v>193</v>
+      <c r="B85" t="s">
+        <v>251</v>
+      </c>
+      <c r="C85" t="s">
+        <v>400</v>
       </c>
       <c r="D85" t="s">
-        <v>102</v>
+        <v>447</v>
       </c>
       <c r="E85" t="s">
-        <v>168</v>
+        <v>169</v>
+      </c>
+      <c r="F85" t="s">
+        <v>237</v>
       </c>
       <c r="G85" t="s">
-        <v>97</v>
+        <v>393</v>
       </c>
     </row>
     <row r="86" spans="1:7" x14ac:dyDescent="0.2">
-      <c r="A86" t="s">
-        <v>60</v>
-      </c>
-      <c r="B86" s="3" t="s">
-        <v>161</v>
-      </c>
-      <c r="C86" s="3" t="s">
-        <v>196</v>
+      <c r="B86" t="s">
+        <v>252</v>
+      </c>
+      <c r="C86" t="s">
+        <v>400</v>
       </c>
       <c r="D86" t="s">
-        <v>102</v>
+        <v>447</v>
       </c>
       <c r="E86" t="s">
-        <v>168</v>
+        <v>169</v>
       </c>
       <c r="F86" t="s">
-        <v>164</v>
+        <v>238</v>
       </c>
       <c r="G86" t="s">
-        <v>100</v>
+        <v>393</v>
       </c>
     </row>
     <row r="87" spans="1:7" x14ac:dyDescent="0.2">
       <c r="B87" t="s">
-        <v>251</v>
+        <v>256</v>
       </c>
       <c r="C87" t="s">
         <v>400</v>
@@ -4214,7 +4232,7 @@
         <v>169</v>
       </c>
       <c r="F87" t="s">
-        <v>237</v>
+        <v>242</v>
       </c>
       <c r="G87" t="s">
         <v>393</v>
@@ -4222,7 +4240,7 @@
     </row>
     <row r="88" spans="1:7" x14ac:dyDescent="0.2">
       <c r="B88" t="s">
-        <v>252</v>
+        <v>255</v>
       </c>
       <c r="C88" t="s">
         <v>400</v>
@@ -4234,7 +4252,7 @@
         <v>169</v>
       </c>
       <c r="F88" t="s">
-        <v>238</v>
+        <v>241</v>
       </c>
       <c r="G88" t="s">
         <v>393</v>
@@ -4242,7 +4260,7 @@
     </row>
     <row r="89" spans="1:7" x14ac:dyDescent="0.2">
       <c r="B89" t="s">
-        <v>256</v>
+        <v>254</v>
       </c>
       <c r="C89" t="s">
         <v>400</v>
@@ -4254,7 +4272,7 @@
         <v>169</v>
       </c>
       <c r="F89" t="s">
-        <v>242</v>
+        <v>240</v>
       </c>
       <c r="G89" t="s">
         <v>393</v>
@@ -4262,7 +4280,7 @@
     </row>
     <row r="90" spans="1:7" x14ac:dyDescent="0.2">
       <c r="B90" t="s">
-        <v>255</v>
+        <v>253</v>
       </c>
       <c r="C90" t="s">
         <v>400</v>
@@ -4274,7 +4292,7 @@
         <v>169</v>
       </c>
       <c r="F90" t="s">
-        <v>241</v>
+        <v>239</v>
       </c>
       <c r="G90" t="s">
         <v>393</v>
@@ -4282,70 +4300,73 @@
     </row>
     <row r="91" spans="1:7" x14ac:dyDescent="0.2">
       <c r="B91" t="s">
-        <v>254</v>
+        <v>382</v>
       </c>
       <c r="C91" t="s">
-        <v>400</v>
+        <v>434</v>
       </c>
       <c r="D91" t="s">
         <v>447</v>
       </c>
       <c r="E91" t="s">
-        <v>169</v>
+        <v>168</v>
       </c>
       <c r="F91" t="s">
-        <v>240</v>
+        <v>373</v>
       </c>
       <c r="G91" t="s">
-        <v>393</v>
+        <v>390</v>
       </c>
     </row>
     <row r="92" spans="1:7" x14ac:dyDescent="0.2">
       <c r="B92" t="s">
-        <v>253</v>
+        <v>398</v>
       </c>
       <c r="C92" t="s">
-        <v>400</v>
+        <v>403</v>
       </c>
       <c r="D92" t="s">
-        <v>447</v>
+        <v>102</v>
       </c>
       <c r="E92" t="s">
-        <v>169</v>
+        <v>168</v>
       </c>
       <c r="F92" t="s">
-        <v>239</v>
+        <v>213</v>
       </c>
       <c r="G92" t="s">
-        <v>393</v>
+        <v>402</v>
       </c>
     </row>
     <row r="93" spans="1:7" x14ac:dyDescent="0.2">
       <c r="B93" t="s">
-        <v>382</v>
+        <v>407</v>
       </c>
       <c r="C93" t="s">
-        <v>434</v>
+        <v>203</v>
       </c>
       <c r="D93" t="s">
-        <v>447</v>
+        <v>102</v>
       </c>
       <c r="E93" t="s">
-        <v>168</v>
+        <v>169</v>
       </c>
       <c r="F93" t="s">
-        <v>373</v>
+        <v>230</v>
       </c>
       <c r="G93" t="s">
-        <v>390</v>
+        <v>391</v>
       </c>
     </row>
     <row r="94" spans="1:7" x14ac:dyDescent="0.2">
-      <c r="B94" t="s">
-        <v>398</v>
-      </c>
-      <c r="C94" t="s">
-        <v>403</v>
+      <c r="A94" t="s">
+        <v>14</v>
+      </c>
+      <c r="B94" s="3" t="s">
+        <v>115</v>
+      </c>
+      <c r="C94" s="4" t="s">
+        <v>193</v>
       </c>
       <c r="D94" t="s">
         <v>102</v>
@@ -4353,79 +4374,76 @@
       <c r="E94" t="s">
         <v>168</v>
       </c>
-      <c r="F94" t="s">
-        <v>213</v>
-      </c>
       <c r="G94" t="s">
-        <v>402</v>
+        <v>97</v>
       </c>
     </row>
     <row r="95" spans="1:7" x14ac:dyDescent="0.2">
-      <c r="B95" t="s">
-        <v>407</v>
-      </c>
-      <c r="C95" t="s">
-        <v>203</v>
+      <c r="A95" t="s">
+        <v>15</v>
+      </c>
+      <c r="B95" s="3" t="s">
+        <v>116</v>
+      </c>
+      <c r="C95" s="4" t="s">
+        <v>193</v>
       </c>
       <c r="D95" t="s">
         <v>102</v>
       </c>
       <c r="E95" t="s">
-        <v>169</v>
-      </c>
-      <c r="F95" t="s">
-        <v>230</v>
+        <v>168</v>
       </c>
       <c r="G95" t="s">
-        <v>391</v>
+        <v>97</v>
       </c>
     </row>
     <row r="96" spans="1:7" x14ac:dyDescent="0.2">
       <c r="A96" t="s">
-        <v>14</v>
+        <v>45</v>
       </c>
       <c r="B96" s="3" t="s">
-        <v>115</v>
-      </c>
-      <c r="C96" s="4" t="s">
-        <v>193</v>
+        <v>146</v>
+      </c>
+      <c r="C96" s="3" t="s">
+        <v>194</v>
       </c>
       <c r="D96" t="s">
-        <v>102</v>
+        <v>447</v>
       </c>
       <c r="E96" t="s">
-        <v>168</v>
+        <v>169</v>
       </c>
       <c r="G96" t="s">
-        <v>97</v>
+        <v>98</v>
       </c>
     </row>
     <row r="97" spans="1:7" x14ac:dyDescent="0.2">
       <c r="A97" t="s">
-        <v>15</v>
+        <v>46</v>
       </c>
       <c r="B97" s="3" t="s">
-        <v>116</v>
-      </c>
-      <c r="C97" s="4" t="s">
-        <v>193</v>
+        <v>147</v>
+      </c>
+      <c r="C97" s="3" t="s">
+        <v>194</v>
       </c>
       <c r="D97" t="s">
-        <v>102</v>
+        <v>447</v>
       </c>
       <c r="E97" t="s">
-        <v>168</v>
+        <v>169</v>
       </c>
       <c r="G97" t="s">
-        <v>97</v>
+        <v>98</v>
       </c>
     </row>
     <row r="98" spans="1:7" x14ac:dyDescent="0.2">
       <c r="A98" t="s">
-        <v>45</v>
+        <v>47</v>
       </c>
       <c r="B98" s="3" t="s">
-        <v>146</v>
+        <v>148</v>
       </c>
       <c r="C98" s="3" t="s">
         <v>194</v>
@@ -4442,10 +4460,10 @@
     </row>
     <row r="99" spans="1:7" x14ac:dyDescent="0.2">
       <c r="A99" t="s">
-        <v>46</v>
+        <v>48</v>
       </c>
       <c r="B99" s="3" t="s">
-        <v>147</v>
+        <v>149</v>
       </c>
       <c r="C99" s="3" t="s">
         <v>194</v>
@@ -4462,10 +4480,10 @@
     </row>
     <row r="100" spans="1:7" x14ac:dyDescent="0.2">
       <c r="A100" t="s">
-        <v>47</v>
+        <v>49</v>
       </c>
       <c r="B100" s="3" t="s">
-        <v>148</v>
+        <v>150</v>
       </c>
       <c r="C100" s="3" t="s">
         <v>194</v>
@@ -4482,10 +4500,10 @@
     </row>
     <row r="101" spans="1:7" x14ac:dyDescent="0.2">
       <c r="A101" t="s">
-        <v>48</v>
+        <v>50</v>
       </c>
       <c r="B101" s="3" t="s">
-        <v>149</v>
+        <v>151</v>
       </c>
       <c r="C101" s="3" t="s">
         <v>194</v>
@@ -4502,10 +4520,10 @@
     </row>
     <row r="102" spans="1:7" x14ac:dyDescent="0.2">
       <c r="A102" t="s">
-        <v>49</v>
+        <v>51</v>
       </c>
       <c r="B102" s="3" t="s">
-        <v>150</v>
+        <v>152</v>
       </c>
       <c r="C102" s="3" t="s">
         <v>194</v>
@@ -4522,10 +4540,10 @@
     </row>
     <row r="103" spans="1:7" x14ac:dyDescent="0.2">
       <c r="A103" t="s">
-        <v>50</v>
+        <v>52</v>
       </c>
       <c r="B103" s="3" t="s">
-        <v>151</v>
+        <v>153</v>
       </c>
       <c r="C103" s="3" t="s">
         <v>194</v>
@@ -4542,10 +4560,10 @@
     </row>
     <row r="104" spans="1:7" x14ac:dyDescent="0.2">
       <c r="A104" t="s">
-        <v>51</v>
+        <v>53</v>
       </c>
       <c r="B104" s="3" t="s">
-        <v>152</v>
+        <v>154</v>
       </c>
       <c r="C104" s="3" t="s">
         <v>194</v>
@@ -4562,10 +4580,10 @@
     </row>
     <row r="105" spans="1:7" x14ac:dyDescent="0.2">
       <c r="A105" t="s">
-        <v>52</v>
+        <v>54</v>
       </c>
       <c r="B105" s="3" t="s">
-        <v>153</v>
+        <v>155</v>
       </c>
       <c r="C105" s="3" t="s">
         <v>194</v>
@@ -4581,74 +4599,71 @@
       </c>
     </row>
     <row r="106" spans="1:7" x14ac:dyDescent="0.2">
-      <c r="A106" t="s">
-        <v>53</v>
-      </c>
-      <c r="B106" s="3" t="s">
-        <v>154</v>
-      </c>
-      <c r="C106" s="3" t="s">
-        <v>194</v>
+      <c r="B106" t="s">
+        <v>406</v>
+      </c>
+      <c r="C106" t="s">
+        <v>203</v>
       </c>
       <c r="D106" t="s">
-        <v>447</v>
+        <v>102</v>
       </c>
       <c r="E106" t="s">
         <v>169</v>
       </c>
+      <c r="F106" t="s">
+        <v>229</v>
+      </c>
       <c r="G106" t="s">
-        <v>98</v>
+        <v>391</v>
       </c>
     </row>
     <row r="107" spans="1:7" x14ac:dyDescent="0.2">
       <c r="A107" t="s">
-        <v>54</v>
+        <v>16</v>
       </c>
       <c r="B107" s="3" t="s">
-        <v>155</v>
-      </c>
-      <c r="C107" s="3" t="s">
-        <v>194</v>
+        <v>117</v>
+      </c>
+      <c r="C107" s="4" t="s">
+        <v>193</v>
       </c>
       <c r="D107" t="s">
-        <v>447</v>
+        <v>102</v>
       </c>
       <c r="E107" t="s">
-        <v>169</v>
+        <v>168</v>
       </c>
       <c r="G107" t="s">
-        <v>98</v>
+        <v>97</v>
       </c>
     </row>
     <row r="108" spans="1:7" x14ac:dyDescent="0.2">
       <c r="B108" t="s">
-        <v>406</v>
-      </c>
-      <c r="C108" t="s">
-        <v>203</v>
+        <v>92</v>
+      </c>
+      <c r="C108" s="2" t="s">
+        <v>197</v>
       </c>
       <c r="D108" t="s">
-        <v>102</v>
+        <v>447</v>
       </c>
       <c r="E108" t="s">
-        <v>169</v>
-      </c>
-      <c r="F108" t="s">
-        <v>229</v>
+        <v>168</v>
       </c>
       <c r="G108" t="s">
-        <v>391</v>
+        <v>204</v>
       </c>
     </row>
     <row r="109" spans="1:7" x14ac:dyDescent="0.2">
       <c r="A109" t="s">
-        <v>16</v>
+        <v>62</v>
       </c>
       <c r="B109" s="3" t="s">
-        <v>117</v>
-      </c>
-      <c r="C109" s="4" t="s">
-        <v>193</v>
+        <v>162</v>
+      </c>
+      <c r="C109" s="3" t="s">
+        <v>196</v>
       </c>
       <c r="D109" t="s">
         <v>102</v>
@@ -4656,70 +4671,73 @@
       <c r="E109" t="s">
         <v>168</v>
       </c>
+      <c r="F109" t="s">
+        <v>165</v>
+      </c>
       <c r="G109" t="s">
-        <v>97</v>
+        <v>100</v>
       </c>
     </row>
     <row r="110" spans="1:7" x14ac:dyDescent="0.2">
       <c r="B110" t="s">
-        <v>92</v>
-      </c>
-      <c r="C110" s="2" t="s">
-        <v>197</v>
+        <v>336</v>
+      </c>
+      <c r="C110" t="s">
+        <v>449</v>
       </c>
       <c r="D110" t="s">
         <v>447</v>
       </c>
-      <c r="E110" t="s">
-        <v>168</v>
+      <c r="F110" t="s">
+        <v>334</v>
       </c>
       <c r="G110" t="s">
-        <v>204</v>
+        <v>395</v>
       </c>
     </row>
     <row r="111" spans="1:7" x14ac:dyDescent="0.2">
-      <c r="A111" t="s">
-        <v>62</v>
-      </c>
-      <c r="B111" s="3" t="s">
-        <v>162</v>
-      </c>
-      <c r="C111" s="3" t="s">
-        <v>196</v>
+      <c r="B111" t="s">
+        <v>260</v>
+      </c>
+      <c r="C111" t="s">
+        <v>400</v>
       </c>
       <c r="D111" t="s">
-        <v>102</v>
+        <v>447</v>
       </c>
       <c r="E111" t="s">
-        <v>168</v>
+        <v>169</v>
       </c>
       <c r="F111" t="s">
-        <v>165</v>
+        <v>247</v>
       </c>
       <c r="G111" t="s">
-        <v>100</v>
+        <v>393</v>
       </c>
     </row>
     <row r="112" spans="1:7" x14ac:dyDescent="0.2">
       <c r="B112" t="s">
-        <v>336</v>
+        <v>261</v>
       </c>
       <c r="C112" t="s">
-        <v>449</v>
+        <v>400</v>
       </c>
       <c r="D112" t="s">
         <v>447</v>
       </c>
+      <c r="E112" t="s">
+        <v>169</v>
+      </c>
       <c r="F112" t="s">
-        <v>334</v>
+        <v>246</v>
       </c>
       <c r="G112" t="s">
-        <v>395</v>
+        <v>393</v>
       </c>
     </row>
     <row r="113" spans="1:7" x14ac:dyDescent="0.2">
       <c r="B113" t="s">
-        <v>260</v>
+        <v>259</v>
       </c>
       <c r="C113" t="s">
         <v>400</v>
@@ -4731,7 +4749,7 @@
         <v>169</v>
       </c>
       <c r="F113" t="s">
-        <v>247</v>
+        <v>248</v>
       </c>
       <c r="G113" t="s">
         <v>393</v>
@@ -4739,27 +4757,27 @@
     </row>
     <row r="114" spans="1:7" x14ac:dyDescent="0.2">
       <c r="B114" t="s">
-        <v>261</v>
+        <v>396</v>
       </c>
       <c r="C114" t="s">
-        <v>400</v>
+        <v>403</v>
       </c>
       <c r="D114" t="s">
-        <v>447</v>
+        <v>102</v>
       </c>
       <c r="E114" t="s">
-        <v>169</v>
+        <v>168</v>
       </c>
       <c r="F114" t="s">
-        <v>246</v>
+        <v>211</v>
       </c>
       <c r="G114" t="s">
-        <v>393</v>
+        <v>386</v>
       </c>
     </row>
     <row r="115" spans="1:7" x14ac:dyDescent="0.2">
       <c r="B115" t="s">
-        <v>259</v>
+        <v>419</v>
       </c>
       <c r="C115" t="s">
         <v>400</v>
@@ -4768,41 +4786,38 @@
         <v>447</v>
       </c>
       <c r="E115" t="s">
-        <v>169</v>
+        <v>168</v>
       </c>
       <c r="F115" t="s">
-        <v>248</v>
+        <v>421</v>
       </c>
       <c r="G115" t="s">
-        <v>393</v>
+        <v>389</v>
       </c>
     </row>
     <row r="116" spans="1:7" x14ac:dyDescent="0.2">
       <c r="B116" t="s">
-        <v>396</v>
+        <v>93</v>
       </c>
       <c r="C116" t="s">
-        <v>403</v>
+        <v>200</v>
       </c>
       <c r="D116" t="s">
-        <v>102</v>
+        <v>447</v>
       </c>
       <c r="E116" t="s">
         <v>168</v>
       </c>
-      <c r="F116" t="s">
-        <v>211</v>
-      </c>
       <c r="G116" t="s">
-        <v>386</v>
+        <v>207</v>
       </c>
     </row>
     <row r="117" spans="1:7" x14ac:dyDescent="0.2">
       <c r="B117" t="s">
-        <v>419</v>
-      </c>
-      <c r="C117" t="s">
-        <v>400</v>
+        <v>94</v>
+      </c>
+      <c r="C117" s="2" t="s">
+        <v>197</v>
       </c>
       <c r="D117" t="s">
         <v>447</v>
@@ -4810,107 +4825,110 @@
       <c r="E117" t="s">
         <v>168</v>
       </c>
-      <c r="F117" t="s">
-        <v>421</v>
-      </c>
       <c r="G117" t="s">
-        <v>389</v>
+        <v>204</v>
       </c>
     </row>
     <row r="118" spans="1:7" x14ac:dyDescent="0.2">
-      <c r="B118" t="s">
-        <v>93</v>
-      </c>
-      <c r="C118" t="s">
-        <v>200</v>
+      <c r="A118" t="s">
+        <v>17</v>
+      </c>
+      <c r="B118" s="3" t="s">
+        <v>118</v>
+      </c>
+      <c r="C118" s="4" t="s">
+        <v>193</v>
       </c>
       <c r="D118" t="s">
-        <v>447</v>
+        <v>102</v>
       </c>
       <c r="E118" t="s">
         <v>168</v>
       </c>
       <c r="G118" t="s">
-        <v>207</v>
+        <v>97</v>
       </c>
     </row>
     <row r="119" spans="1:7" x14ac:dyDescent="0.2">
       <c r="B119" t="s">
-        <v>94</v>
-      </c>
-      <c r="C119" s="2" t="s">
-        <v>197</v>
+        <v>409</v>
+      </c>
+      <c r="C119" t="s">
+        <v>403</v>
       </c>
       <c r="D119" t="s">
-        <v>447</v>
+        <v>102</v>
       </c>
       <c r="E119" t="s">
-        <v>168</v>
+        <v>169</v>
+      </c>
+      <c r="F119" t="s">
+        <v>412</v>
       </c>
       <c r="G119" t="s">
-        <v>204</v>
+        <v>410</v>
       </c>
     </row>
     <row r="120" spans="1:7" x14ac:dyDescent="0.2">
-      <c r="A120" t="s">
-        <v>17</v>
-      </c>
-      <c r="B120" s="3" t="s">
-        <v>118</v>
-      </c>
-      <c r="C120" s="4" t="s">
-        <v>193</v>
+      <c r="B120" t="s">
+        <v>95</v>
+      </c>
+      <c r="C120" t="s">
+        <v>202</v>
       </c>
       <c r="D120" t="s">
         <v>102</v>
       </c>
       <c r="E120" t="s">
-        <v>168</v>
+        <v>169</v>
       </c>
       <c r="G120" t="s">
-        <v>97</v>
+        <v>208</v>
       </c>
     </row>
     <row r="121" spans="1:7" x14ac:dyDescent="0.2">
       <c r="B121" t="s">
-        <v>409</v>
+        <v>333</v>
       </c>
       <c r="C121" t="s">
-        <v>403</v>
+        <v>401</v>
       </c>
       <c r="D121" t="s">
         <v>102</v>
       </c>
       <c r="E121" t="s">
-        <v>169</v>
+        <v>168</v>
       </c>
       <c r="F121" t="s">
-        <v>412</v>
+        <v>319</v>
       </c>
       <c r="G121" t="s">
-        <v>410</v>
+        <v>385</v>
       </c>
     </row>
     <row r="122" spans="1:7" x14ac:dyDescent="0.2">
       <c r="B122" t="s">
-        <v>95</v>
+        <v>329</v>
       </c>
       <c r="C122" t="s">
-        <v>202</v>
+        <v>401</v>
       </c>
       <c r="D122" t="s">
         <v>102</v>
       </c>
       <c r="E122" t="s">
-        <v>169</v>
+        <v>168</v>
+      </c>
+      <c r="F122" t="s">
+        <v>315</v>
       </c>
       <c r="G122" t="s">
-        <v>208</v>
+        <v>385</v>
       </c>
     </row>
     <row r="123" spans="1:7" x14ac:dyDescent="0.2">
       <c r="B123" t="s">
-        <v>333</v>
+        <v>327</v>
       </c>
       <c r="C123" t="s">
         <v>401</v>
@@ -4922,7 +4940,7 @@
         <v>168</v>
       </c>
       <c r="F123" t="s">
-        <v>319</v>
+        <v>313</v>
       </c>
       <c r="G123" t="s">
         <v>385</v>
@@ -4930,7 +4948,7 @@
     </row>
     <row r="124" spans="1:7" x14ac:dyDescent="0.2">
       <c r="B124" t="s">
-        <v>329</v>
+        <v>331</v>
       </c>
       <c r="C124" t="s">
         <v>401</v>
@@ -4939,10 +4957,10 @@
         <v>102</v>
       </c>
       <c r="E124" t="s">
-        <v>168</v>
+        <v>169</v>
       </c>
       <c r="F124" t="s">
-        <v>315</v>
+        <v>317</v>
       </c>
       <c r="G124" t="s">
         <v>385</v>
@@ -4950,7 +4968,7 @@
     </row>
     <row r="125" spans="1:7" x14ac:dyDescent="0.2">
       <c r="B125" t="s">
-        <v>327</v>
+        <v>330</v>
       </c>
       <c r="C125" t="s">
         <v>401</v>
@@ -4962,7 +4980,7 @@
         <v>168</v>
       </c>
       <c r="F125" t="s">
-        <v>313</v>
+        <v>316</v>
       </c>
       <c r="G125" t="s">
         <v>385</v>
@@ -4970,7 +4988,7 @@
     </row>
     <row r="126" spans="1:7" x14ac:dyDescent="0.2">
       <c r="B126" t="s">
-        <v>331</v>
+        <v>328</v>
       </c>
       <c r="C126" t="s">
         <v>401</v>
@@ -4979,10 +4997,10 @@
         <v>102</v>
       </c>
       <c r="E126" t="s">
-        <v>169</v>
+        <v>168</v>
       </c>
       <c r="F126" t="s">
-        <v>317</v>
+        <v>314</v>
       </c>
       <c r="G126" t="s">
         <v>385</v>
@@ -4990,7 +5008,7 @@
     </row>
     <row r="127" spans="1:7" x14ac:dyDescent="0.2">
       <c r="B127" t="s">
-        <v>330</v>
+        <v>332</v>
       </c>
       <c r="C127" t="s">
         <v>401</v>
@@ -4999,10 +5017,10 @@
         <v>102</v>
       </c>
       <c r="E127" t="s">
-        <v>168</v>
+        <v>169</v>
       </c>
       <c r="F127" t="s">
-        <v>316</v>
+        <v>318</v>
       </c>
       <c r="G127" t="s">
         <v>385</v>
@@ -5010,113 +5028,113 @@
     </row>
     <row r="128" spans="1:7" x14ac:dyDescent="0.2">
       <c r="B128" t="s">
-        <v>328</v>
+        <v>377</v>
       </c>
       <c r="C128" t="s">
-        <v>401</v>
+        <v>434</v>
       </c>
       <c r="D128" t="s">
-        <v>102</v>
+        <v>447</v>
       </c>
       <c r="E128" t="s">
-        <v>168</v>
+        <v>169</v>
       </c>
       <c r="F128" t="s">
-        <v>314</v>
+        <v>219</v>
       </c>
       <c r="G128" t="s">
-        <v>385</v>
+        <v>390</v>
       </c>
     </row>
     <row r="129" spans="1:19" x14ac:dyDescent="0.2">
       <c r="B129" t="s">
-        <v>332</v>
+        <v>96</v>
       </c>
       <c r="C129" t="s">
-        <v>401</v>
+        <v>203</v>
       </c>
       <c r="D129" t="s">
         <v>102</v>
       </c>
       <c r="E129" t="s">
-        <v>169</v>
-      </c>
-      <c r="F129" t="s">
-        <v>318</v>
+        <v>168</v>
       </c>
       <c r="G129" t="s">
-        <v>385</v>
+        <v>209</v>
+      </c>
+      <c r="S129" t="s">
+        <v>235</v>
       </c>
     </row>
     <row r="130" spans="1:19" x14ac:dyDescent="0.2">
       <c r="B130" t="s">
-        <v>377</v>
+        <v>399</v>
       </c>
       <c r="C130" t="s">
-        <v>434</v>
+        <v>403</v>
       </c>
       <c r="D130" t="s">
-        <v>447</v>
+        <v>102</v>
       </c>
       <c r="E130" t="s">
-        <v>169</v>
+        <v>168</v>
       </c>
       <c r="F130" t="s">
-        <v>219</v>
+        <v>214</v>
       </c>
       <c r="G130" t="s">
-        <v>390</v>
+        <v>402</v>
+      </c>
+      <c r="S130" t="s">
+        <v>234</v>
       </c>
     </row>
     <row r="131" spans="1:19" x14ac:dyDescent="0.2">
-      <c r="B131" t="s">
-        <v>96</v>
-      </c>
-      <c r="C131" t="s">
-        <v>203</v>
+      <c r="A131" t="s">
+        <v>66</v>
+      </c>
+      <c r="B131" s="3" t="s">
+        <v>174</v>
+      </c>
+      <c r="C131" s="3" t="s">
+        <v>201</v>
       </c>
       <c r="D131" t="s">
-        <v>102</v>
+        <v>447</v>
       </c>
       <c r="E131" t="s">
-        <v>168</v>
+        <v>169</v>
       </c>
       <c r="G131" t="s">
-        <v>209</v>
-      </c>
-      <c r="S131" t="s">
-        <v>235</v>
+        <v>101</v>
       </c>
     </row>
     <row r="132" spans="1:19" x14ac:dyDescent="0.2">
-      <c r="B132" t="s">
-        <v>399</v>
-      </c>
-      <c r="C132" t="s">
-        <v>403</v>
+      <c r="A132" t="s">
+        <v>67</v>
+      </c>
+      <c r="B132" s="3" t="s">
+        <v>175</v>
+      </c>
+      <c r="C132" s="3" t="s">
+        <v>201</v>
       </c>
       <c r="D132" t="s">
-        <v>102</v>
+        <v>447</v>
       </c>
       <c r="E132" t="s">
-        <v>168</v>
-      </c>
-      <c r="F132" t="s">
-        <v>214</v>
+        <v>169</v>
       </c>
       <c r="G132" t="s">
-        <v>402</v>
-      </c>
-      <c r="S132" t="s">
-        <v>234</v>
+        <v>101</v>
       </c>
     </row>
     <row r="133" spans="1:19" x14ac:dyDescent="0.2">
       <c r="A133" t="s">
-        <v>66</v>
+        <v>68</v>
       </c>
       <c r="B133" s="3" t="s">
-        <v>174</v>
+        <v>176</v>
       </c>
       <c r="C133" s="3" t="s">
         <v>201</v>
@@ -5133,10 +5151,10 @@
     </row>
     <row r="134" spans="1:19" x14ac:dyDescent="0.2">
       <c r="A134" t="s">
-        <v>67</v>
+        <v>64</v>
       </c>
       <c r="B134" s="3" t="s">
-        <v>175</v>
+        <v>172</v>
       </c>
       <c r="C134" s="3" t="s">
         <v>201</v>
@@ -5153,10 +5171,10 @@
     </row>
     <row r="135" spans="1:19" x14ac:dyDescent="0.2">
       <c r="A135" t="s">
-        <v>68</v>
+        <v>70</v>
       </c>
       <c r="B135" s="3" t="s">
-        <v>176</v>
+        <v>178</v>
       </c>
       <c r="C135" s="3" t="s">
         <v>201</v>
@@ -5173,10 +5191,10 @@
     </row>
     <row r="136" spans="1:19" x14ac:dyDescent="0.2">
       <c r="A136" t="s">
-        <v>64</v>
+        <v>65</v>
       </c>
       <c r="B136" s="3" t="s">
-        <v>172</v>
+        <v>173</v>
       </c>
       <c r="C136" s="3" t="s">
         <v>201</v>
@@ -5193,10 +5211,10 @@
     </row>
     <row r="137" spans="1:19" x14ac:dyDescent="0.2">
       <c r="A137" t="s">
-        <v>70</v>
+        <v>72</v>
       </c>
       <c r="B137" s="3" t="s">
-        <v>178</v>
+        <v>180</v>
       </c>
       <c r="C137" s="3" t="s">
         <v>201</v>
@@ -5213,10 +5231,10 @@
     </row>
     <row r="138" spans="1:19" x14ac:dyDescent="0.2">
       <c r="A138" t="s">
-        <v>65</v>
+        <v>69</v>
       </c>
       <c r="B138" s="3" t="s">
-        <v>173</v>
+        <v>177</v>
       </c>
       <c r="C138" s="3" t="s">
         <v>201</v>
@@ -5233,10 +5251,10 @@
     </row>
     <row r="139" spans="1:19" x14ac:dyDescent="0.2">
       <c r="A139" t="s">
-        <v>72</v>
+        <v>61</v>
       </c>
       <c r="B139" s="3" t="s">
-        <v>180</v>
+        <v>170</v>
       </c>
       <c r="C139" s="3" t="s">
         <v>201</v>
@@ -5253,10 +5271,10 @@
     </row>
     <row r="140" spans="1:19" x14ac:dyDescent="0.2">
       <c r="A140" t="s">
-        <v>69</v>
+        <v>63</v>
       </c>
       <c r="B140" s="3" t="s">
-        <v>177</v>
+        <v>171</v>
       </c>
       <c r="C140" s="3" t="s">
         <v>201</v>
@@ -5273,10 +5291,10 @@
     </row>
     <row r="141" spans="1:19" x14ac:dyDescent="0.2">
       <c r="A141" t="s">
-        <v>61</v>
+        <v>71</v>
       </c>
       <c r="B141" s="3" t="s">
-        <v>170</v>
+        <v>179</v>
       </c>
       <c r="C141" s="3" t="s">
         <v>201</v>
@@ -5293,10 +5311,10 @@
     </row>
     <row r="142" spans="1:19" x14ac:dyDescent="0.2">
       <c r="A142" t="s">
-        <v>63</v>
+        <v>77</v>
       </c>
       <c r="B142" s="3" t="s">
-        <v>171</v>
+        <v>185</v>
       </c>
       <c r="C142" s="3" t="s">
         <v>201</v>
@@ -5313,10 +5331,10 @@
     </row>
     <row r="143" spans="1:19" x14ac:dyDescent="0.2">
       <c r="A143" t="s">
-        <v>71</v>
+        <v>78</v>
       </c>
       <c r="B143" s="3" t="s">
-        <v>179</v>
+        <v>186</v>
       </c>
       <c r="C143" s="3" t="s">
         <v>201</v>
@@ -5333,10 +5351,10 @@
     </row>
     <row r="144" spans="1:19" x14ac:dyDescent="0.2">
       <c r="A144" t="s">
-        <v>77</v>
+        <v>79</v>
       </c>
       <c r="B144" s="3" t="s">
-        <v>185</v>
+        <v>187</v>
       </c>
       <c r="C144" s="3" t="s">
         <v>201</v>
@@ -5353,10 +5371,10 @@
     </row>
     <row r="145" spans="1:7" x14ac:dyDescent="0.2">
       <c r="A145" t="s">
-        <v>78</v>
+        <v>75</v>
       </c>
       <c r="B145" s="3" t="s">
-        <v>186</v>
+        <v>183</v>
       </c>
       <c r="C145" s="3" t="s">
         <v>201</v>
@@ -5373,10 +5391,10 @@
     </row>
     <row r="146" spans="1:7" x14ac:dyDescent="0.2">
       <c r="A146" t="s">
-        <v>79</v>
+        <v>81</v>
       </c>
       <c r="B146" s="3" t="s">
-        <v>187</v>
+        <v>189</v>
       </c>
       <c r="C146" s="3" t="s">
         <v>201</v>
@@ -5393,10 +5411,10 @@
     </row>
     <row r="147" spans="1:7" x14ac:dyDescent="0.2">
       <c r="A147" t="s">
-        <v>75</v>
+        <v>76</v>
       </c>
       <c r="B147" s="3" t="s">
-        <v>183</v>
+        <v>184</v>
       </c>
       <c r="C147" s="3" t="s">
         <v>201</v>
@@ -5413,10 +5431,10 @@
     </row>
     <row r="148" spans="1:7" x14ac:dyDescent="0.2">
       <c r="A148" t="s">
-        <v>81</v>
+        <v>83</v>
       </c>
       <c r="B148" s="3" t="s">
-        <v>189</v>
+        <v>191</v>
       </c>
       <c r="C148" s="3" t="s">
         <v>201</v>
@@ -5433,10 +5451,10 @@
     </row>
     <row r="149" spans="1:7" x14ac:dyDescent="0.2">
       <c r="A149" t="s">
-        <v>76</v>
+        <v>80</v>
       </c>
       <c r="B149" s="3" t="s">
-        <v>184</v>
+        <v>188</v>
       </c>
       <c r="C149" s="3" t="s">
         <v>201</v>
@@ -5453,10 +5471,10 @@
     </row>
     <row r="150" spans="1:7" x14ac:dyDescent="0.2">
       <c r="A150" t="s">
-        <v>83</v>
+        <v>73</v>
       </c>
       <c r="B150" s="3" t="s">
-        <v>191</v>
+        <v>181</v>
       </c>
       <c r="C150" s="3" t="s">
         <v>201</v>
@@ -5473,10 +5491,10 @@
     </row>
     <row r="151" spans="1:7" x14ac:dyDescent="0.2">
       <c r="A151" t="s">
-        <v>80</v>
+        <v>74</v>
       </c>
       <c r="B151" s="3" t="s">
-        <v>188</v>
+        <v>182</v>
       </c>
       <c r="C151" s="3" t="s">
         <v>201</v>
@@ -5493,10 +5511,10 @@
     </row>
     <row r="152" spans="1:7" x14ac:dyDescent="0.2">
       <c r="A152" t="s">
-        <v>73</v>
+        <v>82</v>
       </c>
       <c r="B152" s="3" t="s">
-        <v>181</v>
+        <v>190</v>
       </c>
       <c r="C152" s="3" t="s">
         <v>201</v>
@@ -5512,48 +5530,48 @@
       </c>
     </row>
     <row r="153" spans="1:7" x14ac:dyDescent="0.2">
-      <c r="A153" t="s">
-        <v>74</v>
-      </c>
-      <c r="B153" s="3" t="s">
-        <v>182</v>
-      </c>
-      <c r="C153" s="3" t="s">
-        <v>201</v>
+      <c r="B153" t="s">
+        <v>359</v>
+      </c>
+      <c r="C153" t="s">
+        <v>400</v>
       </c>
       <c r="D153" t="s">
         <v>447</v>
       </c>
       <c r="E153" t="s">
-        <v>169</v>
+        <v>168</v>
+      </c>
+      <c r="F153" t="s">
+        <v>237</v>
       </c>
       <c r="G153" t="s">
-        <v>101</v>
+        <v>408</v>
       </c>
     </row>
     <row r="154" spans="1:7" x14ac:dyDescent="0.2">
-      <c r="A154" t="s">
-        <v>82</v>
-      </c>
-      <c r="B154" s="3" t="s">
-        <v>190</v>
-      </c>
-      <c r="C154" s="3" t="s">
-        <v>201</v>
+      <c r="B154" t="s">
+        <v>360</v>
+      </c>
+      <c r="C154" t="s">
+        <v>400</v>
       </c>
       <c r="D154" t="s">
         <v>447</v>
       </c>
       <c r="E154" t="s">
-        <v>169</v>
+        <v>168</v>
+      </c>
+      <c r="F154" t="s">
+        <v>238</v>
       </c>
       <c r="G154" t="s">
-        <v>101</v>
+        <v>408</v>
       </c>
     </row>
     <row r="155" spans="1:7" x14ac:dyDescent="0.2">
       <c r="B155" t="s">
-        <v>359</v>
+        <v>361</v>
       </c>
       <c r="C155" t="s">
         <v>400</v>
@@ -5565,7 +5583,7 @@
         <v>168</v>
       </c>
       <c r="F155" t="s">
-        <v>237</v>
+        <v>239</v>
       </c>
       <c r="G155" t="s">
         <v>408</v>
@@ -5573,7 +5591,7 @@
     </row>
     <row r="156" spans="1:7" x14ac:dyDescent="0.2">
       <c r="B156" t="s">
-        <v>360</v>
+        <v>362</v>
       </c>
       <c r="C156" t="s">
         <v>400</v>
@@ -5585,7 +5603,7 @@
         <v>168</v>
       </c>
       <c r="F156" t="s">
-        <v>238</v>
+        <v>240</v>
       </c>
       <c r="G156" t="s">
         <v>408</v>
@@ -5593,7 +5611,7 @@
     </row>
     <row r="157" spans="1:7" x14ac:dyDescent="0.2">
       <c r="B157" t="s">
-        <v>361</v>
+        <v>363</v>
       </c>
       <c r="C157" t="s">
         <v>400</v>
@@ -5605,7 +5623,7 @@
         <v>168</v>
       </c>
       <c r="F157" t="s">
-        <v>239</v>
+        <v>236</v>
       </c>
       <c r="G157" t="s">
         <v>408</v>
@@ -5613,7 +5631,7 @@
     </row>
     <row r="158" spans="1:7" x14ac:dyDescent="0.2">
       <c r="B158" t="s">
-        <v>362</v>
+        <v>364</v>
       </c>
       <c r="C158" t="s">
         <v>400</v>
@@ -5625,7 +5643,7 @@
         <v>168</v>
       </c>
       <c r="F158" t="s">
-        <v>240</v>
+        <v>246</v>
       </c>
       <c r="G158" t="s">
         <v>408</v>
@@ -5633,7 +5651,7 @@
     </row>
     <row r="159" spans="1:7" x14ac:dyDescent="0.2">
       <c r="B159" t="s">
-        <v>363</v>
+        <v>365</v>
       </c>
       <c r="C159" t="s">
         <v>400</v>
@@ -5645,7 +5663,7 @@
         <v>168</v>
       </c>
       <c r="F159" t="s">
-        <v>236</v>
+        <v>354</v>
       </c>
       <c r="G159" t="s">
         <v>408</v>
@@ -5653,7 +5671,7 @@
     </row>
     <row r="160" spans="1:7" x14ac:dyDescent="0.2">
       <c r="B160" t="s">
-        <v>364</v>
+        <v>366</v>
       </c>
       <c r="C160" t="s">
         <v>400</v>
@@ -5665,7 +5683,7 @@
         <v>168</v>
       </c>
       <c r="F160" t="s">
-        <v>246</v>
+        <v>355</v>
       </c>
       <c r="G160" t="s">
         <v>408</v>
@@ -5673,7 +5691,7 @@
     </row>
     <row r="161" spans="2:7" x14ac:dyDescent="0.2">
       <c r="B161" t="s">
-        <v>365</v>
+        <v>367</v>
       </c>
       <c r="C161" t="s">
         <v>400</v>
@@ -5685,7 +5703,7 @@
         <v>168</v>
       </c>
       <c r="F161" t="s">
-        <v>354</v>
+        <v>241</v>
       </c>
       <c r="G161" t="s">
         <v>408</v>
@@ -5693,7 +5711,7 @@
     </row>
     <row r="162" spans="2:7" x14ac:dyDescent="0.2">
       <c r="B162" t="s">
-        <v>366</v>
+        <v>368</v>
       </c>
       <c r="C162" t="s">
         <v>400</v>
@@ -5705,7 +5723,7 @@
         <v>168</v>
       </c>
       <c r="F162" t="s">
-        <v>355</v>
+        <v>242</v>
       </c>
       <c r="G162" t="s">
         <v>408</v>
@@ -5713,7 +5731,7 @@
     </row>
     <row r="163" spans="2:7" x14ac:dyDescent="0.2">
       <c r="B163" t="s">
-        <v>367</v>
+        <v>369</v>
       </c>
       <c r="C163" t="s">
         <v>400</v>
@@ -5725,7 +5743,7 @@
         <v>168</v>
       </c>
       <c r="F163" t="s">
-        <v>241</v>
+        <v>356</v>
       </c>
       <c r="G163" t="s">
         <v>408</v>
@@ -5733,7 +5751,7 @@
     </row>
     <row r="164" spans="2:7" x14ac:dyDescent="0.2">
       <c r="B164" t="s">
-        <v>368</v>
+        <v>370</v>
       </c>
       <c r="C164" t="s">
         <v>400</v>
@@ -5745,7 +5763,7 @@
         <v>168</v>
       </c>
       <c r="F164" t="s">
-        <v>242</v>
+        <v>243</v>
       </c>
       <c r="G164" t="s">
         <v>408</v>
@@ -5753,7 +5771,7 @@
     </row>
     <row r="165" spans="2:7" x14ac:dyDescent="0.2">
       <c r="B165" t="s">
-        <v>369</v>
+        <v>371</v>
       </c>
       <c r="C165" t="s">
         <v>400</v>
@@ -5765,7 +5783,7 @@
         <v>168</v>
       </c>
       <c r="F165" t="s">
-        <v>356</v>
+        <v>357</v>
       </c>
       <c r="G165" t="s">
         <v>408</v>
@@ -5773,7 +5791,7 @@
     </row>
     <row r="166" spans="2:7" x14ac:dyDescent="0.2">
       <c r="B166" t="s">
-        <v>370</v>
+        <v>372</v>
       </c>
       <c r="C166" t="s">
         <v>400</v>
@@ -5785,78 +5803,38 @@
         <v>168</v>
       </c>
       <c r="F166" t="s">
-        <v>243</v>
+        <v>358</v>
       </c>
       <c r="G166" t="s">
         <v>408</v>
       </c>
     </row>
-    <row r="167" spans="2:7" x14ac:dyDescent="0.2">
-      <c r="B167" t="s">
-        <v>371</v>
-      </c>
-      <c r="C167" t="s">
-        <v>400</v>
-      </c>
-      <c r="D167" t="s">
-        <v>447</v>
-      </c>
-      <c r="E167" t="s">
-        <v>168</v>
-      </c>
-      <c r="F167" t="s">
-        <v>357</v>
-      </c>
-      <c r="G167" t="s">
-        <v>408</v>
-      </c>
-    </row>
-    <row r="168" spans="2:7" x14ac:dyDescent="0.2">
-      <c r="B168" t="s">
-        <v>372</v>
-      </c>
-      <c r="C168" t="s">
-        <v>400</v>
-      </c>
-      <c r="D168" t="s">
-        <v>447</v>
-      </c>
-      <c r="E168" t="s">
-        <v>168</v>
-      </c>
-      <c r="F168" t="s">
-        <v>358</v>
-      </c>
-      <c r="G168" t="s">
-        <v>408</v>
-      </c>
-    </row>
-    <row r="180" spans="1:1" x14ac:dyDescent="0.2">
-      <c r="A180" s="1"/>
-    </row>
-    <row r="186" spans="1:1" x14ac:dyDescent="0.2">
-      <c r="A186" s="1"/>
-    </row>
-    <row r="200" spans="1:1" x14ac:dyDescent="0.2">
-      <c r="A200" s="1"/>
-    </row>
-    <row r="216" spans="1:8" x14ac:dyDescent="0.2">
-      <c r="F216" s="5"/>
-      <c r="H216" s="5"/>
-    </row>
-    <row r="219" spans="1:8" x14ac:dyDescent="0.2">
-      <c r="A219" s="1"/>
-    </row>
-    <row r="229" spans="1:1" x14ac:dyDescent="0.2">
-      <c r="A229" s="1"/>
+    <row r="178" spans="1:1" x14ac:dyDescent="0.2">
+      <c r="A178" s="1"/>
+    </row>
+    <row r="184" spans="1:1" x14ac:dyDescent="0.2">
+      <c r="A184" s="1"/>
+    </row>
+    <row r="198" spans="1:1" x14ac:dyDescent="0.2">
+      <c r="A198" s="1"/>
+    </row>
+    <row r="214" spans="1:8" x14ac:dyDescent="0.2">
+      <c r="F214" s="5"/>
+      <c r="H214" s="5"/>
+    </row>
+    <row r="217" spans="1:8" x14ac:dyDescent="0.2">
+      <c r="A217" s="1"/>
+    </row>
+    <row r="227" spans="1:1" x14ac:dyDescent="0.2">
+      <c r="A227" s="1"/>
     </row>
   </sheetData>
-  <sortState xmlns:xlrd2="http://schemas.microsoft.com/office/spreadsheetml/2017/richdata2" ref="A2:G229">
-    <sortCondition ref="B1:B229"/>
+  <sortState xmlns:xlrd2="http://schemas.microsoft.com/office/spreadsheetml/2017/richdata2" ref="A2:G227">
+    <sortCondition ref="B1:B227"/>
   </sortState>
   <phoneticPr fontId="3" type="noConversion"/>
   <conditionalFormatting sqref="D1:D1048576">
-    <cfRule type="cellIs" dxfId="0" priority="1" operator="equal">
+    <cfRule type="cellIs" dxfId="1" priority="1" operator="equal">
       <formula>"NSC"</formula>
     </cfRule>
   </conditionalFormatting>
@@ -5866,10 +5844,10 @@
 
 <file path=xl/worksheets/sheet2.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{8C91914E-3409-184C-AC43-CBCE957AC7EF}">
-  <dimension ref="A1:H49"/>
+  <dimension ref="A1:H55"/>
   <sheetViews>
     <sheetView workbookViewId="0">
-      <selection activeCell="D14" sqref="D14"/>
+      <selection activeCell="E22" sqref="E22"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="16" x14ac:dyDescent="0.2"/>
@@ -6229,33 +6207,21 @@
     </row>
     <row r="20" spans="1:7" x14ac:dyDescent="0.2">
       <c r="A20" s="1"/>
-      <c r="B20" t="s">
-        <v>451</v>
+      <c r="B20" s="7" t="s">
+        <v>458</v>
+      </c>
+    </row>
+    <row r="21" spans="1:7" x14ac:dyDescent="0.2">
+      <c r="B21" s="7" t="s">
+        <v>457</v>
       </c>
     </row>
     <row r="22" spans="1:7" x14ac:dyDescent="0.2">
-      <c r="B22" t="s">
-        <v>289</v>
-      </c>
-      <c r="C22" t="s">
-        <v>413</v>
-      </c>
-      <c r="D22" t="s">
-        <v>102</v>
-      </c>
-      <c r="E22" t="s">
-        <v>169</v>
-      </c>
-      <c r="F22" t="s">
-        <v>272</v>
-      </c>
-      <c r="G22" t="s">
-        <v>392</v>
-      </c>
+      <c r="B22" s="6"/>
     </row>
     <row r="23" spans="1:7" x14ac:dyDescent="0.2">
       <c r="B23" t="s">
-        <v>290</v>
+        <v>289</v>
       </c>
       <c r="C23" t="s">
         <v>413</v>
@@ -6267,7 +6233,7 @@
         <v>169</v>
       </c>
       <c r="F23" t="s">
-        <v>273</v>
+        <v>272</v>
       </c>
       <c r="G23" t="s">
         <v>392</v>
@@ -6275,7 +6241,7 @@
     </row>
     <row r="24" spans="1:7" x14ac:dyDescent="0.2">
       <c r="B24" t="s">
-        <v>291</v>
+        <v>290</v>
       </c>
       <c r="C24" t="s">
         <v>413</v>
@@ -6287,7 +6253,7 @@
         <v>169</v>
       </c>
       <c r="F24" t="s">
-        <v>274</v>
+        <v>273</v>
       </c>
       <c r="G24" t="s">
         <v>392</v>
@@ -6295,7 +6261,7 @@
     </row>
     <row r="25" spans="1:7" x14ac:dyDescent="0.2">
       <c r="B25" t="s">
-        <v>292</v>
+        <v>291</v>
       </c>
       <c r="C25" t="s">
         <v>413</v>
@@ -6307,7 +6273,7 @@
         <v>169</v>
       </c>
       <c r="F25" t="s">
-        <v>275</v>
+        <v>274</v>
       </c>
       <c r="G25" t="s">
         <v>392</v>
@@ -6315,7 +6281,7 @@
     </row>
     <row r="26" spans="1:7" x14ac:dyDescent="0.2">
       <c r="B26" t="s">
-        <v>293</v>
+        <v>292</v>
       </c>
       <c r="C26" t="s">
         <v>413</v>
@@ -6327,7 +6293,7 @@
         <v>169</v>
       </c>
       <c r="F26" t="s">
-        <v>276</v>
+        <v>275</v>
       </c>
       <c r="G26" t="s">
         <v>392</v>
@@ -6335,7 +6301,7 @@
     </row>
     <row r="27" spans="1:7" x14ac:dyDescent="0.2">
       <c r="B27" t="s">
-        <v>294</v>
+        <v>293</v>
       </c>
       <c r="C27" t="s">
         <v>413</v>
@@ -6347,7 +6313,7 @@
         <v>169</v>
       </c>
       <c r="F27" t="s">
-        <v>277</v>
+        <v>276</v>
       </c>
       <c r="G27" t="s">
         <v>392</v>
@@ -6355,7 +6321,7 @@
     </row>
     <row r="28" spans="1:7" x14ac:dyDescent="0.2">
       <c r="B28" t="s">
-        <v>295</v>
+        <v>294</v>
       </c>
       <c r="C28" t="s">
         <v>413</v>
@@ -6367,7 +6333,7 @@
         <v>169</v>
       </c>
       <c r="F28" t="s">
-        <v>278</v>
+        <v>277</v>
       </c>
       <c r="G28" t="s">
         <v>392</v>
@@ -6375,7 +6341,7 @@
     </row>
     <row r="29" spans="1:7" x14ac:dyDescent="0.2">
       <c r="B29" t="s">
-        <v>296</v>
+        <v>295</v>
       </c>
       <c r="C29" t="s">
         <v>413</v>
@@ -6387,7 +6353,7 @@
         <v>169</v>
       </c>
       <c r="F29" t="s">
-        <v>279</v>
+        <v>278</v>
       </c>
       <c r="G29" t="s">
         <v>392</v>
@@ -6395,7 +6361,7 @@
     </row>
     <row r="30" spans="1:7" x14ac:dyDescent="0.2">
       <c r="B30" t="s">
-        <v>297</v>
+        <v>296</v>
       </c>
       <c r="C30" t="s">
         <v>413</v>
@@ -6407,7 +6373,7 @@
         <v>169</v>
       </c>
       <c r="F30" t="s">
-        <v>280</v>
+        <v>279</v>
       </c>
       <c r="G30" t="s">
         <v>392</v>
@@ -6415,7 +6381,7 @@
     </row>
     <row r="31" spans="1:7" x14ac:dyDescent="0.2">
       <c r="B31" t="s">
-        <v>298</v>
+        <v>297</v>
       </c>
       <c r="C31" t="s">
         <v>413</v>
@@ -6427,7 +6393,7 @@
         <v>169</v>
       </c>
       <c r="F31" t="s">
-        <v>281</v>
+        <v>280</v>
       </c>
       <c r="G31" t="s">
         <v>392</v>
@@ -6435,7 +6401,7 @@
     </row>
     <row r="32" spans="1:7" x14ac:dyDescent="0.2">
       <c r="B32" t="s">
-        <v>299</v>
+        <v>298</v>
       </c>
       <c r="C32" t="s">
         <v>413</v>
@@ -6447,7 +6413,7 @@
         <v>169</v>
       </c>
       <c r="F32" t="s">
-        <v>282</v>
+        <v>281</v>
       </c>
       <c r="G32" t="s">
         <v>392</v>
@@ -6455,7 +6421,7 @@
     </row>
     <row r="33" spans="1:8" x14ac:dyDescent="0.2">
       <c r="B33" t="s">
-        <v>300</v>
+        <v>299</v>
       </c>
       <c r="C33" t="s">
         <v>413</v>
@@ -6467,7 +6433,7 @@
         <v>169</v>
       </c>
       <c r="F33" t="s">
-        <v>283</v>
+        <v>282</v>
       </c>
       <c r="G33" t="s">
         <v>392</v>
@@ -6475,7 +6441,7 @@
     </row>
     <row r="34" spans="1:8" x14ac:dyDescent="0.2">
       <c r="B34" t="s">
-        <v>301</v>
+        <v>300</v>
       </c>
       <c r="C34" t="s">
         <v>413</v>
@@ -6487,7 +6453,7 @@
         <v>169</v>
       </c>
       <c r="F34" t="s">
-        <v>284</v>
+        <v>283</v>
       </c>
       <c r="G34" t="s">
         <v>392</v>
@@ -6495,7 +6461,7 @@
     </row>
     <row r="35" spans="1:8" x14ac:dyDescent="0.2">
       <c r="B35" t="s">
-        <v>302</v>
+        <v>301</v>
       </c>
       <c r="C35" t="s">
         <v>413</v>
@@ -6507,7 +6473,7 @@
         <v>169</v>
       </c>
       <c r="F35" t="s">
-        <v>285</v>
+        <v>284</v>
       </c>
       <c r="G35" t="s">
         <v>392</v>
@@ -6515,7 +6481,7 @@
     </row>
     <row r="36" spans="1:8" x14ac:dyDescent="0.2">
       <c r="B36" t="s">
-        <v>303</v>
+        <v>302</v>
       </c>
       <c r="C36" t="s">
         <v>413</v>
@@ -6526,17 +6492,16 @@
       <c r="E36" t="s">
         <v>169</v>
       </c>
-      <c r="F36" s="5" t="s">
-        <v>286</v>
+      <c r="F36" t="s">
+        <v>285</v>
       </c>
       <c r="G36" t="s">
         <v>392</v>
       </c>
-      <c r="H36" s="5"/>
     </row>
     <row r="37" spans="1:8" x14ac:dyDescent="0.2">
       <c r="B37" t="s">
-        <v>304</v>
+        <v>303</v>
       </c>
       <c r="C37" t="s">
         <v>413</v>
@@ -6547,16 +6512,17 @@
       <c r="E37" t="s">
         <v>169</v>
       </c>
-      <c r="F37" t="s">
-        <v>287</v>
+      <c r="F37" s="5" t="s">
+        <v>286</v>
       </c>
       <c r="G37" t="s">
         <v>392</v>
       </c>
+      <c r="H37" s="5"/>
     </row>
     <row r="38" spans="1:8" x14ac:dyDescent="0.2">
       <c r="B38" t="s">
-        <v>305</v>
+        <v>304</v>
       </c>
       <c r="C38" t="s">
         <v>413</v>
@@ -6568,41 +6534,41 @@
         <v>169</v>
       </c>
       <c r="F38" t="s">
-        <v>288</v>
+        <v>287</v>
       </c>
       <c r="G38" t="s">
         <v>392</v>
       </c>
     </row>
     <row r="39" spans="1:8" x14ac:dyDescent="0.2">
-      <c r="A39" s="1"/>
       <c r="B39" t="s">
-        <v>452</v>
-      </c>
-    </row>
-    <row r="41" spans="1:8" x14ac:dyDescent="0.2">
-      <c r="B41" t="s">
-        <v>337</v>
-      </c>
-      <c r="C41" t="s">
-        <v>405</v>
-      </c>
-      <c r="D41" t="s">
-        <v>102</v>
-      </c>
-      <c r="E41" t="s">
-        <v>168</v>
-      </c>
-      <c r="F41" t="s">
-        <v>454</v>
-      </c>
-      <c r="G41" t="s">
-        <v>404</v>
+        <v>305</v>
+      </c>
+      <c r="C39" t="s">
+        <v>413</v>
+      </c>
+      <c r="D39" t="s">
+        <v>102</v>
+      </c>
+      <c r="E39" t="s">
+        <v>169</v>
+      </c>
+      <c r="F39" t="s">
+        <v>288</v>
+      </c>
+      <c r="G39" t="s">
+        <v>392</v>
+      </c>
+    </row>
+    <row r="40" spans="1:8" x14ac:dyDescent="0.2">
+      <c r="A40" s="1"/>
+      <c r="B40" t="s">
+        <v>451</v>
       </c>
     </row>
     <row r="42" spans="1:8" x14ac:dyDescent="0.2">
       <c r="B42" t="s">
-        <v>338</v>
+        <v>337</v>
       </c>
       <c r="C42" t="s">
         <v>405</v>
@@ -6614,7 +6580,7 @@
         <v>168</v>
       </c>
       <c r="F42" t="s">
-        <v>454</v>
+        <v>453</v>
       </c>
       <c r="G42" t="s">
         <v>404</v>
@@ -6622,7 +6588,7 @@
     </row>
     <row r="43" spans="1:8" x14ac:dyDescent="0.2">
       <c r="B43" t="s">
-        <v>339</v>
+        <v>338</v>
       </c>
       <c r="C43" t="s">
         <v>405</v>
@@ -6634,7 +6600,7 @@
         <v>168</v>
       </c>
       <c r="F43" t="s">
-        <v>454</v>
+        <v>453</v>
       </c>
       <c r="G43" t="s">
         <v>404</v>
@@ -6642,7 +6608,7 @@
     </row>
     <row r="44" spans="1:8" x14ac:dyDescent="0.2">
       <c r="B44" t="s">
-        <v>340</v>
+        <v>339</v>
       </c>
       <c r="C44" t="s">
         <v>405</v>
@@ -6654,7 +6620,7 @@
         <v>168</v>
       </c>
       <c r="F44" t="s">
-        <v>454</v>
+        <v>453</v>
       </c>
       <c r="G44" t="s">
         <v>404</v>
@@ -6662,7 +6628,7 @@
     </row>
     <row r="45" spans="1:8" x14ac:dyDescent="0.2">
       <c r="B45" t="s">
-        <v>341</v>
+        <v>340</v>
       </c>
       <c r="C45" t="s">
         <v>405</v>
@@ -6674,7 +6640,7 @@
         <v>168</v>
       </c>
       <c r="F45" t="s">
-        <v>455</v>
+        <v>453</v>
       </c>
       <c r="G45" t="s">
         <v>404</v>
@@ -6682,7 +6648,7 @@
     </row>
     <row r="46" spans="1:8" x14ac:dyDescent="0.2">
       <c r="B46" t="s">
-        <v>342</v>
+        <v>341</v>
       </c>
       <c r="C46" t="s">
         <v>405</v>
@@ -6694,7 +6660,7 @@
         <v>168</v>
       </c>
       <c r="F46" t="s">
-        <v>455</v>
+        <v>454</v>
       </c>
       <c r="G46" t="s">
         <v>404</v>
@@ -6702,7 +6668,7 @@
     </row>
     <row r="47" spans="1:8" x14ac:dyDescent="0.2">
       <c r="B47" t="s">
-        <v>343</v>
+        <v>342</v>
       </c>
       <c r="C47" t="s">
         <v>405</v>
@@ -6714,7 +6680,7 @@
         <v>168</v>
       </c>
       <c r="F47" t="s">
-        <v>455</v>
+        <v>454</v>
       </c>
       <c r="G47" t="s">
         <v>404</v>
@@ -6722,7 +6688,7 @@
     </row>
     <row r="48" spans="1:8" x14ac:dyDescent="0.2">
       <c r="B48" t="s">
-        <v>344</v>
+        <v>343</v>
       </c>
       <c r="C48" t="s">
         <v>405</v>
@@ -6734,19 +6700,102 @@
         <v>168</v>
       </c>
       <c r="F48" t="s">
-        <v>455</v>
+        <v>454</v>
       </c>
       <c r="G48" t="s">
         <v>404</v>
       </c>
     </row>
-    <row r="49" spans="1:2" x14ac:dyDescent="0.2">
-      <c r="A49" s="1"/>
+    <row r="49" spans="1:7" x14ac:dyDescent="0.2">
       <c r="B49" t="s">
-        <v>453</v>
+        <v>344</v>
+      </c>
+      <c r="C49" t="s">
+        <v>405</v>
+      </c>
+      <c r="D49" t="s">
+        <v>102</v>
+      </c>
+      <c r="E49" t="s">
+        <v>168</v>
+      </c>
+      <c r="F49" t="s">
+        <v>454</v>
+      </c>
+      <c r="G49" t="s">
+        <v>404</v>
+      </c>
+    </row>
+    <row r="50" spans="1:7" x14ac:dyDescent="0.2">
+      <c r="A50" s="1"/>
+      <c r="B50" t="s">
+        <v>452</v>
+      </c>
+    </row>
+    <row r="52" spans="1:7" x14ac:dyDescent="0.2">
+      <c r="A52" t="s">
+        <v>55</v>
+      </c>
+      <c r="B52" s="3" t="s">
+        <v>156</v>
+      </c>
+      <c r="C52" s="4" t="s">
+        <v>195</v>
+      </c>
+      <c r="D52" t="s">
+        <v>102</v>
+      </c>
+      <c r="E52" t="s">
+        <v>168</v>
+      </c>
+      <c r="F52" t="s">
+        <v>166</v>
+      </c>
+      <c r="G52" s="6" t="s">
+        <v>99</v>
+      </c>
+    </row>
+    <row r="53" spans="1:7" x14ac:dyDescent="0.2">
+      <c r="B53" s="3" t="s">
+        <v>455</v>
+      </c>
+      <c r="C53" s="4"/>
+      <c r="G53" s="6"/>
+    </row>
+    <row r="54" spans="1:7" x14ac:dyDescent="0.2">
+      <c r="A54" t="s">
+        <v>56</v>
+      </c>
+      <c r="B54" s="3" t="s">
+        <v>157</v>
+      </c>
+      <c r="C54" s="4" t="s">
+        <v>195</v>
+      </c>
+      <c r="D54" t="s">
+        <v>102</v>
+      </c>
+      <c r="E54" t="s">
+        <v>168</v>
+      </c>
+      <c r="F54" t="s">
+        <v>166</v>
+      </c>
+      <c r="G54" s="6" t="s">
+        <v>99</v>
+      </c>
+    </row>
+    <row r="55" spans="1:7" x14ac:dyDescent="0.2">
+      <c r="B55" s="3" t="s">
+        <v>456</v>
       </c>
     </row>
   </sheetData>
+  <conditionalFormatting sqref="D52:D54">
+    <cfRule type="cellIs" dxfId="0" priority="1" operator="equal">
+      <formula>"NSC"</formula>
+    </cfRule>
+  </conditionalFormatting>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
 </worksheet>
 </file>
</xml_diff>

<commit_message>
update to ref, added unfinished new data folder
jorja has a process for new data folder - do not disturb
</commit_message>
<xml_diff>
--- a/data/ref.xlsx
+++ b/data/ref.xlsx
@@ -8,9 +8,9 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="/Users/jorjaelliott/Desktop/Repositories/LCAdata/data/"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{66059E71-7F6D-0648-9D5B-5328DCC678B9}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{54649D89-38D1-1F4B-BC0D-7386A155EDF8}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="39180" yWindow="1180" windowWidth="17120" windowHeight="15880" activeTab="1" xr2:uid="{4F28B243-04AE-1E4D-B411-E86C9FDA2FDF}"/>
+    <workbookView xWindow="39260" yWindow="500" windowWidth="26660" windowHeight="17620" activeTab="1" xr2:uid="{4F28B243-04AE-1E4D-B411-E86C9FDA2FDF}"/>
   </bookViews>
   <sheets>
     <sheet name="data" sheetId="1" r:id="rId1"/>
@@ -37,7 +37,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="3233" uniqueCount="737">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="4344" uniqueCount="920">
   <si>
     <t>old file name</t>
   </si>
@@ -3620,15 +3620,9 @@
     <t>rye (Secale cereale L..)</t>
   </si>
   <si>
-    <t>wheat</t>
-  </si>
-  <si>
     <t>rice (Oryza sativa L.)</t>
   </si>
   <si>
-    <t>beans (Phaseolus vulgaris L.)</t>
-  </si>
-  <si>
     <t>spanish clover</t>
   </si>
   <si>
@@ -3638,17 +3632,754 @@
     <t>Drosophila hibisci</t>
   </si>
   <si>
-    <t>poltry</t>
-  </si>
-  <si>
-    <t>Astyanax</t>
+    <t>space.internode.len.csv</t>
+  </si>
+  <si>
+    <t>space.lateral.num.csv</t>
+  </si>
+  <si>
+    <t>space.node.num.csv</t>
+  </si>
+  <si>
+    <t>space.stem.len.csv</t>
+  </si>
+  <si>
+    <t>space.fruit.num.csv</t>
+  </si>
+  <si>
+    <t>NCSU.node.num.csv</t>
+  </si>
+  <si>
+    <t>NCSU.lateral.num.csv</t>
+  </si>
+  <si>
+    <t>NCSU.internode.len.csv</t>
+  </si>
+  <si>
+    <t>NCSU.stem.len.csv</t>
+  </si>
+  <si>
+    <t>NCSU.fruit.num.csv</t>
+  </si>
+  <si>
+    <t>number of nodes</t>
+  </si>
+  <si>
+    <t>average internode length (cm)</t>
+  </si>
+  <si>
+    <t>number of primary laterals</t>
+  </si>
+  <si>
+    <t>main stem length (cm)</t>
+  </si>
+  <si>
+    <t>number of fruits per plant</t>
+  </si>
+  <si>
+    <t>bodyweight69.csv</t>
+  </si>
+  <si>
+    <t>bodyweight71.csv</t>
+  </si>
+  <si>
+    <t>eggbody69.csv</t>
+  </si>
+  <si>
+    <t>eggbody71.csv</t>
+  </si>
+  <si>
+    <t>eggnum69.csv</t>
+  </si>
+  <si>
+    <t>eggnum71.csv</t>
+  </si>
+  <si>
+    <t>eggsize69.csv</t>
+  </si>
+  <si>
+    <t>eggsize71.csv</t>
+  </si>
+  <si>
+    <t>eggvol69.csv</t>
+  </si>
+  <si>
+    <t>eggvol71.csv</t>
+  </si>
+  <si>
+    <t>body weight</t>
+  </si>
+  <si>
+    <t>number of eggs per unit body weight</t>
+  </si>
+  <si>
+    <t>egg number</t>
+  </si>
+  <si>
+    <t>egg size</t>
+  </si>
+  <si>
+    <t xml:space="preserve">egg volume </t>
+  </si>
+  <si>
+    <t>fruitplot1.csv</t>
+  </si>
+  <si>
+    <t>fruitplot2.csv</t>
+  </si>
+  <si>
+    <t>fruitplot3.csv</t>
+  </si>
+  <si>
+    <t>fruitplot4.csv</t>
+  </si>
+  <si>
+    <t>fruitplot5.csv</t>
+  </si>
+  <si>
+    <t>fruitplot6.csv</t>
+  </si>
+  <si>
+    <t>fruitnum1.csv</t>
+  </si>
+  <si>
+    <t>fruitnum2.csv</t>
+  </si>
+  <si>
+    <t>fruitnum3.csv</t>
+  </si>
+  <si>
+    <t>fruitnum4.csv</t>
+  </si>
+  <si>
+    <t>fruitnum5.csv</t>
+  </si>
+  <si>
+    <t>fruitnum6.csv</t>
+  </si>
+  <si>
+    <t>fruitwt1.csv</t>
+  </si>
+  <si>
+    <t>fruitwt2.csv</t>
+  </si>
+  <si>
+    <t>fruitwt3.csv</t>
+  </si>
+  <si>
+    <t>fruitwt4.csv</t>
+  </si>
+  <si>
+    <t>fruitwt5.csv</t>
+  </si>
+  <si>
+    <t>fruitwt6.csv</t>
+  </si>
+  <si>
+    <t>fruitindex1.csv</t>
+  </si>
+  <si>
+    <t>fruitindex2.csv</t>
+  </si>
+  <si>
+    <t>fruitindex3.csv</t>
+  </si>
+  <si>
+    <t>fruitindex4.csv</t>
+  </si>
+  <si>
+    <t>fruitindex5.csv</t>
+  </si>
+  <si>
+    <t>fruitindex6.csv</t>
+  </si>
+  <si>
+    <t>fruit weight per plot (kg)</t>
+  </si>
+  <si>
+    <t>fruit number per plot</t>
+  </si>
+  <si>
+    <t>average fruit weight (g)</t>
+  </si>
+  <si>
+    <t>fruit bearing index</t>
+  </si>
+  <si>
+    <r>
+      <t xml:space="preserve">Al-Falluji, R.A., Trinklein, D.H., Lambeth, V.N. (1982) Inheritance of pericarp firmness in tomato by generation mean analysis. </t>
+    </r>
+    <r>
+      <rPr>
+        <i/>
+        <sz val="12"/>
+        <color theme="1"/>
+        <rFont val="Calibri"/>
+        <family val="2"/>
+        <scheme val="minor"/>
+      </rPr>
+      <t>HortScience</t>
+    </r>
+    <r>
+      <rPr>
+        <sz val="12"/>
+        <color theme="1"/>
+        <rFont val="Calibri"/>
+        <family val="2"/>
+        <scheme val="minor"/>
+      </rPr>
+      <t>. 17(5), 763-764.</t>
+    </r>
+  </si>
+  <si>
+    <t>pericarp firmness</t>
+  </si>
+  <si>
+    <r>
+      <t>tomato (</t>
+    </r>
+    <r>
+      <rPr>
+        <i/>
+        <sz val="12"/>
+        <color theme="1"/>
+        <rFont val="Calibri"/>
+        <family val="2"/>
+        <scheme val="minor"/>
+      </rPr>
+      <t xml:space="preserve">Lycopersicon esculentum </t>
+    </r>
+    <r>
+      <rPr>
+        <sz val="12"/>
+        <color theme="1"/>
+        <rFont val="Calibri"/>
+        <family val="2"/>
+        <scheme val="minor"/>
+      </rPr>
+      <t>Mill.)</t>
+    </r>
+  </si>
+  <si>
+    <t>pericarp.firm.csv</t>
+  </si>
+  <si>
+    <t>bodyweight60.fem.csv</t>
+  </si>
+  <si>
+    <t>bodyweight60.male.csv</t>
+  </si>
+  <si>
+    <t>60 day bodyweight in females</t>
+  </si>
+  <si>
+    <t>60 day bodyweight in males</t>
+  </si>
+  <si>
+    <t>parental sex unknown</t>
+  </si>
+  <si>
+    <t>peri.677a.b37.csv</t>
+  </si>
+  <si>
+    <t>peri.677a.b68.csv</t>
+  </si>
+  <si>
+    <t>peri.677a.h55.csv</t>
+  </si>
+  <si>
+    <t>peri.677a.hi26.csv</t>
+  </si>
+  <si>
+    <t>peri.AA8.b37.csv</t>
+  </si>
+  <si>
+    <t>peri.AA8.b68.csv</t>
+  </si>
+  <si>
+    <t>peri.AA8.h55.csv</t>
+  </si>
+  <si>
+    <t>peri.AA8.hi26.csv</t>
+  </si>
+  <si>
+    <t>Zea mays</t>
+  </si>
+  <si>
+    <t>coleolen1.csv</t>
+  </si>
+  <si>
+    <t>coleolen2.csv</t>
+  </si>
+  <si>
+    <t>coleolen3.csv</t>
+  </si>
+  <si>
+    <t>coleolen4.csv</t>
+  </si>
+  <si>
+    <t>coleolen5.csv</t>
+  </si>
+  <si>
+    <t>seedht1.csv</t>
+  </si>
+  <si>
+    <t>seedht2.csv</t>
+  </si>
+  <si>
+    <t>seedht3.csv</t>
+  </si>
+  <si>
+    <t>seedht4.csv</t>
+  </si>
+  <si>
+    <t>seedht5.csv</t>
+  </si>
+  <si>
+    <t>plantht1.csv</t>
+  </si>
+  <si>
+    <t>plantht2.csv</t>
+  </si>
+  <si>
+    <t>plantht3.csv</t>
+  </si>
+  <si>
+    <t>plantht4.csv</t>
+  </si>
+  <si>
+    <t>plantht5.csv</t>
+  </si>
+  <si>
+    <t>spikelen1.csv</t>
+  </si>
+  <si>
+    <t>spikelen2.csv</t>
+  </si>
+  <si>
+    <t>spikelen3.csv</t>
+  </si>
+  <si>
+    <t>spikelen4.csv</t>
+  </si>
+  <si>
+    <t>spikelen5.csv</t>
+  </si>
+  <si>
+    <t>yieldspike1.csv</t>
+  </si>
+  <si>
+    <t>yieldspike2.csv</t>
+  </si>
+  <si>
+    <t>yieldspike3.csv</t>
+  </si>
+  <si>
+    <t>yieldspike4.csv</t>
+  </si>
+  <si>
+    <t>yieldspike5.csv</t>
+  </si>
+  <si>
+    <t>coleoptile length (mm)</t>
+  </si>
+  <si>
+    <t>seedling height (mm)</t>
+  </si>
+  <si>
+    <t>plant height (cm)</t>
+  </si>
+  <si>
+    <t>spike length (cm)</t>
+  </si>
+  <si>
+    <t>yield per spike (g)</t>
+  </si>
+  <si>
+    <t>spike.culms1.csv</t>
+  </si>
+  <si>
+    <t>spike.culms2.csv</t>
+  </si>
+  <si>
+    <r>
+      <t xml:space="preserve">Merrit, R.G. (1988) Inheritance of culm number in two uniculm x multiculm wheat crosses. </t>
+    </r>
+    <r>
+      <rPr>
+        <i/>
+        <sz val="12"/>
+        <color theme="1"/>
+        <rFont val="Calibri"/>
+        <family val="2"/>
+        <scheme val="minor"/>
+      </rPr>
+      <t>Euphytica</t>
+    </r>
+    <r>
+      <rPr>
+        <sz val="12"/>
+        <color theme="1"/>
+        <rFont val="Calibri"/>
+        <family val="2"/>
+        <scheme val="minor"/>
+      </rPr>
+      <t>. 38, 105-112</t>
+    </r>
+    <r>
+      <rPr>
+        <sz val="12"/>
+        <color theme="1"/>
+        <rFont val="Calibri"/>
+        <family val="2"/>
+        <scheme val="minor"/>
+      </rPr>
+      <t/>
+    </r>
+  </si>
+  <si>
+    <r>
+      <t>wheat (</t>
+    </r>
+    <r>
+      <rPr>
+        <i/>
+        <sz val="12"/>
+        <color theme="1"/>
+        <rFont val="Calibri"/>
+        <family val="2"/>
+        <scheme val="minor"/>
+      </rPr>
+      <t xml:space="preserve">Triticum aestivum </t>
+    </r>
+    <r>
+      <rPr>
+        <sz val="12"/>
+        <color theme="1"/>
+        <rFont val="Calibri"/>
+        <family val="2"/>
+        <scheme val="minor"/>
+      </rPr>
+      <t>L.)</t>
+    </r>
+  </si>
+  <si>
+    <t>number of spike bearing culms</t>
+  </si>
+  <si>
+    <t>mesolen1/csv</t>
+  </si>
+  <si>
+    <t>mesolen2.csv</t>
+  </si>
+  <si>
+    <t>mesolen3.csv</t>
+  </si>
+  <si>
+    <t>mesocotyl length</t>
+  </si>
+  <si>
+    <t>seed.length.csv</t>
+  </si>
+  <si>
+    <t>seed.width.csv</t>
+  </si>
+  <si>
+    <t>seed.height.csv</t>
+  </si>
+  <si>
+    <t>seed.weight.csv</t>
+  </si>
+  <si>
+    <r>
+      <t>beans (</t>
+    </r>
+    <r>
+      <rPr>
+        <i/>
+        <sz val="12"/>
+        <color theme="1"/>
+        <rFont val="Calibri"/>
+        <family val="2"/>
+        <scheme val="minor"/>
+      </rPr>
+      <t>Phaseolus vulgaris</t>
+    </r>
+    <r>
+      <rPr>
+        <sz val="12"/>
+        <color theme="1"/>
+        <rFont val="Calibri"/>
+        <family val="2"/>
+        <scheme val="minor"/>
+      </rPr>
+      <t xml:space="preserve"> L.)</t>
+    </r>
+  </si>
+  <si>
+    <t>seed length (mm)</t>
+  </si>
+  <si>
+    <t>seed width (mm)</t>
+  </si>
+  <si>
+    <t>seed height (mm)</t>
+  </si>
+  <si>
+    <t>seed weight (mg)</t>
+  </si>
+  <si>
+    <t>cot.area.csv</t>
+  </si>
+  <si>
+    <t>juv.leafwd.csv</t>
+  </si>
+  <si>
+    <t>acetyl.red.csv</t>
+  </si>
+  <si>
+    <t>shootwt.fresh.csv</t>
+  </si>
+  <si>
+    <t>rootwt.csv</t>
+  </si>
+  <si>
+    <t>shootwt.dry.csv</t>
+  </si>
+  <si>
+    <t>nitrogenfix.csv</t>
+  </si>
+  <si>
+    <t>cotyledon area (mm2)</t>
+  </si>
+  <si>
+    <t>juvenile leaf width (mm)</t>
+  </si>
+  <si>
+    <t>acetylene reduced (nmoles/h)</t>
+  </si>
+  <si>
+    <t>shoot fresh weight (mg)</t>
+  </si>
+  <si>
+    <t>root fresh weight (g)</t>
+  </si>
+  <si>
+    <t>shoot dry weight (mg)</t>
+  </si>
+  <si>
+    <t>nitrogen fixation component</t>
+  </si>
+  <si>
+    <t>yield.normal.csv</t>
+  </si>
+  <si>
+    <t>yield.late.csv</t>
+  </si>
+  <si>
+    <t>grain yield (g/plant) for normal sowing</t>
+  </si>
+  <si>
+    <t>grain yield (g/plant) for late sowing</t>
+  </si>
+  <si>
+    <t>seed.sylvia.csv</t>
+  </si>
+  <si>
+    <t>seed.mf.csv</t>
+  </si>
+  <si>
+    <t>seed number per pod, sylviaxsp16</t>
+  </si>
+  <si>
+    <t>seed number per pod, 6207xmf</t>
+  </si>
+  <si>
+    <t>cmat.starmer.csv</t>
+  </si>
+  <si>
+    <t>thorax.len25.csv</t>
+  </si>
+  <si>
+    <t>ova25.csv</t>
+  </si>
+  <si>
+    <t>thorax.len21.csv</t>
+  </si>
+  <si>
+    <t>thorax.len18.csv</t>
+  </si>
+  <si>
+    <t>ova21.csv</t>
+  </si>
+  <si>
+    <t>ova18.csv</t>
+  </si>
+  <si>
+    <t>thorax length</t>
+  </si>
+  <si>
+    <t>ovariole number</t>
+  </si>
+  <si>
+    <t>shell.color.csv</t>
+  </si>
+  <si>
+    <t>chickens</t>
+  </si>
+  <si>
+    <t>eggshell color</t>
+  </si>
+  <si>
+    <t>ZW</t>
+  </si>
+  <si>
+    <t>eyesize.csv</t>
+  </si>
+  <si>
+    <t>eye-ball size</t>
+  </si>
+  <si>
+    <r>
+      <rPr>
+        <sz val="12"/>
+        <color theme="1"/>
+        <rFont val="Calibri"/>
+        <family val="2"/>
+        <scheme val="minor"/>
+      </rPr>
+      <t xml:space="preserve">cavefish </t>
+    </r>
+    <r>
+      <rPr>
+        <i/>
+        <sz val="12"/>
+        <color theme="1"/>
+        <rFont val="Calibri"/>
+        <family val="2"/>
+        <scheme val="minor"/>
+      </rPr>
+      <t>(Astyanax)</t>
+    </r>
+  </si>
+  <si>
+    <t>baghat-1984</t>
+  </si>
+  <si>
+    <t>stevens-1976</t>
+  </si>
+  <si>
+    <t>plant.height1.csv</t>
+  </si>
+  <si>
+    <t>plant.height2.csv</t>
+  </si>
+  <si>
+    <t>plant.height3.csv</t>
+  </si>
+  <si>
+    <t>plant.height4.csv</t>
+  </si>
+  <si>
+    <t>internode.num1.csv</t>
+  </si>
+  <si>
+    <t>internode.num2.csv</t>
+  </si>
+  <si>
+    <t>internode.num3.csv</t>
+  </si>
+  <si>
+    <t>internode.num4.csv</t>
+  </si>
+  <si>
+    <t>stemwt2.csv</t>
+  </si>
+  <si>
+    <t>stemwt1.csv</t>
+  </si>
+  <si>
+    <t>stemwt3.csv</t>
+  </si>
+  <si>
+    <t>stemwt4.csv</t>
+  </si>
+  <si>
+    <t>leafwt1.csv</t>
+  </si>
+  <si>
+    <t>leafwt2.csv</t>
+  </si>
+  <si>
+    <t>leafwt3.csv</t>
+  </si>
+  <si>
+    <t>leafwt4.csv</t>
+  </si>
+  <si>
+    <r>
+      <rPr>
+        <sz val="12"/>
+        <color theme="1"/>
+        <rFont val="Calibri"/>
+        <family val="2"/>
+        <scheme val="minor"/>
+      </rPr>
+      <t>Jimsonweed (</t>
+    </r>
+    <r>
+      <rPr>
+        <i/>
+        <sz val="12"/>
+        <color theme="1"/>
+        <rFont val="Calibri"/>
+        <family val="2"/>
+        <scheme val="minor"/>
+      </rPr>
+      <t xml:space="preserve">Datura stramonium </t>
+    </r>
+    <r>
+      <rPr>
+        <sz val="12"/>
+        <color theme="1"/>
+        <rFont val="Calibri"/>
+        <family val="2"/>
+        <scheme val="minor"/>
+      </rPr>
+      <t>L.)</t>
+    </r>
+  </si>
+  <si>
+    <t>internode number</t>
+  </si>
+  <si>
+    <t>stem weight (g)</t>
+  </si>
+  <si>
+    <t>leaf weight (g)</t>
+  </si>
+  <si>
+    <t>viscosity.csv</t>
+  </si>
+  <si>
+    <t>tomato (Lycopersicon esculentum)</t>
+  </si>
+  <si>
+    <t>gross viscosity</t>
   </si>
 </sst>
 </file>
 
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
 <styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:x16r2="http://schemas.microsoft.com/office/spreadsheetml/2015/02/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" mc:Ignorable="x14ac x16r2 xr">
-  <fonts count="7" x14ac:knownFonts="1">
+  <fonts count="8" x14ac:knownFonts="1">
+    <font>
+      <sz val="12"/>
+      <color theme="1"/>
+      <name val="Calibri"/>
+      <family val="2"/>
+      <scheme val="minor"/>
+    </font>
     <font>
       <sz val="12"/>
       <color theme="1"/>
@@ -3731,17 +4462,18 @@
   <cellStyleXfs count="1">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
   </cellStyleXfs>
-  <cellXfs count="10">
+  <cellXfs count="11">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
-    <xf numFmtId="0" fontId="1" fillId="0" borderId="0" xfId="0" applyFont="1"/>
     <xf numFmtId="0" fontId="2" fillId="0" borderId="0" xfId="0" applyFont="1"/>
-    <xf numFmtId="0" fontId="4" fillId="0" borderId="0" xfId="0" applyFont="1"/>
+    <xf numFmtId="0" fontId="3" fillId="0" borderId="0" xfId="0" applyFont="1"/>
     <xf numFmtId="0" fontId="5" fillId="0" borderId="0" xfId="0" applyFont="1"/>
+    <xf numFmtId="0" fontId="6" fillId="0" borderId="0" xfId="0" applyFont="1"/>
     <xf numFmtId="16" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1"/>
     <xf numFmtId="0" fontId="0" fillId="2" borderId="0" xfId="0" applyFill="1"/>
     <xf numFmtId="0" fontId="0" fillId="3" borderId="0" xfId="0" applyFill="1"/>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyFill="1"/>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyFont="1"/>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" quotePrefix="1"/>
   </cellXfs>
   <cellStyles count="1">
     <cellStyle name="Normal" xfId="0" builtinId="0"/>
@@ -10754,7 +11486,7 @@
   <sortState xmlns:xlrd2="http://schemas.microsoft.com/office/spreadsheetml/2017/richdata2" ref="A2:L215">
     <sortCondition ref="B1:B215"/>
   </sortState>
-  <phoneticPr fontId="3" type="noConversion"/>
+  <phoneticPr fontId="4" type="noConversion"/>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
   <pageSetup orientation="portrait" horizontalDpi="0" verticalDpi="0"/>
 </worksheet>
@@ -10762,10 +11494,11 @@
 
 <file path=xl/worksheets/sheet2.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{B1AC297A-A885-7C40-9A4E-22B5A2A054BE}">
-  <dimension ref="A1:L167"/>
+  <dimension ref="A1:L275"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="A129" zoomScale="75" workbookViewId="0">
-      <selection activeCell="D163" sqref="D163"/>
+    <sheetView tabSelected="1" topLeftCell="D1" zoomScale="108" workbookViewId="0">
+      <pane ySplit="1" topLeftCell="A120" activePane="bottomLeft" state="frozen"/>
+      <selection pane="bottomLeft" activeCell="J143" sqref="J143"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="16" x14ac:dyDescent="0.2"/>
@@ -10776,6 +11509,7 @@
     <col min="4" max="4" width="19.6640625" customWidth="1"/>
     <col min="7" max="7" width="17.5" customWidth="1"/>
     <col min="8" max="9" width="23.6640625" customWidth="1"/>
+    <col min="10" max="10" width="24.1640625" customWidth="1"/>
     <col min="11" max="11" width="17.5" customWidth="1"/>
   </cols>
   <sheetData>
@@ -14386,229 +15120,3769 @@
       </c>
     </row>
     <row r="134" spans="2:12" x14ac:dyDescent="0.2">
+      <c r="B134" t="s">
+        <v>748</v>
+      </c>
       <c r="C134" s="9" t="s">
         <v>724</v>
       </c>
+      <c r="D134" t="s">
+        <v>758</v>
+      </c>
+      <c r="F134" t="s">
+        <v>166</v>
+      </c>
       <c r="G134" t="s">
         <v>424</v>
       </c>
+      <c r="I134" t="s">
+        <v>705</v>
+      </c>
       <c r="L134" t="s">
         <v>709</v>
       </c>
     </row>
     <row r="135" spans="2:12" x14ac:dyDescent="0.2">
-      <c r="C135" s="9"/>
+      <c r="B135" t="s">
+        <v>749</v>
+      </c>
+      <c r="C135" s="9" t="s">
+        <v>724</v>
+      </c>
+      <c r="D135" t="s">
+        <v>758</v>
+      </c>
+      <c r="F135" t="s">
+        <v>166</v>
+      </c>
+      <c r="G135" t="s">
+        <v>424</v>
+      </c>
+      <c r="I135" t="s">
+        <v>705</v>
+      </c>
+      <c r="L135" t="s">
+        <v>709</v>
+      </c>
     </row>
     <row r="136" spans="2:12" x14ac:dyDescent="0.2">
+      <c r="B136" t="s">
+        <v>750</v>
+      </c>
       <c r="C136" s="9" t="s">
-        <v>725</v>
+        <v>724</v>
+      </c>
+      <c r="D136" t="s">
+        <v>759</v>
+      </c>
+      <c r="F136" t="s">
+        <v>165</v>
       </c>
       <c r="G136" t="s">
         <v>424</v>
       </c>
+      <c r="I136" t="s">
+        <v>705</v>
+      </c>
       <c r="L136" t="s">
+        <v>709</v>
+      </c>
+    </row>
+    <row r="137" spans="2:12" x14ac:dyDescent="0.2">
+      <c r="B137" t="s">
+        <v>751</v>
+      </c>
+      <c r="C137" s="9" t="s">
+        <v>724</v>
+      </c>
+      <c r="D137" t="s">
+        <v>759</v>
+      </c>
+      <c r="F137" t="s">
+        <v>165</v>
+      </c>
+      <c r="G137" t="s">
+        <v>424</v>
+      </c>
+      <c r="I137" t="s">
+        <v>705</v>
+      </c>
+      <c r="L137" t="s">
+        <v>709</v>
+      </c>
+    </row>
+    <row r="138" spans="2:12" x14ac:dyDescent="0.2">
+      <c r="B138" t="s">
+        <v>752</v>
+      </c>
+      <c r="C138" s="9" t="s">
+        <v>724</v>
+      </c>
+      <c r="D138" t="s">
+        <v>760</v>
+      </c>
+      <c r="F138" t="s">
+        <v>165</v>
+      </c>
+      <c r="G138" t="s">
+        <v>424</v>
+      </c>
+      <c r="I138" t="s">
+        <v>705</v>
+      </c>
+      <c r="L138" t="s">
+        <v>709</v>
+      </c>
+    </row>
+    <row r="139" spans="2:12" x14ac:dyDescent="0.2">
+      <c r="B139" t="s">
+        <v>753</v>
+      </c>
+      <c r="C139" s="9" t="s">
+        <v>724</v>
+      </c>
+      <c r="D139" t="s">
+        <v>760</v>
+      </c>
+      <c r="F139" t="s">
+        <v>165</v>
+      </c>
+      <c r="G139" t="s">
+        <v>424</v>
+      </c>
+      <c r="I139" t="s">
+        <v>705</v>
+      </c>
+      <c r="L139" t="s">
+        <v>709</v>
+      </c>
+    </row>
+    <row r="140" spans="2:12" x14ac:dyDescent="0.2">
+      <c r="B140" t="s">
+        <v>754</v>
+      </c>
+      <c r="C140" s="9" t="s">
+        <v>724</v>
+      </c>
+      <c r="D140" t="s">
+        <v>761</v>
+      </c>
+      <c r="F140" t="s">
+        <v>165</v>
+      </c>
+      <c r="G140" t="s">
+        <v>424</v>
+      </c>
+      <c r="I140" t="s">
+        <v>705</v>
+      </c>
+      <c r="L140" t="s">
+        <v>709</v>
+      </c>
+    </row>
+    <row r="141" spans="2:12" x14ac:dyDescent="0.2">
+      <c r="B141" t="s">
+        <v>755</v>
+      </c>
+      <c r="C141" s="9" t="s">
+        <v>724</v>
+      </c>
+      <c r="D141" t="s">
+        <v>761</v>
+      </c>
+      <c r="F141" t="s">
+        <v>165</v>
+      </c>
+      <c r="G141" t="s">
+        <v>424</v>
+      </c>
+      <c r="I141" t="s">
+        <v>705</v>
+      </c>
+      <c r="L141" t="s">
+        <v>709</v>
+      </c>
+    </row>
+    <row r="142" spans="2:12" x14ac:dyDescent="0.2">
+      <c r="B142" t="s">
+        <v>756</v>
+      </c>
+      <c r="C142" s="9" t="s">
+        <v>724</v>
+      </c>
+      <c r="D142" t="s">
+        <v>762</v>
+      </c>
+      <c r="F142" t="s">
+        <v>165</v>
+      </c>
+      <c r="G142" t="s">
+        <v>424</v>
+      </c>
+      <c r="I142" t="s">
+        <v>705</v>
+      </c>
+      <c r="L142" t="s">
+        <v>709</v>
+      </c>
+    </row>
+    <row r="143" spans="2:12" x14ac:dyDescent="0.2">
+      <c r="B143" t="s">
+        <v>757</v>
+      </c>
+      <c r="C143" s="9" t="s">
+        <v>724</v>
+      </c>
+      <c r="D143" t="s">
+        <v>762</v>
+      </c>
+      <c r="F143" t="s">
+        <v>165</v>
+      </c>
+      <c r="G143" t="s">
+        <v>424</v>
+      </c>
+      <c r="I143" t="s">
+        <v>705</v>
+      </c>
+      <c r="L143" t="s">
+        <v>709</v>
+      </c>
+    </row>
+    <row r="144" spans="2:12" x14ac:dyDescent="0.2">
+      <c r="C144" s="9"/>
+    </row>
+    <row r="145" spans="2:12" x14ac:dyDescent="0.2">
+      <c r="B145" t="s">
+        <v>794</v>
+      </c>
+      <c r="C145" s="9" t="s">
+        <v>793</v>
+      </c>
+      <c r="D145" t="s">
+        <v>792</v>
+      </c>
+      <c r="E145" t="s">
+        <v>418</v>
+      </c>
+      <c r="F145" t="s">
+        <v>166</v>
+      </c>
+      <c r="G145" t="s">
+        <v>423</v>
+      </c>
+      <c r="I145" t="s">
+        <v>705</v>
+      </c>
+      <c r="J145" t="s">
+        <v>799</v>
+      </c>
+      <c r="L145" t="s">
+        <v>791</v>
+      </c>
+    </row>
+    <row r="146" spans="2:12" x14ac:dyDescent="0.2">
+      <c r="C146" s="9"/>
+    </row>
+    <row r="147" spans="2:12" x14ac:dyDescent="0.2">
+      <c r="B147" t="s">
+        <v>795</v>
+      </c>
+      <c r="C147" s="9" t="s">
+        <v>725</v>
+      </c>
+      <c r="D147" t="s">
+        <v>797</v>
+      </c>
+      <c r="E147" t="s">
+        <v>101</v>
+      </c>
+      <c r="F147" t="s">
+        <v>166</v>
+      </c>
+      <c r="G147" t="s">
+        <v>424</v>
+      </c>
+      <c r="I147" t="s">
+        <v>705</v>
+      </c>
+      <c r="J147" t="s">
+        <v>799</v>
+      </c>
+      <c r="L147" t="s">
         <v>710</v>
       </c>
     </row>
-    <row r="137" spans="2:12" x14ac:dyDescent="0.2">
-      <c r="C137" s="9"/>
-    </row>
-    <row r="138" spans="2:12" x14ac:dyDescent="0.2">
-      <c r="C138" s="9" t="s">
+    <row r="148" spans="2:12" x14ac:dyDescent="0.2">
+      <c r="B148" t="s">
+        <v>796</v>
+      </c>
+      <c r="C148" s="9" t="s">
+        <v>725</v>
+      </c>
+      <c r="D148" t="s">
+        <v>798</v>
+      </c>
+      <c r="E148" t="s">
+        <v>101</v>
+      </c>
+      <c r="F148" t="s">
+        <v>166</v>
+      </c>
+      <c r="G148" t="s">
+        <v>424</v>
+      </c>
+      <c r="I148" t="s">
+        <v>705</v>
+      </c>
+      <c r="J148" t="s">
+        <v>799</v>
+      </c>
+      <c r="L148" t="s">
+        <v>710</v>
+      </c>
+    </row>
+    <row r="149" spans="2:12" x14ac:dyDescent="0.2">
+      <c r="C149" s="9"/>
+    </row>
+    <row r="150" spans="2:12" x14ac:dyDescent="0.2">
+      <c r="B150" t="s">
+        <v>733</v>
+      </c>
+      <c r="C150" s="9" t="s">
         <v>726</v>
       </c>
-      <c r="G138" t="s">
-        <v>423</v>
-      </c>
-      <c r="L138" t="s">
+      <c r="D150" t="s">
+        <v>744</v>
+      </c>
+      <c r="E150" t="s">
+        <v>418</v>
+      </c>
+      <c r="F150" t="s">
+        <v>166</v>
+      </c>
+      <c r="G150" t="s">
+        <v>423</v>
+      </c>
+      <c r="I150" t="s">
+        <v>706</v>
+      </c>
+      <c r="J150" s="10" t="s">
+        <v>799</v>
+      </c>
+      <c r="L150" t="s">
         <v>711</v>
       </c>
     </row>
-    <row r="139" spans="2:12" x14ac:dyDescent="0.2">
-      <c r="C139" s="9"/>
-    </row>
-    <row r="140" spans="2:12" x14ac:dyDescent="0.2">
-      <c r="C140" s="9" t="s">
+    <row r="151" spans="2:12" x14ac:dyDescent="0.2">
+      <c r="B151" t="s">
+        <v>734</v>
+      </c>
+      <c r="C151" s="9" t="s">
         <v>726</v>
       </c>
-      <c r="G140" t="s">
-        <v>423</v>
-      </c>
-      <c r="L140" t="s">
+      <c r="D151" t="s">
+        <v>745</v>
+      </c>
+      <c r="E151" t="s">
+        <v>418</v>
+      </c>
+      <c r="F151" t="s">
+        <v>166</v>
+      </c>
+      <c r="G151" t="s">
+        <v>423</v>
+      </c>
+      <c r="I151" t="s">
+        <v>706</v>
+      </c>
+      <c r="J151" s="10" t="s">
+        <v>799</v>
+      </c>
+      <c r="L151" t="s">
+        <v>711</v>
+      </c>
+    </row>
+    <row r="152" spans="2:12" x14ac:dyDescent="0.2">
+      <c r="B152" t="s">
+        <v>735</v>
+      </c>
+      <c r="C152" s="9" t="s">
+        <v>726</v>
+      </c>
+      <c r="D152" t="s">
+        <v>743</v>
+      </c>
+      <c r="E152" t="s">
+        <v>418</v>
+      </c>
+      <c r="F152" t="s">
+        <v>166</v>
+      </c>
+      <c r="G152" t="s">
+        <v>423</v>
+      </c>
+      <c r="I152" t="s">
+        <v>706</v>
+      </c>
+      <c r="J152" s="10" t="s">
+        <v>799</v>
+      </c>
+      <c r="L152" t="s">
+        <v>711</v>
+      </c>
+    </row>
+    <row r="153" spans="2:12" x14ac:dyDescent="0.2">
+      <c r="B153" t="s">
+        <v>736</v>
+      </c>
+      <c r="C153" s="9" t="s">
+        <v>726</v>
+      </c>
+      <c r="D153" t="s">
+        <v>746</v>
+      </c>
+      <c r="E153" t="s">
+        <v>418</v>
+      </c>
+      <c r="F153" t="s">
+        <v>166</v>
+      </c>
+      <c r="G153" t="s">
+        <v>423</v>
+      </c>
+      <c r="I153" t="s">
+        <v>706</v>
+      </c>
+      <c r="J153" s="10" t="s">
+        <v>799</v>
+      </c>
+      <c r="L153" t="s">
+        <v>711</v>
+      </c>
+    </row>
+    <row r="154" spans="2:12" x14ac:dyDescent="0.2">
+      <c r="B154" t="s">
+        <v>737</v>
+      </c>
+      <c r="C154" s="9" t="s">
+        <v>726</v>
+      </c>
+      <c r="D154" t="s">
+        <v>747</v>
+      </c>
+      <c r="E154" t="s">
+        <v>418</v>
+      </c>
+      <c r="F154" t="s">
+        <v>165</v>
+      </c>
+      <c r="G154" t="s">
+        <v>423</v>
+      </c>
+      <c r="I154" t="s">
+        <v>706</v>
+      </c>
+      <c r="J154" s="10" t="s">
+        <v>799</v>
+      </c>
+      <c r="L154" t="s">
+        <v>711</v>
+      </c>
+    </row>
+    <row r="155" spans="2:12" x14ac:dyDescent="0.2">
+      <c r="B155" t="s">
+        <v>738</v>
+      </c>
+      <c r="C155" s="9" t="s">
+        <v>726</v>
+      </c>
+      <c r="D155" t="s">
+        <v>743</v>
+      </c>
+      <c r="E155" t="s">
+        <v>418</v>
+      </c>
+      <c r="F155" t="s">
+        <v>166</v>
+      </c>
+      <c r="G155" t="s">
+        <v>423</v>
+      </c>
+      <c r="I155" t="s">
+        <v>706</v>
+      </c>
+      <c r="J155" s="10" t="s">
+        <v>799</v>
+      </c>
+      <c r="L155" t="s">
+        <v>711</v>
+      </c>
+    </row>
+    <row r="156" spans="2:12" x14ac:dyDescent="0.2">
+      <c r="B156" t="s">
+        <v>739</v>
+      </c>
+      <c r="C156" s="9" t="s">
+        <v>726</v>
+      </c>
+      <c r="D156" t="s">
+        <v>745</v>
+      </c>
+      <c r="E156" t="s">
+        <v>418</v>
+      </c>
+      <c r="F156" t="s">
+        <v>166</v>
+      </c>
+      <c r="G156" t="s">
+        <v>423</v>
+      </c>
+      <c r="I156" t="s">
+        <v>706</v>
+      </c>
+      <c r="J156" s="10" t="s">
+        <v>799</v>
+      </c>
+      <c r="L156" t="s">
+        <v>711</v>
+      </c>
+    </row>
+    <row r="157" spans="2:12" x14ac:dyDescent="0.2">
+      <c r="B157" t="s">
+        <v>740</v>
+      </c>
+      <c r="C157" s="9" t="s">
+        <v>726</v>
+      </c>
+      <c r="D157" t="s">
+        <v>744</v>
+      </c>
+      <c r="E157" t="s">
+        <v>418</v>
+      </c>
+      <c r="F157" t="s">
+        <v>166</v>
+      </c>
+      <c r="G157" t="s">
+        <v>423</v>
+      </c>
+      <c r="I157" t="s">
+        <v>706</v>
+      </c>
+      <c r="J157" s="10" t="s">
+        <v>799</v>
+      </c>
+      <c r="L157" t="s">
+        <v>711</v>
+      </c>
+    </row>
+    <row r="158" spans="2:12" x14ac:dyDescent="0.2">
+      <c r="B158" t="s">
+        <v>741</v>
+      </c>
+      <c r="C158" s="9" t="s">
+        <v>726</v>
+      </c>
+      <c r="D158" t="s">
+        <v>746</v>
+      </c>
+      <c r="E158" t="s">
+        <v>418</v>
+      </c>
+      <c r="F158" t="s">
+        <v>166</v>
+      </c>
+      <c r="G158" t="s">
+        <v>423</v>
+      </c>
+      <c r="I158" t="s">
+        <v>706</v>
+      </c>
+      <c r="J158" s="10" t="s">
+        <v>799</v>
+      </c>
+      <c r="L158" t="s">
+        <v>711</v>
+      </c>
+    </row>
+    <row r="159" spans="2:12" x14ac:dyDescent="0.2">
+      <c r="B159" t="s">
+        <v>742</v>
+      </c>
+      <c r="C159" s="9" t="s">
+        <v>726</v>
+      </c>
+      <c r="D159" t="s">
+        <v>747</v>
+      </c>
+      <c r="E159" t="s">
+        <v>418</v>
+      </c>
+      <c r="F159" t="s">
+        <v>165</v>
+      </c>
+      <c r="G159" t="s">
+        <v>423</v>
+      </c>
+      <c r="I159" t="s">
+        <v>706</v>
+      </c>
+      <c r="J159" s="10" t="s">
+        <v>799</v>
+      </c>
+      <c r="L159" t="s">
+        <v>711</v>
+      </c>
+    </row>
+    <row r="160" spans="2:12" x14ac:dyDescent="0.2">
+      <c r="C160" s="9"/>
+    </row>
+    <row r="161" spans="2:12" x14ac:dyDescent="0.2">
+      <c r="B161" t="s">
+        <v>763</v>
+      </c>
+      <c r="C161" s="9" t="s">
+        <v>726</v>
+      </c>
+      <c r="D161" t="s">
+        <v>787</v>
+      </c>
+      <c r="E161" t="s">
+        <v>418</v>
+      </c>
+      <c r="F161" t="s">
+        <v>165</v>
+      </c>
+      <c r="G161" t="s">
+        <v>423</v>
+      </c>
+      <c r="H161" t="s">
+        <v>427</v>
+      </c>
+      <c r="I161" t="s">
+        <v>706</v>
+      </c>
+      <c r="L161" t="s">
         <v>712</v>
       </c>
     </row>
-    <row r="141" spans="2:12" x14ac:dyDescent="0.2">
-      <c r="C141" s="9"/>
-    </row>
-    <row r="142" spans="2:12" x14ac:dyDescent="0.2">
-      <c r="C142" s="9" t="s">
+    <row r="162" spans="2:12" x14ac:dyDescent="0.2">
+      <c r="B162" t="s">
+        <v>764</v>
+      </c>
+      <c r="C162" s="9" t="s">
+        <v>726</v>
+      </c>
+      <c r="D162" t="s">
+        <v>787</v>
+      </c>
+      <c r="E162" t="s">
+        <v>418</v>
+      </c>
+      <c r="F162" t="s">
+        <v>165</v>
+      </c>
+      <c r="G162" t="s">
+        <v>423</v>
+      </c>
+      <c r="H162" t="s">
+        <v>427</v>
+      </c>
+      <c r="I162" t="s">
+        <v>706</v>
+      </c>
+      <c r="L162" t="s">
+        <v>712</v>
+      </c>
+    </row>
+    <row r="163" spans="2:12" x14ac:dyDescent="0.2">
+      <c r="B163" t="s">
+        <v>765</v>
+      </c>
+      <c r="C163" s="9" t="s">
+        <v>726</v>
+      </c>
+      <c r="D163" t="s">
+        <v>787</v>
+      </c>
+      <c r="E163" t="s">
+        <v>418</v>
+      </c>
+      <c r="F163" t="s">
+        <v>165</v>
+      </c>
+      <c r="G163" t="s">
+        <v>423</v>
+      </c>
+      <c r="H163" t="s">
+        <v>427</v>
+      </c>
+      <c r="I163" t="s">
+        <v>706</v>
+      </c>
+      <c r="L163" t="s">
+        <v>712</v>
+      </c>
+    </row>
+    <row r="164" spans="2:12" x14ac:dyDescent="0.2">
+      <c r="B164" t="s">
+        <v>766</v>
+      </c>
+      <c r="C164" s="9" t="s">
+        <v>726</v>
+      </c>
+      <c r="D164" t="s">
+        <v>787</v>
+      </c>
+      <c r="E164" t="s">
+        <v>418</v>
+      </c>
+      <c r="F164" t="s">
+        <v>165</v>
+      </c>
+      <c r="G164" t="s">
+        <v>423</v>
+      </c>
+      <c r="H164" t="s">
+        <v>427</v>
+      </c>
+      <c r="I164" t="s">
+        <v>706</v>
+      </c>
+      <c r="L164" t="s">
+        <v>712</v>
+      </c>
+    </row>
+    <row r="165" spans="2:12" x14ac:dyDescent="0.2">
+      <c r="B165" t="s">
+        <v>767</v>
+      </c>
+      <c r="C165" s="9" t="s">
+        <v>726</v>
+      </c>
+      <c r="D165" t="s">
+        <v>787</v>
+      </c>
+      <c r="E165" t="s">
+        <v>418</v>
+      </c>
+      <c r="F165" t="s">
+        <v>165</v>
+      </c>
+      <c r="G165" t="s">
+        <v>423</v>
+      </c>
+      <c r="H165" t="s">
+        <v>427</v>
+      </c>
+      <c r="I165" t="s">
+        <v>706</v>
+      </c>
+      <c r="L165" t="s">
+        <v>712</v>
+      </c>
+    </row>
+    <row r="166" spans="2:12" x14ac:dyDescent="0.2">
+      <c r="B166" t="s">
+        <v>768</v>
+      </c>
+      <c r="C166" s="9" t="s">
+        <v>726</v>
+      </c>
+      <c r="D166" t="s">
+        <v>787</v>
+      </c>
+      <c r="E166" t="s">
+        <v>418</v>
+      </c>
+      <c r="F166" t="s">
+        <v>165</v>
+      </c>
+      <c r="G166" t="s">
+        <v>423</v>
+      </c>
+      <c r="H166" t="s">
+        <v>427</v>
+      </c>
+      <c r="I166" t="s">
+        <v>706</v>
+      </c>
+      <c r="L166" t="s">
+        <v>712</v>
+      </c>
+    </row>
+    <row r="167" spans="2:12" x14ac:dyDescent="0.2">
+      <c r="B167" t="s">
+        <v>769</v>
+      </c>
+      <c r="C167" s="9" t="s">
+        <v>726</v>
+      </c>
+      <c r="D167" t="s">
+        <v>788</v>
+      </c>
+      <c r="E167" t="s">
+        <v>418</v>
+      </c>
+      <c r="F167" t="s">
+        <v>165</v>
+      </c>
+      <c r="G167" t="s">
+        <v>423</v>
+      </c>
+      <c r="H167" t="s">
+        <v>427</v>
+      </c>
+      <c r="I167" t="s">
+        <v>706</v>
+      </c>
+      <c r="L167" t="s">
+        <v>712</v>
+      </c>
+    </row>
+    <row r="168" spans="2:12" x14ac:dyDescent="0.2">
+      <c r="B168" t="s">
+        <v>770</v>
+      </c>
+      <c r="C168" s="9" t="s">
+        <v>726</v>
+      </c>
+      <c r="D168" t="s">
+        <v>788</v>
+      </c>
+      <c r="E168" t="s">
+        <v>418</v>
+      </c>
+      <c r="F168" t="s">
+        <v>165</v>
+      </c>
+      <c r="G168" t="s">
+        <v>423</v>
+      </c>
+      <c r="H168" t="s">
+        <v>427</v>
+      </c>
+      <c r="I168" t="s">
+        <v>706</v>
+      </c>
+      <c r="L168" t="s">
+        <v>712</v>
+      </c>
+    </row>
+    <row r="169" spans="2:12" x14ac:dyDescent="0.2">
+      <c r="B169" t="s">
+        <v>771</v>
+      </c>
+      <c r="C169" s="9" t="s">
+        <v>726</v>
+      </c>
+      <c r="D169" t="s">
+        <v>788</v>
+      </c>
+      <c r="E169" t="s">
+        <v>418</v>
+      </c>
+      <c r="F169" t="s">
+        <v>165</v>
+      </c>
+      <c r="G169" t="s">
+        <v>423</v>
+      </c>
+      <c r="H169" t="s">
+        <v>427</v>
+      </c>
+      <c r="I169" t="s">
+        <v>706</v>
+      </c>
+      <c r="L169" t="s">
+        <v>712</v>
+      </c>
+    </row>
+    <row r="170" spans="2:12" x14ac:dyDescent="0.2">
+      <c r="B170" t="s">
+        <v>772</v>
+      </c>
+      <c r="C170" s="9" t="s">
+        <v>726</v>
+      </c>
+      <c r="D170" t="s">
+        <v>788</v>
+      </c>
+      <c r="E170" t="s">
+        <v>418</v>
+      </c>
+      <c r="F170" t="s">
+        <v>165</v>
+      </c>
+      <c r="G170" t="s">
+        <v>423</v>
+      </c>
+      <c r="H170" t="s">
+        <v>427</v>
+      </c>
+      <c r="I170" t="s">
+        <v>706</v>
+      </c>
+      <c r="L170" t="s">
+        <v>712</v>
+      </c>
+    </row>
+    <row r="171" spans="2:12" x14ac:dyDescent="0.2">
+      <c r="B171" t="s">
+        <v>773</v>
+      </c>
+      <c r="C171" s="9" t="s">
+        <v>726</v>
+      </c>
+      <c r="D171" t="s">
+        <v>788</v>
+      </c>
+      <c r="E171" t="s">
+        <v>418</v>
+      </c>
+      <c r="F171" t="s">
+        <v>165</v>
+      </c>
+      <c r="G171" t="s">
+        <v>423</v>
+      </c>
+      <c r="H171" t="s">
+        <v>427</v>
+      </c>
+      <c r="I171" t="s">
+        <v>706</v>
+      </c>
+      <c r="L171" t="s">
+        <v>712</v>
+      </c>
+    </row>
+    <row r="172" spans="2:12" x14ac:dyDescent="0.2">
+      <c r="B172" t="s">
+        <v>774</v>
+      </c>
+      <c r="C172" s="9" t="s">
+        <v>726</v>
+      </c>
+      <c r="D172" t="s">
+        <v>788</v>
+      </c>
+      <c r="E172" t="s">
+        <v>418</v>
+      </c>
+      <c r="F172" t="s">
+        <v>165</v>
+      </c>
+      <c r="G172" t="s">
+        <v>423</v>
+      </c>
+      <c r="H172" t="s">
+        <v>427</v>
+      </c>
+      <c r="I172" t="s">
+        <v>706</v>
+      </c>
+      <c r="L172" t="s">
+        <v>712</v>
+      </c>
+    </row>
+    <row r="173" spans="2:12" x14ac:dyDescent="0.2">
+      <c r="B173" t="s">
+        <v>775</v>
+      </c>
+      <c r="C173" s="9" t="s">
+        <v>726</v>
+      </c>
+      <c r="D173" t="s">
+        <v>789</v>
+      </c>
+      <c r="E173" t="s">
+        <v>418</v>
+      </c>
+      <c r="F173" t="s">
+        <v>165</v>
+      </c>
+      <c r="G173" t="s">
+        <v>423</v>
+      </c>
+      <c r="H173" t="s">
+        <v>427</v>
+      </c>
+      <c r="I173" t="s">
+        <v>706</v>
+      </c>
+      <c r="L173" t="s">
+        <v>712</v>
+      </c>
+    </row>
+    <row r="174" spans="2:12" x14ac:dyDescent="0.2">
+      <c r="B174" t="s">
+        <v>776</v>
+      </c>
+      <c r="C174" s="9" t="s">
+        <v>726</v>
+      </c>
+      <c r="D174" t="s">
+        <v>789</v>
+      </c>
+      <c r="E174" t="s">
+        <v>418</v>
+      </c>
+      <c r="F174" t="s">
+        <v>165</v>
+      </c>
+      <c r="G174" t="s">
+        <v>423</v>
+      </c>
+      <c r="H174" t="s">
+        <v>427</v>
+      </c>
+      <c r="I174" t="s">
+        <v>706</v>
+      </c>
+      <c r="L174" t="s">
+        <v>712</v>
+      </c>
+    </row>
+    <row r="175" spans="2:12" x14ac:dyDescent="0.2">
+      <c r="B175" t="s">
+        <v>777</v>
+      </c>
+      <c r="C175" s="9" t="s">
+        <v>726</v>
+      </c>
+      <c r="D175" t="s">
+        <v>789</v>
+      </c>
+      <c r="E175" t="s">
+        <v>418</v>
+      </c>
+      <c r="F175" t="s">
+        <v>165</v>
+      </c>
+      <c r="G175" t="s">
+        <v>423</v>
+      </c>
+      <c r="H175" t="s">
+        <v>427</v>
+      </c>
+      <c r="I175" t="s">
+        <v>706</v>
+      </c>
+      <c r="L175" t="s">
+        <v>712</v>
+      </c>
+    </row>
+    <row r="176" spans="2:12" x14ac:dyDescent="0.2">
+      <c r="B176" t="s">
+        <v>778</v>
+      </c>
+      <c r="C176" s="9" t="s">
+        <v>726</v>
+      </c>
+      <c r="D176" t="s">
+        <v>789</v>
+      </c>
+      <c r="E176" t="s">
+        <v>418</v>
+      </c>
+      <c r="F176" t="s">
+        <v>165</v>
+      </c>
+      <c r="G176" t="s">
+        <v>423</v>
+      </c>
+      <c r="H176" t="s">
+        <v>427</v>
+      </c>
+      <c r="I176" t="s">
+        <v>706</v>
+      </c>
+      <c r="L176" t="s">
+        <v>712</v>
+      </c>
+    </row>
+    <row r="177" spans="2:12" x14ac:dyDescent="0.2">
+      <c r="B177" t="s">
+        <v>779</v>
+      </c>
+      <c r="C177" s="9" t="s">
+        <v>726</v>
+      </c>
+      <c r="D177" t="s">
+        <v>789</v>
+      </c>
+      <c r="E177" t="s">
+        <v>418</v>
+      </c>
+      <c r="F177" t="s">
+        <v>165</v>
+      </c>
+      <c r="G177" t="s">
+        <v>423</v>
+      </c>
+      <c r="H177" t="s">
+        <v>427</v>
+      </c>
+      <c r="I177" t="s">
+        <v>706</v>
+      </c>
+      <c r="L177" t="s">
+        <v>712</v>
+      </c>
+    </row>
+    <row r="178" spans="2:12" x14ac:dyDescent="0.2">
+      <c r="B178" t="s">
+        <v>780</v>
+      </c>
+      <c r="C178" s="9" t="s">
+        <v>726</v>
+      </c>
+      <c r="D178" t="s">
+        <v>789</v>
+      </c>
+      <c r="E178" t="s">
+        <v>418</v>
+      </c>
+      <c r="F178" t="s">
+        <v>165</v>
+      </c>
+      <c r="G178" t="s">
+        <v>423</v>
+      </c>
+      <c r="H178" t="s">
+        <v>427</v>
+      </c>
+      <c r="I178" t="s">
+        <v>706</v>
+      </c>
+      <c r="L178" t="s">
+        <v>712</v>
+      </c>
+    </row>
+    <row r="179" spans="2:12" x14ac:dyDescent="0.2">
+      <c r="B179" t="s">
+        <v>781</v>
+      </c>
+      <c r="C179" s="9" t="s">
+        <v>726</v>
+      </c>
+      <c r="D179" t="s">
+        <v>790</v>
+      </c>
+      <c r="E179" t="s">
+        <v>418</v>
+      </c>
+      <c r="F179" t="s">
+        <v>165</v>
+      </c>
+      <c r="G179" t="s">
+        <v>423</v>
+      </c>
+      <c r="H179" t="s">
+        <v>427</v>
+      </c>
+      <c r="I179" t="s">
+        <v>706</v>
+      </c>
+      <c r="L179" t="s">
+        <v>712</v>
+      </c>
+    </row>
+    <row r="180" spans="2:12" x14ac:dyDescent="0.2">
+      <c r="B180" t="s">
+        <v>782</v>
+      </c>
+      <c r="C180" s="9" t="s">
+        <v>726</v>
+      </c>
+      <c r="D180" t="s">
+        <v>790</v>
+      </c>
+      <c r="E180" t="s">
+        <v>418</v>
+      </c>
+      <c r="F180" t="s">
+        <v>165</v>
+      </c>
+      <c r="G180" t="s">
+        <v>423</v>
+      </c>
+      <c r="H180" t="s">
+        <v>427</v>
+      </c>
+      <c r="I180" t="s">
+        <v>706</v>
+      </c>
+      <c r="L180" t="s">
+        <v>712</v>
+      </c>
+    </row>
+    <row r="181" spans="2:12" x14ac:dyDescent="0.2">
+      <c r="B181" t="s">
+        <v>783</v>
+      </c>
+      <c r="C181" s="9" t="s">
+        <v>726</v>
+      </c>
+      <c r="D181" t="s">
+        <v>790</v>
+      </c>
+      <c r="E181" t="s">
+        <v>418</v>
+      </c>
+      <c r="F181" t="s">
+        <v>165</v>
+      </c>
+      <c r="G181" t="s">
+        <v>423</v>
+      </c>
+      <c r="H181" t="s">
+        <v>427</v>
+      </c>
+      <c r="I181" t="s">
+        <v>706</v>
+      </c>
+      <c r="L181" t="s">
+        <v>712</v>
+      </c>
+    </row>
+    <row r="182" spans="2:12" x14ac:dyDescent="0.2">
+      <c r="B182" t="s">
+        <v>784</v>
+      </c>
+      <c r="C182" s="9" t="s">
+        <v>726</v>
+      </c>
+      <c r="D182" t="s">
+        <v>790</v>
+      </c>
+      <c r="E182" t="s">
+        <v>418</v>
+      </c>
+      <c r="F182" t="s">
+        <v>165</v>
+      </c>
+      <c r="G182" t="s">
+        <v>423</v>
+      </c>
+      <c r="H182" t="s">
+        <v>427</v>
+      </c>
+      <c r="I182" t="s">
+        <v>706</v>
+      </c>
+      <c r="L182" t="s">
+        <v>712</v>
+      </c>
+    </row>
+    <row r="183" spans="2:12" x14ac:dyDescent="0.2">
+      <c r="B183" t="s">
+        <v>785</v>
+      </c>
+      <c r="C183" s="9" t="s">
+        <v>726</v>
+      </c>
+      <c r="D183" t="s">
+        <v>790</v>
+      </c>
+      <c r="E183" t="s">
+        <v>418</v>
+      </c>
+      <c r="F183" t="s">
+        <v>165</v>
+      </c>
+      <c r="G183" t="s">
+        <v>423</v>
+      </c>
+      <c r="H183" t="s">
+        <v>427</v>
+      </c>
+      <c r="I183" t="s">
+        <v>706</v>
+      </c>
+      <c r="L183" t="s">
+        <v>712</v>
+      </c>
+    </row>
+    <row r="184" spans="2:12" x14ac:dyDescent="0.2">
+      <c r="B184" t="s">
+        <v>786</v>
+      </c>
+      <c r="C184" s="9" t="s">
+        <v>726</v>
+      </c>
+      <c r="D184" t="s">
+        <v>790</v>
+      </c>
+      <c r="E184" t="s">
+        <v>418</v>
+      </c>
+      <c r="F184" t="s">
+        <v>165</v>
+      </c>
+      <c r="G184" t="s">
+        <v>423</v>
+      </c>
+      <c r="H184" t="s">
+        <v>427</v>
+      </c>
+      <c r="I184" t="s">
+        <v>706</v>
+      </c>
+      <c r="L184" t="s">
+        <v>712</v>
+      </c>
+    </row>
+    <row r="185" spans="2:12" x14ac:dyDescent="0.2">
+      <c r="C185" s="9"/>
+    </row>
+    <row r="186" spans="2:12" x14ac:dyDescent="0.2">
+      <c r="B186" t="s">
+        <v>800</v>
+      </c>
+      <c r="C186" s="9" t="s">
         <v>727</v>
       </c>
-      <c r="G142" t="s">
-        <v>423</v>
-      </c>
-      <c r="L142" t="s">
+      <c r="D186" s="2" t="s">
+        <v>808</v>
+      </c>
+      <c r="E186" s="9" t="s">
+        <v>418</v>
+      </c>
+      <c r="F186" s="7" t="s">
+        <v>165</v>
+      </c>
+      <c r="G186" t="s">
+        <v>423</v>
+      </c>
+      <c r="H186" t="s">
+        <v>427</v>
+      </c>
+      <c r="I186" t="s">
+        <v>705</v>
+      </c>
+      <c r="J186" t="s">
+        <v>799</v>
+      </c>
+      <c r="L186" t="s">
         <v>713</v>
       </c>
     </row>
-    <row r="143" spans="2:12" x14ac:dyDescent="0.2">
-      <c r="C143" s="9"/>
-    </row>
-    <row r="144" spans="2:12" x14ac:dyDescent="0.2">
-      <c r="C144" s="9" t="s">
+    <row r="187" spans="2:12" x14ac:dyDescent="0.2">
+      <c r="B187" t="s">
+        <v>801</v>
+      </c>
+      <c r="C187" s="9" t="s">
+        <v>727</v>
+      </c>
+      <c r="D187" s="2" t="s">
+        <v>808</v>
+      </c>
+      <c r="E187" s="9" t="s">
+        <v>418</v>
+      </c>
+      <c r="F187" s="7" t="s">
+        <v>165</v>
+      </c>
+      <c r="G187" t="s">
+        <v>423</v>
+      </c>
+      <c r="H187" t="s">
+        <v>427</v>
+      </c>
+      <c r="I187" t="s">
+        <v>705</v>
+      </c>
+      <c r="J187" t="s">
+        <v>799</v>
+      </c>
+      <c r="L187" t="s">
+        <v>713</v>
+      </c>
+    </row>
+    <row r="188" spans="2:12" x14ac:dyDescent="0.2">
+      <c r="B188" t="s">
+        <v>802</v>
+      </c>
+      <c r="C188" s="9" t="s">
+        <v>727</v>
+      </c>
+      <c r="D188" s="2" t="s">
+        <v>808</v>
+      </c>
+      <c r="E188" s="9" t="s">
+        <v>418</v>
+      </c>
+      <c r="F188" s="7" t="s">
+        <v>165</v>
+      </c>
+      <c r="G188" t="s">
+        <v>423</v>
+      </c>
+      <c r="H188" t="s">
+        <v>427</v>
+      </c>
+      <c r="I188" t="s">
+        <v>705</v>
+      </c>
+      <c r="J188" t="s">
+        <v>799</v>
+      </c>
+      <c r="L188" t="s">
+        <v>713</v>
+      </c>
+    </row>
+    <row r="189" spans="2:12" x14ac:dyDescent="0.2">
+      <c r="B189" t="s">
+        <v>803</v>
+      </c>
+      <c r="C189" s="9" t="s">
+        <v>727</v>
+      </c>
+      <c r="D189" s="2" t="s">
+        <v>808</v>
+      </c>
+      <c r="E189" s="9" t="s">
+        <v>418</v>
+      </c>
+      <c r="F189" s="7" t="s">
+        <v>165</v>
+      </c>
+      <c r="G189" t="s">
+        <v>423</v>
+      </c>
+      <c r="H189" t="s">
+        <v>427</v>
+      </c>
+      <c r="I189" t="s">
+        <v>705</v>
+      </c>
+      <c r="J189" t="s">
+        <v>799</v>
+      </c>
+      <c r="L189" t="s">
+        <v>713</v>
+      </c>
+    </row>
+    <row r="190" spans="2:12" x14ac:dyDescent="0.2">
+      <c r="B190" t="s">
+        <v>804</v>
+      </c>
+      <c r="C190" s="9" t="s">
+        <v>727</v>
+      </c>
+      <c r="D190" s="2" t="s">
+        <v>808</v>
+      </c>
+      <c r="E190" s="9" t="s">
+        <v>418</v>
+      </c>
+      <c r="F190" s="7" t="s">
+        <v>165</v>
+      </c>
+      <c r="G190" t="s">
+        <v>423</v>
+      </c>
+      <c r="H190" t="s">
+        <v>427</v>
+      </c>
+      <c r="I190" t="s">
+        <v>705</v>
+      </c>
+      <c r="J190" t="s">
+        <v>799</v>
+      </c>
+      <c r="L190" t="s">
+        <v>713</v>
+      </c>
+    </row>
+    <row r="191" spans="2:12" x14ac:dyDescent="0.2">
+      <c r="B191" t="s">
+        <v>805</v>
+      </c>
+      <c r="C191" s="9" t="s">
+        <v>727</v>
+      </c>
+      <c r="D191" s="2" t="s">
+        <v>808</v>
+      </c>
+      <c r="E191" s="9" t="s">
+        <v>418</v>
+      </c>
+      <c r="F191" s="7" t="s">
+        <v>165</v>
+      </c>
+      <c r="G191" t="s">
+        <v>423</v>
+      </c>
+      <c r="H191" t="s">
+        <v>427</v>
+      </c>
+      <c r="I191" t="s">
+        <v>705</v>
+      </c>
+      <c r="J191" t="s">
+        <v>799</v>
+      </c>
+      <c r="L191" t="s">
+        <v>713</v>
+      </c>
+    </row>
+    <row r="192" spans="2:12" x14ac:dyDescent="0.2">
+      <c r="B192" t="s">
+        <v>806</v>
+      </c>
+      <c r="C192" s="9" t="s">
+        <v>727</v>
+      </c>
+      <c r="D192" s="2" t="s">
+        <v>808</v>
+      </c>
+      <c r="E192" s="9" t="s">
+        <v>418</v>
+      </c>
+      <c r="F192" s="7" t="s">
+        <v>165</v>
+      </c>
+      <c r="G192" t="s">
+        <v>423</v>
+      </c>
+      <c r="H192" t="s">
+        <v>427</v>
+      </c>
+      <c r="I192" t="s">
+        <v>705</v>
+      </c>
+      <c r="J192" t="s">
+        <v>799</v>
+      </c>
+      <c r="L192" t="s">
+        <v>713</v>
+      </c>
+    </row>
+    <row r="193" spans="2:12" x14ac:dyDescent="0.2">
+      <c r="B193" t="s">
+        <v>807</v>
+      </c>
+      <c r="C193" s="9" t="s">
+        <v>727</v>
+      </c>
+      <c r="D193" s="2" t="s">
+        <v>808</v>
+      </c>
+      <c r="E193" s="9" t="s">
+        <v>418</v>
+      </c>
+      <c r="F193" s="7" t="s">
+        <v>165</v>
+      </c>
+      <c r="G193" t="s">
+        <v>423</v>
+      </c>
+      <c r="H193" t="s">
+        <v>427</v>
+      </c>
+      <c r="I193" t="s">
+        <v>705</v>
+      </c>
+      <c r="J193" t="s">
+        <v>799</v>
+      </c>
+      <c r="L193" t="s">
+        <v>713</v>
+      </c>
+    </row>
+    <row r="194" spans="2:12" x14ac:dyDescent="0.2">
+      <c r="C194" s="9"/>
+    </row>
+    <row r="195" spans="2:12" x14ac:dyDescent="0.2">
+      <c r="B195" t="s">
+        <v>809</v>
+      </c>
+      <c r="C195" s="9" t="s">
         <v>728</v>
       </c>
-      <c r="G144" t="s">
-        <v>423</v>
-      </c>
-      <c r="L144" t="s">
+      <c r="D195" t="s">
+        <v>834</v>
+      </c>
+      <c r="E195" t="s">
+        <v>418</v>
+      </c>
+      <c r="F195" t="s">
+        <v>166</v>
+      </c>
+      <c r="G195" t="s">
+        <v>423</v>
+      </c>
+      <c r="H195" t="s">
+        <v>427</v>
+      </c>
+      <c r="I195" t="s">
+        <v>706</v>
+      </c>
+      <c r="J195" s="8" t="s">
+        <v>799</v>
+      </c>
+      <c r="L195" t="s">
         <v>714</v>
       </c>
     </row>
-    <row r="145" spans="3:12" x14ac:dyDescent="0.2">
-      <c r="C145" s="9"/>
-    </row>
-    <row r="146" spans="3:12" x14ac:dyDescent="0.2">
-      <c r="C146" s="9" t="s">
+    <row r="196" spans="2:12" x14ac:dyDescent="0.2">
+      <c r="B196" t="s">
+        <v>810</v>
+      </c>
+      <c r="C196" s="9" t="s">
+        <v>728</v>
+      </c>
+      <c r="D196" t="s">
+        <v>834</v>
+      </c>
+      <c r="E196" t="s">
+        <v>418</v>
+      </c>
+      <c r="F196" t="s">
+        <v>166</v>
+      </c>
+      <c r="G196" t="s">
+        <v>423</v>
+      </c>
+      <c r="H196" t="s">
+        <v>427</v>
+      </c>
+      <c r="I196" t="s">
+        <v>706</v>
+      </c>
+      <c r="J196" s="8" t="s">
+        <v>799</v>
+      </c>
+      <c r="L196" t="s">
+        <v>714</v>
+      </c>
+    </row>
+    <row r="197" spans="2:12" x14ac:dyDescent="0.2">
+      <c r="B197" t="s">
+        <v>811</v>
+      </c>
+      <c r="C197" s="9" t="s">
+        <v>728</v>
+      </c>
+      <c r="D197" t="s">
+        <v>834</v>
+      </c>
+      <c r="E197" t="s">
+        <v>418</v>
+      </c>
+      <c r="F197" t="s">
+        <v>166</v>
+      </c>
+      <c r="G197" t="s">
+        <v>423</v>
+      </c>
+      <c r="H197" t="s">
+        <v>427</v>
+      </c>
+      <c r="I197" t="s">
+        <v>706</v>
+      </c>
+      <c r="J197" s="8" t="s">
+        <v>799</v>
+      </c>
+      <c r="L197" t="s">
+        <v>714</v>
+      </c>
+    </row>
+    <row r="198" spans="2:12" x14ac:dyDescent="0.2">
+      <c r="B198" t="s">
+        <v>812</v>
+      </c>
+      <c r="C198" s="9" t="s">
+        <v>728</v>
+      </c>
+      <c r="D198" t="s">
+        <v>834</v>
+      </c>
+      <c r="E198" t="s">
+        <v>418</v>
+      </c>
+      <c r="F198" t="s">
+        <v>166</v>
+      </c>
+      <c r="G198" t="s">
+        <v>423</v>
+      </c>
+      <c r="H198" t="s">
+        <v>427</v>
+      </c>
+      <c r="I198" t="s">
+        <v>706</v>
+      </c>
+      <c r="J198" s="8" t="s">
+        <v>799</v>
+      </c>
+      <c r="L198" t="s">
+        <v>714</v>
+      </c>
+    </row>
+    <row r="199" spans="2:12" x14ac:dyDescent="0.2">
+      <c r="B199" t="s">
+        <v>813</v>
+      </c>
+      <c r="C199" s="9" t="s">
+        <v>728</v>
+      </c>
+      <c r="D199" t="s">
+        <v>834</v>
+      </c>
+      <c r="E199" t="s">
+        <v>418</v>
+      </c>
+      <c r="F199" t="s">
+        <v>166</v>
+      </c>
+      <c r="G199" t="s">
+        <v>423</v>
+      </c>
+      <c r="H199" t="s">
+        <v>427</v>
+      </c>
+      <c r="I199" t="s">
+        <v>706</v>
+      </c>
+      <c r="J199" s="8" t="s">
+        <v>799</v>
+      </c>
+      <c r="L199" t="s">
+        <v>714</v>
+      </c>
+    </row>
+    <row r="200" spans="2:12" x14ac:dyDescent="0.2">
+      <c r="B200" t="s">
+        <v>814</v>
+      </c>
+      <c r="C200" s="9" t="s">
+        <v>728</v>
+      </c>
+      <c r="D200" t="s">
+        <v>835</v>
+      </c>
+      <c r="E200" t="s">
+        <v>418</v>
+      </c>
+      <c r="F200" t="s">
+        <v>166</v>
+      </c>
+      <c r="G200" t="s">
+        <v>423</v>
+      </c>
+      <c r="H200" t="s">
+        <v>427</v>
+      </c>
+      <c r="I200" t="s">
+        <v>706</v>
+      </c>
+      <c r="J200" s="8" t="s">
+        <v>799</v>
+      </c>
+      <c r="L200" t="s">
+        <v>714</v>
+      </c>
+    </row>
+    <row r="201" spans="2:12" x14ac:dyDescent="0.2">
+      <c r="B201" t="s">
+        <v>815</v>
+      </c>
+      <c r="C201" s="9" t="s">
+        <v>728</v>
+      </c>
+      <c r="D201" t="s">
+        <v>835</v>
+      </c>
+      <c r="E201" t="s">
+        <v>418</v>
+      </c>
+      <c r="F201" t="s">
+        <v>166</v>
+      </c>
+      <c r="G201" t="s">
+        <v>423</v>
+      </c>
+      <c r="H201" t="s">
+        <v>427</v>
+      </c>
+      <c r="I201" t="s">
+        <v>706</v>
+      </c>
+      <c r="J201" s="8" t="s">
+        <v>799</v>
+      </c>
+      <c r="L201" t="s">
+        <v>714</v>
+      </c>
+    </row>
+    <row r="202" spans="2:12" x14ac:dyDescent="0.2">
+      <c r="B202" t="s">
+        <v>816</v>
+      </c>
+      <c r="C202" s="9" t="s">
+        <v>728</v>
+      </c>
+      <c r="D202" t="s">
+        <v>835</v>
+      </c>
+      <c r="E202" t="s">
+        <v>418</v>
+      </c>
+      <c r="F202" t="s">
+        <v>166</v>
+      </c>
+      <c r="G202" t="s">
+        <v>423</v>
+      </c>
+      <c r="H202" t="s">
+        <v>427</v>
+      </c>
+      <c r="I202" t="s">
+        <v>706</v>
+      </c>
+      <c r="J202" s="8" t="s">
+        <v>799</v>
+      </c>
+      <c r="L202" t="s">
+        <v>714</v>
+      </c>
+    </row>
+    <row r="203" spans="2:12" x14ac:dyDescent="0.2">
+      <c r="B203" t="s">
+        <v>817</v>
+      </c>
+      <c r="C203" s="9" t="s">
+        <v>728</v>
+      </c>
+      <c r="D203" t="s">
+        <v>835</v>
+      </c>
+      <c r="E203" t="s">
+        <v>418</v>
+      </c>
+      <c r="F203" t="s">
+        <v>166</v>
+      </c>
+      <c r="G203" t="s">
+        <v>423</v>
+      </c>
+      <c r="H203" t="s">
+        <v>427</v>
+      </c>
+      <c r="I203" t="s">
+        <v>706</v>
+      </c>
+      <c r="J203" s="8" t="s">
+        <v>799</v>
+      </c>
+      <c r="L203" t="s">
+        <v>714</v>
+      </c>
+    </row>
+    <row r="204" spans="2:12" x14ac:dyDescent="0.2">
+      <c r="B204" t="s">
+        <v>818</v>
+      </c>
+      <c r="C204" s="9" t="s">
+        <v>728</v>
+      </c>
+      <c r="D204" t="s">
+        <v>835</v>
+      </c>
+      <c r="E204" t="s">
+        <v>418</v>
+      </c>
+      <c r="F204" t="s">
+        <v>166</v>
+      </c>
+      <c r="G204" t="s">
+        <v>423</v>
+      </c>
+      <c r="H204" t="s">
+        <v>427</v>
+      </c>
+      <c r="I204" t="s">
+        <v>706</v>
+      </c>
+      <c r="J204" s="8" t="s">
+        <v>799</v>
+      </c>
+      <c r="L204" t="s">
+        <v>714</v>
+      </c>
+    </row>
+    <row r="205" spans="2:12" x14ac:dyDescent="0.2">
+      <c r="B205" t="s">
+        <v>819</v>
+      </c>
+      <c r="C205" s="9" t="s">
+        <v>728</v>
+      </c>
+      <c r="D205" t="s">
+        <v>836</v>
+      </c>
+      <c r="E205" t="s">
+        <v>418</v>
+      </c>
+      <c r="F205" t="s">
+        <v>166</v>
+      </c>
+      <c r="G205" t="s">
+        <v>423</v>
+      </c>
+      <c r="H205" t="s">
+        <v>427</v>
+      </c>
+      <c r="I205" t="s">
+        <v>706</v>
+      </c>
+      <c r="J205" s="8" t="s">
+        <v>799</v>
+      </c>
+      <c r="L205" t="s">
+        <v>714</v>
+      </c>
+    </row>
+    <row r="206" spans="2:12" x14ac:dyDescent="0.2">
+      <c r="B206" t="s">
+        <v>820</v>
+      </c>
+      <c r="C206" s="9" t="s">
+        <v>728</v>
+      </c>
+      <c r="D206" t="s">
+        <v>836</v>
+      </c>
+      <c r="E206" t="s">
+        <v>418</v>
+      </c>
+      <c r="F206" t="s">
+        <v>166</v>
+      </c>
+      <c r="G206" t="s">
+        <v>423</v>
+      </c>
+      <c r="H206" t="s">
+        <v>427</v>
+      </c>
+      <c r="I206" t="s">
+        <v>706</v>
+      </c>
+      <c r="J206" s="8" t="s">
+        <v>799</v>
+      </c>
+      <c r="L206" t="s">
+        <v>714</v>
+      </c>
+    </row>
+    <row r="207" spans="2:12" x14ac:dyDescent="0.2">
+      <c r="B207" t="s">
+        <v>821</v>
+      </c>
+      <c r="C207" s="9" t="s">
+        <v>728</v>
+      </c>
+      <c r="D207" t="s">
+        <v>836</v>
+      </c>
+      <c r="E207" t="s">
+        <v>418</v>
+      </c>
+      <c r="F207" t="s">
+        <v>166</v>
+      </c>
+      <c r="G207" t="s">
+        <v>423</v>
+      </c>
+      <c r="H207" t="s">
+        <v>427</v>
+      </c>
+      <c r="I207" t="s">
+        <v>706</v>
+      </c>
+      <c r="J207" s="8" t="s">
+        <v>799</v>
+      </c>
+      <c r="L207" t="s">
+        <v>714</v>
+      </c>
+    </row>
+    <row r="208" spans="2:12" x14ac:dyDescent="0.2">
+      <c r="B208" t="s">
+        <v>822</v>
+      </c>
+      <c r="C208" s="9" t="s">
+        <v>728</v>
+      </c>
+      <c r="D208" t="s">
+        <v>836</v>
+      </c>
+      <c r="E208" t="s">
+        <v>418</v>
+      </c>
+      <c r="F208" t="s">
+        <v>166</v>
+      </c>
+      <c r="G208" t="s">
+        <v>423</v>
+      </c>
+      <c r="H208" t="s">
+        <v>427</v>
+      </c>
+      <c r="I208" t="s">
+        <v>706</v>
+      </c>
+      <c r="J208" s="8" t="s">
+        <v>799</v>
+      </c>
+      <c r="L208" t="s">
+        <v>714</v>
+      </c>
+    </row>
+    <row r="209" spans="2:12" x14ac:dyDescent="0.2">
+      <c r="B209" t="s">
+        <v>823</v>
+      </c>
+      <c r="C209" s="9" t="s">
+        <v>728</v>
+      </c>
+      <c r="D209" t="s">
+        <v>836</v>
+      </c>
+      <c r="E209" t="s">
+        <v>418</v>
+      </c>
+      <c r="F209" t="s">
+        <v>166</v>
+      </c>
+      <c r="G209" t="s">
+        <v>423</v>
+      </c>
+      <c r="H209" t="s">
+        <v>427</v>
+      </c>
+      <c r="I209" t="s">
+        <v>706</v>
+      </c>
+      <c r="J209" s="8" t="s">
+        <v>799</v>
+      </c>
+      <c r="L209" t="s">
+        <v>714</v>
+      </c>
+    </row>
+    <row r="210" spans="2:12" x14ac:dyDescent="0.2">
+      <c r="B210" t="s">
+        <v>824</v>
+      </c>
+      <c r="C210" s="9" t="s">
+        <v>728</v>
+      </c>
+      <c r="D210" t="s">
+        <v>837</v>
+      </c>
+      <c r="E210" t="s">
+        <v>418</v>
+      </c>
+      <c r="F210" s="7" t="s">
+        <v>166</v>
+      </c>
+      <c r="G210" t="s">
+        <v>423</v>
+      </c>
+      <c r="H210" t="s">
+        <v>427</v>
+      </c>
+      <c r="I210" t="s">
+        <v>706</v>
+      </c>
+      <c r="J210" s="8" t="s">
+        <v>799</v>
+      </c>
+      <c r="L210" t="s">
+        <v>714</v>
+      </c>
+    </row>
+    <row r="211" spans="2:12" x14ac:dyDescent="0.2">
+      <c r="B211" t="s">
+        <v>825</v>
+      </c>
+      <c r="C211" s="9" t="s">
+        <v>728</v>
+      </c>
+      <c r="D211" t="s">
+        <v>837</v>
+      </c>
+      <c r="E211" t="s">
+        <v>418</v>
+      </c>
+      <c r="F211" s="7" t="s">
+        <v>166</v>
+      </c>
+      <c r="G211" t="s">
+        <v>423</v>
+      </c>
+      <c r="H211" t="s">
+        <v>427</v>
+      </c>
+      <c r="I211" t="s">
+        <v>706</v>
+      </c>
+      <c r="J211" s="8" t="s">
+        <v>799</v>
+      </c>
+      <c r="L211" t="s">
+        <v>714</v>
+      </c>
+    </row>
+    <row r="212" spans="2:12" x14ac:dyDescent="0.2">
+      <c r="B212" t="s">
+        <v>826</v>
+      </c>
+      <c r="C212" s="9" t="s">
+        <v>728</v>
+      </c>
+      <c r="D212" t="s">
+        <v>837</v>
+      </c>
+      <c r="E212" t="s">
+        <v>418</v>
+      </c>
+      <c r="F212" s="7" t="s">
+        <v>166</v>
+      </c>
+      <c r="G212" t="s">
+        <v>423</v>
+      </c>
+      <c r="H212" t="s">
+        <v>427</v>
+      </c>
+      <c r="I212" t="s">
+        <v>706</v>
+      </c>
+      <c r="J212" s="8" t="s">
+        <v>799</v>
+      </c>
+      <c r="L212" t="s">
+        <v>714</v>
+      </c>
+    </row>
+    <row r="213" spans="2:12" x14ac:dyDescent="0.2">
+      <c r="B213" t="s">
+        <v>827</v>
+      </c>
+      <c r="C213" s="9" t="s">
+        <v>728</v>
+      </c>
+      <c r="D213" t="s">
+        <v>837</v>
+      </c>
+      <c r="E213" t="s">
+        <v>418</v>
+      </c>
+      <c r="F213" s="7" t="s">
+        <v>166</v>
+      </c>
+      <c r="G213" t="s">
+        <v>423</v>
+      </c>
+      <c r="H213" t="s">
+        <v>427</v>
+      </c>
+      <c r="I213" t="s">
+        <v>706</v>
+      </c>
+      <c r="J213" s="8" t="s">
+        <v>799</v>
+      </c>
+      <c r="L213" t="s">
+        <v>714</v>
+      </c>
+    </row>
+    <row r="214" spans="2:12" x14ac:dyDescent="0.2">
+      <c r="B214" t="s">
+        <v>828</v>
+      </c>
+      <c r="C214" s="9" t="s">
+        <v>728</v>
+      </c>
+      <c r="D214" t="s">
+        <v>837</v>
+      </c>
+      <c r="E214" t="s">
+        <v>418</v>
+      </c>
+      <c r="F214" s="7" t="s">
+        <v>166</v>
+      </c>
+      <c r="G214" t="s">
+        <v>423</v>
+      </c>
+      <c r="H214" t="s">
+        <v>427</v>
+      </c>
+      <c r="I214" t="s">
+        <v>706</v>
+      </c>
+      <c r="J214" s="8" t="s">
+        <v>799</v>
+      </c>
+      <c r="L214" t="s">
+        <v>714</v>
+      </c>
+    </row>
+    <row r="215" spans="2:12" x14ac:dyDescent="0.2">
+      <c r="B215" t="s">
+        <v>829</v>
+      </c>
+      <c r="C215" s="9" t="s">
+        <v>728</v>
+      </c>
+      <c r="D215" t="s">
+        <v>838</v>
+      </c>
+      <c r="E215" t="s">
+        <v>418</v>
+      </c>
+      <c r="F215" t="s">
+        <v>165</v>
+      </c>
+      <c r="G215" t="s">
+        <v>423</v>
+      </c>
+      <c r="H215" t="s">
+        <v>427</v>
+      </c>
+      <c r="I215" t="s">
+        <v>706</v>
+      </c>
+      <c r="J215" s="8" t="s">
+        <v>799</v>
+      </c>
+      <c r="L215" t="s">
+        <v>714</v>
+      </c>
+    </row>
+    <row r="216" spans="2:12" x14ac:dyDescent="0.2">
+      <c r="B216" t="s">
+        <v>830</v>
+      </c>
+      <c r="C216" s="9" t="s">
+        <v>728</v>
+      </c>
+      <c r="D216" t="s">
+        <v>838</v>
+      </c>
+      <c r="E216" t="s">
+        <v>418</v>
+      </c>
+      <c r="F216" t="s">
+        <v>165</v>
+      </c>
+      <c r="G216" t="s">
+        <v>423</v>
+      </c>
+      <c r="H216" t="s">
+        <v>427</v>
+      </c>
+      <c r="I216" t="s">
+        <v>706</v>
+      </c>
+      <c r="J216" s="8" t="s">
+        <v>799</v>
+      </c>
+      <c r="L216" t="s">
+        <v>714</v>
+      </c>
+    </row>
+    <row r="217" spans="2:12" x14ac:dyDescent="0.2">
+      <c r="B217" t="s">
+        <v>831</v>
+      </c>
+      <c r="C217" s="9" t="s">
+        <v>728</v>
+      </c>
+      <c r="D217" t="s">
+        <v>838</v>
+      </c>
+      <c r="E217" t="s">
+        <v>418</v>
+      </c>
+      <c r="F217" t="s">
+        <v>165</v>
+      </c>
+      <c r="G217" t="s">
+        <v>423</v>
+      </c>
+      <c r="H217" t="s">
+        <v>427</v>
+      </c>
+      <c r="I217" t="s">
+        <v>706</v>
+      </c>
+      <c r="J217" s="8" t="s">
+        <v>799</v>
+      </c>
+      <c r="L217" t="s">
+        <v>714</v>
+      </c>
+    </row>
+    <row r="218" spans="2:12" x14ac:dyDescent="0.2">
+      <c r="B218" t="s">
+        <v>832</v>
+      </c>
+      <c r="C218" s="9" t="s">
+        <v>728</v>
+      </c>
+      <c r="D218" t="s">
+        <v>838</v>
+      </c>
+      <c r="E218" t="s">
+        <v>418</v>
+      </c>
+      <c r="F218" t="s">
+        <v>165</v>
+      </c>
+      <c r="G218" t="s">
+        <v>423</v>
+      </c>
+      <c r="H218" t="s">
+        <v>427</v>
+      </c>
+      <c r="I218" t="s">
+        <v>706</v>
+      </c>
+      <c r="J218" s="8" t="s">
+        <v>799</v>
+      </c>
+      <c r="L218" t="s">
+        <v>714</v>
+      </c>
+    </row>
+    <row r="219" spans="2:12" x14ac:dyDescent="0.2">
+      <c r="B219" t="s">
+        <v>833</v>
+      </c>
+      <c r="C219" s="9" t="s">
+        <v>728</v>
+      </c>
+      <c r="D219" t="s">
+        <v>838</v>
+      </c>
+      <c r="E219" t="s">
+        <v>418</v>
+      </c>
+      <c r="F219" t="s">
+        <v>165</v>
+      </c>
+      <c r="G219" t="s">
+        <v>423</v>
+      </c>
+      <c r="H219" t="s">
+        <v>427</v>
+      </c>
+      <c r="I219" t="s">
+        <v>706</v>
+      </c>
+      <c r="J219" s="8" t="s">
+        <v>799</v>
+      </c>
+      <c r="L219" t="s">
+        <v>714</v>
+      </c>
+    </row>
+    <row r="221" spans="2:12" x14ac:dyDescent="0.2">
+      <c r="B221" t="s">
+        <v>839</v>
+      </c>
+      <c r="C221" s="9" t="s">
+        <v>842</v>
+      </c>
+      <c r="D221" t="s">
+        <v>843</v>
+      </c>
+      <c r="E221" t="s">
+        <v>418</v>
+      </c>
+      <c r="F221" s="7" t="s">
+        <v>166</v>
+      </c>
+      <c r="G221" t="s">
+        <v>423</v>
+      </c>
+      <c r="H221" t="s">
+        <v>427</v>
+      </c>
+      <c r="I221" t="s">
+        <v>706</v>
+      </c>
+      <c r="J221" s="8" t="s">
+        <v>799</v>
+      </c>
+      <c r="L221" t="s">
+        <v>715</v>
+      </c>
+    </row>
+    <row r="222" spans="2:12" x14ac:dyDescent="0.2">
+      <c r="B222" t="s">
+        <v>840</v>
+      </c>
+      <c r="C222" s="9" t="s">
+        <v>842</v>
+      </c>
+      <c r="D222" t="s">
+        <v>843</v>
+      </c>
+      <c r="E222" t="s">
+        <v>418</v>
+      </c>
+      <c r="F222" s="7" t="s">
+        <v>166</v>
+      </c>
+      <c r="G222" t="s">
+        <v>423</v>
+      </c>
+      <c r="H222" t="s">
+        <v>427</v>
+      </c>
+      <c r="I222" t="s">
+        <v>706</v>
+      </c>
+      <c r="J222" s="8" t="s">
+        <v>799</v>
+      </c>
+      <c r="L222" t="s">
+        <v>841</v>
+      </c>
+    </row>
+    <row r="223" spans="2:12" x14ac:dyDescent="0.2">
+      <c r="C223" s="9"/>
+    </row>
+    <row r="224" spans="2:12" x14ac:dyDescent="0.2">
+      <c r="B224" t="s">
+        <v>844</v>
+      </c>
+      <c r="C224" s="9" t="s">
         <v>729</v>
       </c>
-      <c r="G146" t="s">
-        <v>423</v>
-      </c>
-      <c r="L146" t="s">
-        <v>715</v>
-      </c>
-    </row>
-    <row r="147" spans="3:12" x14ac:dyDescent="0.2">
-      <c r="C147" s="9"/>
-    </row>
-    <row r="148" spans="3:12" x14ac:dyDescent="0.2">
-      <c r="C148" s="9" t="s">
+      <c r="D224" t="s">
+        <v>847</v>
+      </c>
+      <c r="E224" t="s">
+        <v>418</v>
+      </c>
+      <c r="F224" s="7" t="s">
+        <v>166</v>
+      </c>
+      <c r="G224" t="s">
+        <v>423</v>
+      </c>
+      <c r="H224" t="s">
+        <v>427</v>
+      </c>
+      <c r="I224" t="s">
+        <v>705</v>
+      </c>
+      <c r="J224" s="8" t="s">
+        <v>799</v>
+      </c>
+      <c r="L224" t="s">
+        <v>716</v>
+      </c>
+    </row>
+    <row r="225" spans="2:12" x14ac:dyDescent="0.2">
+      <c r="B225" t="s">
+        <v>845</v>
+      </c>
+      <c r="C225" s="9" t="s">
+        <v>729</v>
+      </c>
+      <c r="D225" t="s">
+        <v>847</v>
+      </c>
+      <c r="E225" t="s">
+        <v>418</v>
+      </c>
+      <c r="F225" s="7" t="s">
+        <v>166</v>
+      </c>
+      <c r="G225" t="s">
+        <v>423</v>
+      </c>
+      <c r="H225" t="s">
+        <v>427</v>
+      </c>
+      <c r="I225" t="s">
+        <v>705</v>
+      </c>
+      <c r="J225" s="8" t="s">
+        <v>799</v>
+      </c>
+      <c r="L225" t="s">
+        <v>716</v>
+      </c>
+    </row>
+    <row r="226" spans="2:12" x14ac:dyDescent="0.2">
+      <c r="B226" t="s">
+        <v>846</v>
+      </c>
+      <c r="C226" s="9" t="s">
+        <v>729</v>
+      </c>
+      <c r="D226" t="s">
+        <v>847</v>
+      </c>
+      <c r="E226" t="s">
+        <v>418</v>
+      </c>
+      <c r="F226" s="7" t="s">
+        <v>166</v>
+      </c>
+      <c r="G226" t="s">
+        <v>423</v>
+      </c>
+      <c r="H226" t="s">
+        <v>427</v>
+      </c>
+      <c r="I226" t="s">
+        <v>705</v>
+      </c>
+      <c r="J226" s="8" t="s">
+        <v>799</v>
+      </c>
+      <c r="L226" t="s">
+        <v>716</v>
+      </c>
+    </row>
+    <row r="227" spans="2:12" x14ac:dyDescent="0.2">
+      <c r="C227" s="9"/>
+    </row>
+    <row r="228" spans="2:12" x14ac:dyDescent="0.2">
+      <c r="B228" t="s">
+        <v>848</v>
+      </c>
+      <c r="C228" s="9" t="s">
+        <v>852</v>
+      </c>
+      <c r="D228" t="s">
+        <v>853</v>
+      </c>
+      <c r="E228" t="s">
+        <v>418</v>
+      </c>
+      <c r="F228" s="8" t="s">
+        <v>165</v>
+      </c>
+      <c r="G228" t="s">
+        <v>423</v>
+      </c>
+      <c r="H228" s="7" t="s">
+        <v>428</v>
+      </c>
+      <c r="I228" t="s">
+        <v>705</v>
+      </c>
+      <c r="J228" s="8" t="s">
+        <v>799</v>
+      </c>
+      <c r="L228" t="s">
+        <v>717</v>
+      </c>
+    </row>
+    <row r="229" spans="2:12" x14ac:dyDescent="0.2">
+      <c r="B229" t="s">
+        <v>849</v>
+      </c>
+      <c r="C229" s="9" t="s">
+        <v>852</v>
+      </c>
+      <c r="D229" t="s">
+        <v>854</v>
+      </c>
+      <c r="E229" t="s">
+        <v>418</v>
+      </c>
+      <c r="F229" s="8" t="s">
+        <v>165</v>
+      </c>
+      <c r="G229" t="s">
+        <v>423</v>
+      </c>
+      <c r="H229" s="7" t="s">
+        <v>428</v>
+      </c>
+      <c r="I229" t="s">
+        <v>705</v>
+      </c>
+      <c r="J229" s="8" t="s">
+        <v>799</v>
+      </c>
+      <c r="L229" t="s">
+        <v>717</v>
+      </c>
+    </row>
+    <row r="230" spans="2:12" x14ac:dyDescent="0.2">
+      <c r="B230" t="s">
+        <v>850</v>
+      </c>
+      <c r="C230" s="9" t="s">
+        <v>852</v>
+      </c>
+      <c r="D230" t="s">
+        <v>855</v>
+      </c>
+      <c r="E230" t="s">
+        <v>418</v>
+      </c>
+      <c r="F230" s="8" t="s">
+        <v>165</v>
+      </c>
+      <c r="G230" t="s">
+        <v>423</v>
+      </c>
+      <c r="H230" s="7" t="s">
+        <v>428</v>
+      </c>
+      <c r="I230" t="s">
+        <v>705</v>
+      </c>
+      <c r="J230" s="8" t="s">
+        <v>799</v>
+      </c>
+      <c r="L230" t="s">
+        <v>717</v>
+      </c>
+    </row>
+    <row r="231" spans="2:12" x14ac:dyDescent="0.2">
+      <c r="B231" t="s">
+        <v>851</v>
+      </c>
+      <c r="C231" s="9" t="s">
+        <v>852</v>
+      </c>
+      <c r="D231" t="s">
+        <v>856</v>
+      </c>
+      <c r="E231" t="s">
+        <v>418</v>
+      </c>
+      <c r="F231" s="8" t="s">
+        <v>165</v>
+      </c>
+      <c r="G231" t="s">
+        <v>423</v>
+      </c>
+      <c r="H231" s="7" t="s">
+        <v>428</v>
+      </c>
+      <c r="I231" t="s">
+        <v>705</v>
+      </c>
+      <c r="J231" s="8" t="s">
+        <v>799</v>
+      </c>
+      <c r="L231" t="s">
+        <v>717</v>
+      </c>
+    </row>
+    <row r="232" spans="2:12" x14ac:dyDescent="0.2">
+      <c r="C232" s="9"/>
+    </row>
+    <row r="233" spans="2:12" x14ac:dyDescent="0.2">
+      <c r="B233" t="s">
+        <v>857</v>
+      </c>
+      <c r="C233" s="9" t="s">
         <v>730</v>
       </c>
-      <c r="G148" t="s">
-        <v>423</v>
-      </c>
-      <c r="L148" t="s">
-        <v>716</v>
-      </c>
-    </row>
-    <row r="149" spans="3:12" x14ac:dyDescent="0.2">
-      <c r="C149" s="9"/>
-    </row>
-    <row r="150" spans="3:12" x14ac:dyDescent="0.2">
-      <c r="C150" s="9" t="s">
+      <c r="D233" t="s">
+        <v>864</v>
+      </c>
+      <c r="E233" t="s">
+        <v>418</v>
+      </c>
+      <c r="F233" t="s">
+        <v>166</v>
+      </c>
+      <c r="G233" t="s">
+        <v>423</v>
+      </c>
+      <c r="H233" s="8" t="s">
+        <v>427</v>
+      </c>
+      <c r="I233" s="8" t="s">
+        <v>705</v>
+      </c>
+      <c r="J233" s="8" t="s">
+        <v>799</v>
+      </c>
+      <c r="L233" t="s">
+        <v>718</v>
+      </c>
+    </row>
+    <row r="234" spans="2:12" x14ac:dyDescent="0.2">
+      <c r="B234" t="s">
+        <v>858</v>
+      </c>
+      <c r="C234" s="9" t="s">
+        <v>730</v>
+      </c>
+      <c r="D234" t="s">
+        <v>865</v>
+      </c>
+      <c r="E234" t="s">
+        <v>418</v>
+      </c>
+      <c r="F234" t="s">
+        <v>166</v>
+      </c>
+      <c r="G234" t="s">
+        <v>423</v>
+      </c>
+      <c r="H234" s="8" t="s">
+        <v>427</v>
+      </c>
+      <c r="I234" s="8" t="s">
+        <v>705</v>
+      </c>
+      <c r="J234" s="8" t="s">
+        <v>799</v>
+      </c>
+      <c r="L234" t="s">
+        <v>718</v>
+      </c>
+    </row>
+    <row r="235" spans="2:12" x14ac:dyDescent="0.2">
+      <c r="B235" t="s">
+        <v>859</v>
+      </c>
+      <c r="C235" s="9" t="s">
+        <v>730</v>
+      </c>
+      <c r="D235" t="s">
+        <v>866</v>
+      </c>
+      <c r="E235" t="s">
+        <v>418</v>
+      </c>
+      <c r="F235" t="s">
+        <v>166</v>
+      </c>
+      <c r="G235" t="s">
+        <v>423</v>
+      </c>
+      <c r="H235" s="8" t="s">
+        <v>427</v>
+      </c>
+      <c r="I235" s="8" t="s">
+        <v>705</v>
+      </c>
+      <c r="J235" s="8" t="s">
+        <v>799</v>
+      </c>
+      <c r="L235" t="s">
+        <v>718</v>
+      </c>
+    </row>
+    <row r="236" spans="2:12" x14ac:dyDescent="0.2">
+      <c r="B236" t="s">
+        <v>860</v>
+      </c>
+      <c r="C236" s="9" t="s">
+        <v>730</v>
+      </c>
+      <c r="D236" t="s">
+        <v>867</v>
+      </c>
+      <c r="E236" t="s">
+        <v>418</v>
+      </c>
+      <c r="F236" t="s">
+        <v>166</v>
+      </c>
+      <c r="G236" t="s">
+        <v>423</v>
+      </c>
+      <c r="H236" s="8" t="s">
+        <v>427</v>
+      </c>
+      <c r="I236" s="8" t="s">
+        <v>705</v>
+      </c>
+      <c r="J236" s="8" t="s">
+        <v>799</v>
+      </c>
+      <c r="L236" t="s">
+        <v>718</v>
+      </c>
+    </row>
+    <row r="237" spans="2:12" x14ac:dyDescent="0.2">
+      <c r="B237" t="s">
+        <v>861</v>
+      </c>
+      <c r="C237" s="9" t="s">
+        <v>730</v>
+      </c>
+      <c r="D237" t="s">
+        <v>868</v>
+      </c>
+      <c r="E237" t="s">
+        <v>418</v>
+      </c>
+      <c r="F237" t="s">
+        <v>166</v>
+      </c>
+      <c r="G237" t="s">
+        <v>423</v>
+      </c>
+      <c r="H237" s="8" t="s">
+        <v>427</v>
+      </c>
+      <c r="I237" s="8" t="s">
+        <v>705</v>
+      </c>
+      <c r="J237" s="8" t="s">
+        <v>799</v>
+      </c>
+      <c r="L237" t="s">
+        <v>718</v>
+      </c>
+    </row>
+    <row r="238" spans="2:12" x14ac:dyDescent="0.2">
+      <c r="B238" t="s">
+        <v>862</v>
+      </c>
+      <c r="C238" s="9" t="s">
+        <v>730</v>
+      </c>
+      <c r="D238" t="s">
+        <v>869</v>
+      </c>
+      <c r="E238" t="s">
+        <v>418</v>
+      </c>
+      <c r="F238" t="s">
+        <v>166</v>
+      </c>
+      <c r="G238" t="s">
+        <v>423</v>
+      </c>
+      <c r="H238" s="8" t="s">
+        <v>427</v>
+      </c>
+      <c r="I238" s="8" t="s">
+        <v>705</v>
+      </c>
+      <c r="J238" s="8" t="s">
+        <v>799</v>
+      </c>
+      <c r="L238" t="s">
+        <v>718</v>
+      </c>
+    </row>
+    <row r="239" spans="2:12" x14ac:dyDescent="0.2">
+      <c r="B239" t="s">
+        <v>863</v>
+      </c>
+      <c r="C239" s="9" t="s">
+        <v>730</v>
+      </c>
+      <c r="D239" t="s">
+        <v>870</v>
+      </c>
+      <c r="E239" t="s">
+        <v>418</v>
+      </c>
+      <c r="F239" t="s">
+        <v>166</v>
+      </c>
+      <c r="G239" t="s">
+        <v>423</v>
+      </c>
+      <c r="H239" s="8" t="s">
+        <v>427</v>
+      </c>
+      <c r="I239" s="8" t="s">
+        <v>705</v>
+      </c>
+      <c r="J239" s="8" t="s">
+        <v>799</v>
+      </c>
+      <c r="L239" t="s">
+        <v>718</v>
+      </c>
+    </row>
+    <row r="240" spans="2:12" x14ac:dyDescent="0.2">
+      <c r="C240" s="9"/>
+    </row>
+    <row r="241" spans="2:12" x14ac:dyDescent="0.2">
+      <c r="B241" t="s">
+        <v>871</v>
+      </c>
+      <c r="C241" s="9" t="s">
+        <v>842</v>
+      </c>
+      <c r="D241" t="s">
+        <v>873</v>
+      </c>
+      <c r="E241" t="s">
+        <v>418</v>
+      </c>
+      <c r="F241" t="s">
+        <v>165</v>
+      </c>
+      <c r="G241" t="s">
+        <v>423</v>
+      </c>
+      <c r="H241" t="s">
+        <v>427</v>
+      </c>
+      <c r="I241" t="s">
+        <v>705</v>
+      </c>
+      <c r="L241" t="s">
+        <v>719</v>
+      </c>
+    </row>
+    <row r="242" spans="2:12" x14ac:dyDescent="0.2">
+      <c r="B242" t="s">
+        <v>872</v>
+      </c>
+      <c r="C242" s="9" t="s">
+        <v>842</v>
+      </c>
+      <c r="D242" t="s">
+        <v>874</v>
+      </c>
+      <c r="E242" t="s">
+        <v>418</v>
+      </c>
+      <c r="F242" t="s">
+        <v>165</v>
+      </c>
+      <c r="G242" t="s">
+        <v>423</v>
+      </c>
+      <c r="H242" t="s">
+        <v>427</v>
+      </c>
+      <c r="I242" t="s">
+        <v>705</v>
+      </c>
+      <c r="L242" t="s">
+        <v>719</v>
+      </c>
+    </row>
+    <row r="243" spans="2:12" x14ac:dyDescent="0.2">
+      <c r="C243" s="9"/>
+    </row>
+    <row r="244" spans="2:12" x14ac:dyDescent="0.2">
+      <c r="B244" t="s">
+        <v>875</v>
+      </c>
+      <c r="C244" s="9" t="s">
         <v>731</v>
       </c>
-      <c r="G150" t="s">
-        <v>423</v>
-      </c>
-      <c r="L150" t="s">
-        <v>717</v>
-      </c>
-    </row>
-    <row r="151" spans="3:12" x14ac:dyDescent="0.2">
-      <c r="C151" s="9"/>
-    </row>
-    <row r="152" spans="3:12" x14ac:dyDescent="0.2">
-      <c r="C152" s="9" t="s">
+      <c r="D244" t="s">
+        <v>877</v>
+      </c>
+      <c r="E244" t="s">
+        <v>418</v>
+      </c>
+      <c r="F244" t="s">
+        <v>165</v>
+      </c>
+      <c r="G244" t="s">
+        <v>423</v>
+      </c>
+      <c r="H244" t="s">
+        <v>427</v>
+      </c>
+      <c r="I244" t="s">
+        <v>705</v>
+      </c>
+      <c r="L244" t="s">
+        <v>720</v>
+      </c>
+    </row>
+    <row r="245" spans="2:12" x14ac:dyDescent="0.2">
+      <c r="B245" t="s">
+        <v>876</v>
+      </c>
+      <c r="C245" s="9" t="s">
+        <v>731</v>
+      </c>
+      <c r="D245" t="s">
+        <v>878</v>
+      </c>
+      <c r="E245" t="s">
+        <v>418</v>
+      </c>
+      <c r="F245" t="s">
+        <v>165</v>
+      </c>
+      <c r="G245" t="s">
+        <v>423</v>
+      </c>
+      <c r="H245" t="s">
+        <v>427</v>
+      </c>
+      <c r="I245" t="s">
+        <v>705</v>
+      </c>
+      <c r="L245" t="s">
+        <v>720</v>
+      </c>
+    </row>
+    <row r="246" spans="2:12" x14ac:dyDescent="0.2">
+      <c r="C246" s="9"/>
+    </row>
+    <row r="247" spans="2:12" x14ac:dyDescent="0.2">
+      <c r="B247" t="s">
+        <v>880</v>
+      </c>
+      <c r="C247" s="2" t="s">
         <v>732</v>
       </c>
-      <c r="G152" t="s">
-        <v>423</v>
-      </c>
-      <c r="L152" t="s">
-        <v>718</v>
-      </c>
-    </row>
-    <row r="153" spans="3:12" x14ac:dyDescent="0.2">
-      <c r="C153" s="9"/>
-    </row>
-    <row r="154" spans="3:12" x14ac:dyDescent="0.2">
-      <c r="C154" s="9" t="s">
-        <v>729</v>
-      </c>
-      <c r="G154" t="s">
-        <v>423</v>
-      </c>
-      <c r="L154" t="s">
-        <v>719</v>
-      </c>
-    </row>
-    <row r="155" spans="3:12" x14ac:dyDescent="0.2">
-      <c r="C155" s="9"/>
-    </row>
-    <row r="156" spans="3:12" x14ac:dyDescent="0.2">
-      <c r="C156" s="9" t="s">
-        <v>733</v>
-      </c>
-      <c r="G156" t="s">
-        <v>423</v>
-      </c>
-      <c r="L156" t="s">
-        <v>720</v>
-      </c>
-    </row>
-    <row r="157" spans="3:12" x14ac:dyDescent="0.2">
-      <c r="C157" s="9"/>
-    </row>
-    <row r="158" spans="3:12" x14ac:dyDescent="0.2">
-      <c r="C158" s="9" t="s">
-        <v>734</v>
-      </c>
-      <c r="G158" t="s">
+      <c r="D247" t="s">
+        <v>886</v>
+      </c>
+      <c r="E247" t="s">
+        <v>101</v>
+      </c>
+      <c r="F247" t="s">
+        <v>166</v>
+      </c>
+      <c r="G247" t="s">
         <v>424</v>
       </c>
-      <c r="L158" t="s">
+      <c r="H247" t="s">
+        <v>427</v>
+      </c>
+      <c r="I247" t="s">
+        <v>705</v>
+      </c>
+      <c r="K247" t="s">
+        <v>879</v>
+      </c>
+      <c r="L247" t="s">
         <v>721</v>
       </c>
     </row>
-    <row r="159" spans="3:12" x14ac:dyDescent="0.2">
-      <c r="C159" s="9"/>
-    </row>
-    <row r="160" spans="3:12" x14ac:dyDescent="0.2">
-      <c r="C160" s="9" t="s">
-        <v>735</v>
-      </c>
-      <c r="G160" t="s">
+    <row r="248" spans="2:12" x14ac:dyDescent="0.2">
+      <c r="B248" t="s">
+        <v>881</v>
+      </c>
+      <c r="C248" s="2" t="s">
+        <v>732</v>
+      </c>
+      <c r="D248" t="s">
+        <v>887</v>
+      </c>
+      <c r="E248" t="s">
+        <v>101</v>
+      </c>
+      <c r="F248" t="s">
+        <v>165</v>
+      </c>
+      <c r="G248" t="s">
         <v>424</v>
       </c>
-      <c r="L160" t="s">
+      <c r="H248" t="s">
+        <v>427</v>
+      </c>
+      <c r="I248" t="s">
+        <v>705</v>
+      </c>
+      <c r="K248" t="s">
+        <v>879</v>
+      </c>
+      <c r="L248" t="s">
+        <v>721</v>
+      </c>
+    </row>
+    <row r="249" spans="2:12" x14ac:dyDescent="0.2">
+      <c r="B249" t="s">
+        <v>882</v>
+      </c>
+      <c r="C249" s="2" t="s">
+        <v>732</v>
+      </c>
+      <c r="D249" t="s">
+        <v>886</v>
+      </c>
+      <c r="E249" t="s">
+        <v>101</v>
+      </c>
+      <c r="F249" t="s">
+        <v>166</v>
+      </c>
+      <c r="G249" t="s">
+        <v>424</v>
+      </c>
+      <c r="H249" t="s">
+        <v>427</v>
+      </c>
+      <c r="I249" t="s">
+        <v>705</v>
+      </c>
+      <c r="L249" t="s">
+        <v>721</v>
+      </c>
+    </row>
+    <row r="250" spans="2:12" x14ac:dyDescent="0.2">
+      <c r="B250" t="s">
+        <v>883</v>
+      </c>
+      <c r="C250" s="2" t="s">
+        <v>732</v>
+      </c>
+      <c r="D250" t="s">
+        <v>886</v>
+      </c>
+      <c r="E250" t="s">
+        <v>101</v>
+      </c>
+      <c r="F250" t="s">
+        <v>166</v>
+      </c>
+      <c r="G250" t="s">
+        <v>424</v>
+      </c>
+      <c r="H250" t="s">
+        <v>427</v>
+      </c>
+      <c r="I250" t="s">
+        <v>705</v>
+      </c>
+      <c r="L250" t="s">
+        <v>721</v>
+      </c>
+    </row>
+    <row r="251" spans="2:12" x14ac:dyDescent="0.2">
+      <c r="B251" t="s">
+        <v>884</v>
+      </c>
+      <c r="C251" s="2" t="s">
+        <v>732</v>
+      </c>
+      <c r="D251" t="s">
+        <v>887</v>
+      </c>
+      <c r="E251" t="s">
+        <v>101</v>
+      </c>
+      <c r="F251" t="s">
+        <v>165</v>
+      </c>
+      <c r="G251" t="s">
+        <v>424</v>
+      </c>
+      <c r="H251" t="s">
+        <v>427</v>
+      </c>
+      <c r="I251" t="s">
+        <v>705</v>
+      </c>
+      <c r="L251" t="s">
+        <v>721</v>
+      </c>
+    </row>
+    <row r="252" spans="2:12" x14ac:dyDescent="0.2">
+      <c r="B252" t="s">
+        <v>885</v>
+      </c>
+      <c r="C252" s="2" t="s">
+        <v>732</v>
+      </c>
+      <c r="D252" t="s">
+        <v>887</v>
+      </c>
+      <c r="E252" t="s">
+        <v>101</v>
+      </c>
+      <c r="F252" t="s">
+        <v>165</v>
+      </c>
+      <c r="G252" t="s">
+        <v>424</v>
+      </c>
+      <c r="H252" t="s">
+        <v>427</v>
+      </c>
+      <c r="I252" t="s">
+        <v>705</v>
+      </c>
+      <c r="L252" t="s">
+        <v>721</v>
+      </c>
+    </row>
+    <row r="253" spans="2:12" x14ac:dyDescent="0.2">
+      <c r="C253" s="9"/>
+    </row>
+    <row r="254" spans="2:12" x14ac:dyDescent="0.2">
+      <c r="B254" t="s">
+        <v>888</v>
+      </c>
+      <c r="C254" s="9" t="s">
+        <v>889</v>
+      </c>
+      <c r="D254" t="s">
+        <v>890</v>
+      </c>
+      <c r="E254" s="7" t="s">
+        <v>891</v>
+      </c>
+      <c r="F254" t="s">
+        <v>166</v>
+      </c>
+      <c r="G254" t="s">
+        <v>424</v>
+      </c>
+      <c r="H254" t="s">
+        <v>427</v>
+      </c>
+      <c r="I254" t="s">
+        <v>705</v>
+      </c>
+      <c r="L254" t="s">
         <v>722</v>
       </c>
     </row>
-    <row r="161" spans="3:12" x14ac:dyDescent="0.2">
-      <c r="C161" s="9"/>
-    </row>
-    <row r="162" spans="3:12" x14ac:dyDescent="0.2">
-      <c r="C162" s="2" t="s">
-        <v>736</v>
-      </c>
-      <c r="G162" t="s">
+    <row r="255" spans="2:12" x14ac:dyDescent="0.2">
+      <c r="C255" s="9"/>
+    </row>
+    <row r="256" spans="2:12" x14ac:dyDescent="0.2">
+      <c r="B256" t="s">
+        <v>892</v>
+      </c>
+      <c r="C256" s="2" t="s">
+        <v>894</v>
+      </c>
+      <c r="D256" t="s">
+        <v>893</v>
+      </c>
+      <c r="E256" s="7"/>
+      <c r="F256" t="s">
+        <v>166</v>
+      </c>
+      <c r="G256" t="s">
         <v>424</v>
       </c>
-      <c r="L162" t="s">
+      <c r="H256" s="7"/>
+      <c r="I256" t="s">
+        <v>705</v>
+      </c>
+      <c r="L256" t="s">
         <v>723</v>
       </c>
     </row>
-    <row r="163" spans="3:12" x14ac:dyDescent="0.2">
-      <c r="C163" s="9"/>
-    </row>
-    <row r="164" spans="3:12" x14ac:dyDescent="0.2">
-      <c r="C164" s="9"/>
-    </row>
-    <row r="165" spans="3:12" x14ac:dyDescent="0.2">
-      <c r="C165" s="9"/>
-    </row>
-    <row r="166" spans="3:12" x14ac:dyDescent="0.2">
-      <c r="C166" s="9"/>
-    </row>
-    <row r="167" spans="3:12" x14ac:dyDescent="0.2">
-      <c r="C167" s="9"/>
+    <row r="258" spans="2:12" x14ac:dyDescent="0.2">
+      <c r="B258" t="s">
+        <v>897</v>
+      </c>
+      <c r="C258" s="2" t="s">
+        <v>913</v>
+      </c>
+      <c r="D258" t="s">
+        <v>836</v>
+      </c>
+      <c r="E258" t="s">
+        <v>418</v>
+      </c>
+      <c r="F258" t="s">
+        <v>166</v>
+      </c>
+      <c r="G258" t="s">
+        <v>423</v>
+      </c>
+      <c r="H258" t="s">
+        <v>427</v>
+      </c>
+      <c r="I258" t="s">
+        <v>706</v>
+      </c>
+      <c r="J258" t="s">
+        <v>799</v>
+      </c>
+      <c r="L258" t="s">
+        <v>895</v>
+      </c>
+    </row>
+    <row r="259" spans="2:12" x14ac:dyDescent="0.2">
+      <c r="B259" t="s">
+        <v>898</v>
+      </c>
+      <c r="C259" s="2" t="s">
+        <v>913</v>
+      </c>
+      <c r="D259" t="s">
+        <v>836</v>
+      </c>
+      <c r="E259" t="s">
+        <v>418</v>
+      </c>
+      <c r="F259" t="s">
+        <v>166</v>
+      </c>
+      <c r="G259" t="s">
+        <v>423</v>
+      </c>
+      <c r="H259" t="s">
+        <v>427</v>
+      </c>
+      <c r="I259" t="s">
+        <v>706</v>
+      </c>
+      <c r="J259" t="s">
+        <v>799</v>
+      </c>
+    </row>
+    <row r="260" spans="2:12" x14ac:dyDescent="0.2">
+      <c r="B260" t="s">
+        <v>899</v>
+      </c>
+      <c r="C260" s="2" t="s">
+        <v>913</v>
+      </c>
+      <c r="D260" t="s">
+        <v>836</v>
+      </c>
+      <c r="E260" t="s">
+        <v>418</v>
+      </c>
+      <c r="F260" t="s">
+        <v>166</v>
+      </c>
+      <c r="G260" t="s">
+        <v>423</v>
+      </c>
+      <c r="H260" t="s">
+        <v>427</v>
+      </c>
+      <c r="I260" t="s">
+        <v>706</v>
+      </c>
+      <c r="J260" t="s">
+        <v>799</v>
+      </c>
+    </row>
+    <row r="261" spans="2:12" x14ac:dyDescent="0.2">
+      <c r="B261" t="s">
+        <v>900</v>
+      </c>
+      <c r="C261" s="2" t="s">
+        <v>913</v>
+      </c>
+      <c r="D261" t="s">
+        <v>836</v>
+      </c>
+      <c r="E261" t="s">
+        <v>418</v>
+      </c>
+      <c r="F261" t="s">
+        <v>166</v>
+      </c>
+      <c r="G261" t="s">
+        <v>423</v>
+      </c>
+      <c r="H261" t="s">
+        <v>427</v>
+      </c>
+      <c r="I261" t="s">
+        <v>706</v>
+      </c>
+      <c r="J261" t="s">
+        <v>799</v>
+      </c>
+    </row>
+    <row r="262" spans="2:12" x14ac:dyDescent="0.2">
+      <c r="B262" t="s">
+        <v>901</v>
+      </c>
+      <c r="C262" s="2" t="s">
+        <v>913</v>
+      </c>
+      <c r="D262" t="s">
+        <v>914</v>
+      </c>
+      <c r="E262" t="s">
+        <v>418</v>
+      </c>
+      <c r="F262" t="s">
+        <v>166</v>
+      </c>
+      <c r="G262" t="s">
+        <v>423</v>
+      </c>
+      <c r="H262" t="s">
+        <v>427</v>
+      </c>
+      <c r="I262" t="s">
+        <v>706</v>
+      </c>
+      <c r="J262" t="s">
+        <v>799</v>
+      </c>
+    </row>
+    <row r="263" spans="2:12" x14ac:dyDescent="0.2">
+      <c r="B263" t="s">
+        <v>902</v>
+      </c>
+      <c r="C263" s="2" t="s">
+        <v>913</v>
+      </c>
+      <c r="D263" t="s">
+        <v>914</v>
+      </c>
+      <c r="E263" t="s">
+        <v>418</v>
+      </c>
+      <c r="F263" t="s">
+        <v>166</v>
+      </c>
+      <c r="G263" t="s">
+        <v>423</v>
+      </c>
+      <c r="H263" t="s">
+        <v>427</v>
+      </c>
+      <c r="I263" t="s">
+        <v>706</v>
+      </c>
+      <c r="J263" t="s">
+        <v>799</v>
+      </c>
+    </row>
+    <row r="264" spans="2:12" x14ac:dyDescent="0.2">
+      <c r="B264" t="s">
+        <v>903</v>
+      </c>
+      <c r="C264" s="2" t="s">
+        <v>913</v>
+      </c>
+      <c r="D264" t="s">
+        <v>914</v>
+      </c>
+      <c r="E264" t="s">
+        <v>418</v>
+      </c>
+      <c r="F264" t="s">
+        <v>166</v>
+      </c>
+      <c r="G264" t="s">
+        <v>423</v>
+      </c>
+      <c r="H264" t="s">
+        <v>427</v>
+      </c>
+      <c r="I264" t="s">
+        <v>706</v>
+      </c>
+      <c r="J264" t="s">
+        <v>799</v>
+      </c>
+    </row>
+    <row r="265" spans="2:12" x14ac:dyDescent="0.2">
+      <c r="B265" t="s">
+        <v>904</v>
+      </c>
+      <c r="C265" s="2" t="s">
+        <v>913</v>
+      </c>
+      <c r="D265" t="s">
+        <v>914</v>
+      </c>
+      <c r="E265" t="s">
+        <v>418</v>
+      </c>
+      <c r="F265" t="s">
+        <v>166</v>
+      </c>
+      <c r="G265" t="s">
+        <v>423</v>
+      </c>
+      <c r="H265" t="s">
+        <v>427</v>
+      </c>
+      <c r="I265" t="s">
+        <v>706</v>
+      </c>
+      <c r="J265" t="s">
+        <v>799</v>
+      </c>
+    </row>
+    <row r="266" spans="2:12" x14ac:dyDescent="0.2">
+      <c r="B266" t="s">
+        <v>906</v>
+      </c>
+      <c r="C266" s="2" t="s">
+        <v>913</v>
+      </c>
+      <c r="D266" t="s">
+        <v>915</v>
+      </c>
+      <c r="E266" t="s">
+        <v>418</v>
+      </c>
+      <c r="F266" t="s">
+        <v>166</v>
+      </c>
+      <c r="G266" t="s">
+        <v>423</v>
+      </c>
+      <c r="H266" t="s">
+        <v>427</v>
+      </c>
+      <c r="I266" t="s">
+        <v>706</v>
+      </c>
+      <c r="J266" t="s">
+        <v>799</v>
+      </c>
+    </row>
+    <row r="267" spans="2:12" x14ac:dyDescent="0.2">
+      <c r="B267" t="s">
+        <v>905</v>
+      </c>
+      <c r="C267" s="2" t="s">
+        <v>913</v>
+      </c>
+      <c r="D267" t="s">
+        <v>915</v>
+      </c>
+      <c r="E267" t="s">
+        <v>418</v>
+      </c>
+      <c r="F267" t="s">
+        <v>166</v>
+      </c>
+      <c r="G267" t="s">
+        <v>423</v>
+      </c>
+      <c r="H267" t="s">
+        <v>427</v>
+      </c>
+      <c r="I267" t="s">
+        <v>706</v>
+      </c>
+      <c r="J267" t="s">
+        <v>799</v>
+      </c>
+    </row>
+    <row r="268" spans="2:12" x14ac:dyDescent="0.2">
+      <c r="B268" t="s">
+        <v>907</v>
+      </c>
+      <c r="C268" s="2" t="s">
+        <v>913</v>
+      </c>
+      <c r="D268" t="s">
+        <v>915</v>
+      </c>
+      <c r="E268" t="s">
+        <v>418</v>
+      </c>
+      <c r="F268" t="s">
+        <v>166</v>
+      </c>
+      <c r="G268" t="s">
+        <v>423</v>
+      </c>
+      <c r="H268" t="s">
+        <v>427</v>
+      </c>
+      <c r="I268" t="s">
+        <v>706</v>
+      </c>
+      <c r="J268" t="s">
+        <v>799</v>
+      </c>
+    </row>
+    <row r="269" spans="2:12" x14ac:dyDescent="0.2">
+      <c r="B269" t="s">
+        <v>908</v>
+      </c>
+      <c r="C269" s="2" t="s">
+        <v>913</v>
+      </c>
+      <c r="D269" t="s">
+        <v>915</v>
+      </c>
+      <c r="E269" t="s">
+        <v>418</v>
+      </c>
+      <c r="F269" t="s">
+        <v>166</v>
+      </c>
+      <c r="G269" t="s">
+        <v>423</v>
+      </c>
+      <c r="H269" t="s">
+        <v>427</v>
+      </c>
+      <c r="I269" t="s">
+        <v>706</v>
+      </c>
+      <c r="J269" t="s">
+        <v>799</v>
+      </c>
+    </row>
+    <row r="270" spans="2:12" x14ac:dyDescent="0.2">
+      <c r="B270" t="s">
+        <v>909</v>
+      </c>
+      <c r="C270" s="2" t="s">
+        <v>913</v>
+      </c>
+      <c r="D270" t="s">
+        <v>916</v>
+      </c>
+      <c r="E270" t="s">
+        <v>418</v>
+      </c>
+      <c r="F270" t="s">
+        <v>166</v>
+      </c>
+      <c r="G270" t="s">
+        <v>423</v>
+      </c>
+      <c r="H270" t="s">
+        <v>427</v>
+      </c>
+      <c r="I270" t="s">
+        <v>706</v>
+      </c>
+      <c r="J270" t="s">
+        <v>799</v>
+      </c>
+    </row>
+    <row r="271" spans="2:12" x14ac:dyDescent="0.2">
+      <c r="B271" t="s">
+        <v>910</v>
+      </c>
+      <c r="C271" s="2" t="s">
+        <v>913</v>
+      </c>
+      <c r="D271" t="s">
+        <v>916</v>
+      </c>
+      <c r="E271" t="s">
+        <v>418</v>
+      </c>
+      <c r="F271" t="s">
+        <v>166</v>
+      </c>
+      <c r="G271" t="s">
+        <v>423</v>
+      </c>
+      <c r="H271" t="s">
+        <v>427</v>
+      </c>
+      <c r="I271" t="s">
+        <v>706</v>
+      </c>
+      <c r="J271" t="s">
+        <v>799</v>
+      </c>
+    </row>
+    <row r="272" spans="2:12" x14ac:dyDescent="0.2">
+      <c r="B272" t="s">
+        <v>911</v>
+      </c>
+      <c r="C272" s="2" t="s">
+        <v>913</v>
+      </c>
+      <c r="D272" t="s">
+        <v>916</v>
+      </c>
+      <c r="E272" t="s">
+        <v>418</v>
+      </c>
+      <c r="F272" t="s">
+        <v>166</v>
+      </c>
+      <c r="G272" t="s">
+        <v>423</v>
+      </c>
+      <c r="H272" t="s">
+        <v>427</v>
+      </c>
+      <c r="I272" t="s">
+        <v>706</v>
+      </c>
+      <c r="J272" t="s">
+        <v>799</v>
+      </c>
+    </row>
+    <row r="273" spans="2:12" x14ac:dyDescent="0.2">
+      <c r="B273" t="s">
+        <v>912</v>
+      </c>
+      <c r="C273" s="2" t="s">
+        <v>913</v>
+      </c>
+      <c r="D273" t="s">
+        <v>916</v>
+      </c>
+      <c r="E273" t="s">
+        <v>418</v>
+      </c>
+      <c r="F273" t="s">
+        <v>166</v>
+      </c>
+      <c r="G273" t="s">
+        <v>423</v>
+      </c>
+      <c r="H273" t="s">
+        <v>427</v>
+      </c>
+      <c r="I273" t="s">
+        <v>706</v>
+      </c>
+      <c r="J273" t="s">
+        <v>799</v>
+      </c>
+    </row>
+    <row r="275" spans="2:12" x14ac:dyDescent="0.2">
+      <c r="B275" t="s">
+        <v>917</v>
+      </c>
+      <c r="C275" s="2" t="s">
+        <v>918</v>
+      </c>
+      <c r="D275" t="s">
+        <v>919</v>
+      </c>
+      <c r="E275" t="s">
+        <v>418</v>
+      </c>
+      <c r="F275" t="s">
+        <v>166</v>
+      </c>
+      <c r="G275" t="s">
+        <v>423</v>
+      </c>
+      <c r="H275" t="s">
+        <v>427</v>
+      </c>
+      <c r="I275" t="s">
+        <v>705</v>
+      </c>
+      <c r="J275" t="s">
+        <v>799</v>
+      </c>
+      <c r="L275" t="s">
+        <v>896</v>
+      </c>
     </row>
   </sheetData>
-  <phoneticPr fontId="3" type="noConversion"/>
+  <phoneticPr fontId="4" type="noConversion"/>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
 </worksheet>
 </file>
</xml_diff>